<commit_message>
update excel templates: fill in telephone number
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\urvdp\Documents\Datenbank\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\04_Hiwi\Datenbank\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE68B1A-E018-44D6-A0A0-7EC7505C1079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <definedName name="kursname">Notenliste!$A$52:$A$60</definedName>
     <definedName name="semester">Notenliste!$D$52:$D$62</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -339,7 +340,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -833,8 +834,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -944,7 +945,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1194,54 +1195,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DATA" displayName="DATA" ref="B1:L2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B1:L2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DATA" displayName="DATA" ref="B1:L2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B1:L2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Nachname" dataDxfId="21"/>
-    <tableColumn id="2" name="Vorname" dataDxfId="20"/>
-    <tableColumn id="3" name="Hochschule" dataDxfId="19"/>
-    <tableColumn id="4" name="Matrikelnummer" dataDxfId="18"/>
-    <tableColumn id="8" name="Note" dataDxfId="17"/>
-    <tableColumn id="7" name="LP" dataDxfId="16"/>
-    <tableColumn id="5" name="E-Mail" dataDxfId="15"/>
-    <tableColumn id="9" name="Telefon" dataDxfId="14"/>
-    <tableColumn id="11" name="bestanden" dataDxfId="13"/>
-    <tableColumn id="10" name="Teilnahmeschein" dataDxfId="12"/>
-    <tableColumn id="6" name="Schein erhalten" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vorname" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hochschule" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Matrikelnummer" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Note" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="LP" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E-Mail" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Telefon" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="bestanden" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Teilnahmeschein" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Schein erhalten" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="10">
-  <autoFilter ref="A1:H36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Matrikelnummer" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Matrikelnummer" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>IF(Notenliste!D2=0," ",Notenliste!D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Status" dataDxfId="7"/>
-    <tableColumn id="3" name="LP" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Status" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="LP" dataDxfId="6">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,IF(Notenliste!I2&lt;&gt;0,Notenliste!I2,Notenliste!$B$33)," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Note" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Note" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(Notenliste!D2=0," ",IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Datum" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Datum" dataDxfId="3">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$48," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Individueller Titel deutsch" dataDxfId="2"/>
-    <tableColumn id="7" name="Individueller Titel englisch" dataDxfId="1"/>
-    <tableColumn id="8" name="Anmerkungen" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Individueller Titel deutsch" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Individueller Titel englisch" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Anmerkungen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1279,9 +1280,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1316,7 +1317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1351,7 +1352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1524,32 +1525,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="39" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="40" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="39" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="40" customWidth="1"/>
     <col min="6" max="7" width="9" style="40" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.85546875" style="39" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="39" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" style="39" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="39" customWidth="1"/>
-    <col min="13" max="13" width="45.140625" style="39" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="39" hidden="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" hidden="1"/>
+    <col min="8" max="8" width="31.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" style="39" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="39" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="39" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" style="39" customWidth="1"/>
+    <col min="13" max="13" width="45.109375" style="39" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="39" hidden="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.44140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1667,7 +1668,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1689,7 +1690,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1766,7 +1767,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1777,7 +1778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1810,7 +1811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1843,7 +1844,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1854,7 +1855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1876,62 +1877,62 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1947,557 +1948,557 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:WVY71"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" style="1" hidden="1"/>
-    <col min="16" max="16" width="5.140625" style="1" hidden="1"/>
-    <col min="17" max="17" width="6.85546875" style="2" hidden="1"/>
-    <col min="18" max="18" width="17.7109375" style="1" hidden="1"/>
+    <col min="15" max="15" width="6.44140625" style="1" hidden="1"/>
+    <col min="16" max="16" width="5.109375" style="1" hidden="1"/>
+    <col min="17" max="17" width="6.88671875" style="2" hidden="1"/>
+    <col min="18" max="18" width="17.6640625" style="1" hidden="1"/>
     <col min="19" max="19" width="16" style="1" hidden="1"/>
-    <col min="20" max="20" width="17.7109375" style="1" hidden="1"/>
-    <col min="21" max="245" width="11.42578125" style="1" hidden="1"/>
-    <col min="246" max="246" width="15.42578125" style="1" hidden="1"/>
-    <col min="247" max="247" width="11.42578125" style="1" hidden="1"/>
-    <col min="248" max="248" width="15.7109375" style="1" hidden="1"/>
-    <col min="249" max="249" width="21.85546875" style="1" hidden="1"/>
-    <col min="250" max="252" width="11.42578125" style="1" hidden="1"/>
+    <col min="20" max="20" width="17.6640625" style="1" hidden="1"/>
+    <col min="21" max="245" width="11.44140625" style="1" hidden="1"/>
+    <col min="246" max="246" width="15.44140625" style="1" hidden="1"/>
+    <col min="247" max="247" width="11.44140625" style="1" hidden="1"/>
+    <col min="248" max="248" width="15.6640625" style="1" hidden="1"/>
+    <col min="249" max="249" width="21.88671875" style="1" hidden="1"/>
+    <col min="250" max="252" width="11.44140625" style="1" hidden="1"/>
     <col min="253" max="253" width="16" style="1" hidden="1"/>
-    <col min="254" max="254" width="20.42578125" style="1" hidden="1"/>
-    <col min="255" max="501" width="11.42578125" style="1" hidden="1"/>
-    <col min="502" max="502" width="15.42578125" style="1" hidden="1"/>
-    <col min="503" max="503" width="11.42578125" style="1" hidden="1"/>
-    <col min="504" max="504" width="15.7109375" style="1" hidden="1"/>
-    <col min="505" max="505" width="21.85546875" style="1" hidden="1"/>
-    <col min="506" max="508" width="11.42578125" style="1" hidden="1"/>
+    <col min="254" max="254" width="20.44140625" style="1" hidden="1"/>
+    <col min="255" max="501" width="11.44140625" style="1" hidden="1"/>
+    <col min="502" max="502" width="15.44140625" style="1" hidden="1"/>
+    <col min="503" max="503" width="11.44140625" style="1" hidden="1"/>
+    <col min="504" max="504" width="15.6640625" style="1" hidden="1"/>
+    <col min="505" max="505" width="21.88671875" style="1" hidden="1"/>
+    <col min="506" max="508" width="11.44140625" style="1" hidden="1"/>
     <col min="509" max="509" width="16" style="1" hidden="1"/>
-    <col min="510" max="510" width="20.42578125" style="1" hidden="1"/>
-    <col min="511" max="757" width="11.42578125" style="1" hidden="1"/>
-    <col min="758" max="758" width="15.42578125" style="1" hidden="1"/>
-    <col min="759" max="759" width="11.42578125" style="1" hidden="1"/>
-    <col min="760" max="760" width="15.7109375" style="1" hidden="1"/>
-    <col min="761" max="761" width="21.85546875" style="1" hidden="1"/>
-    <col min="762" max="764" width="11.42578125" style="1" hidden="1"/>
+    <col min="510" max="510" width="20.44140625" style="1" hidden="1"/>
+    <col min="511" max="757" width="11.44140625" style="1" hidden="1"/>
+    <col min="758" max="758" width="15.44140625" style="1" hidden="1"/>
+    <col min="759" max="759" width="11.44140625" style="1" hidden="1"/>
+    <col min="760" max="760" width="15.6640625" style="1" hidden="1"/>
+    <col min="761" max="761" width="21.88671875" style="1" hidden="1"/>
+    <col min="762" max="764" width="11.44140625" style="1" hidden="1"/>
     <col min="765" max="765" width="16" style="1" hidden="1"/>
-    <col min="766" max="766" width="20.42578125" style="1" hidden="1"/>
-    <col min="767" max="1013" width="11.42578125" style="1" hidden="1"/>
-    <col min="1014" max="1014" width="15.42578125" style="1" hidden="1"/>
-    <col min="1015" max="1015" width="11.42578125" style="1" hidden="1"/>
-    <col min="1016" max="1016" width="15.7109375" style="1" hidden="1"/>
-    <col min="1017" max="1017" width="21.85546875" style="1" hidden="1"/>
-    <col min="1018" max="1020" width="11.42578125" style="1" hidden="1"/>
+    <col min="766" max="766" width="20.44140625" style="1" hidden="1"/>
+    <col min="767" max="1013" width="11.44140625" style="1" hidden="1"/>
+    <col min="1014" max="1014" width="15.44140625" style="1" hidden="1"/>
+    <col min="1015" max="1015" width="11.44140625" style="1" hidden="1"/>
+    <col min="1016" max="1016" width="15.6640625" style="1" hidden="1"/>
+    <col min="1017" max="1017" width="21.88671875" style="1" hidden="1"/>
+    <col min="1018" max="1020" width="11.44140625" style="1" hidden="1"/>
     <col min="1021" max="1021" width="16" style="1" hidden="1"/>
-    <col min="1022" max="1022" width="20.42578125" style="1" hidden="1"/>
-    <col min="1023" max="1269" width="11.42578125" style="1" hidden="1"/>
-    <col min="1270" max="1270" width="15.42578125" style="1" hidden="1"/>
-    <col min="1271" max="1271" width="11.42578125" style="1" hidden="1"/>
-    <col min="1272" max="1272" width="15.7109375" style="1" hidden="1"/>
-    <col min="1273" max="1273" width="21.85546875" style="1" hidden="1"/>
-    <col min="1274" max="1276" width="11.42578125" style="1" hidden="1"/>
+    <col min="1022" max="1022" width="20.44140625" style="1" hidden="1"/>
+    <col min="1023" max="1269" width="11.44140625" style="1" hidden="1"/>
+    <col min="1270" max="1270" width="15.44140625" style="1" hidden="1"/>
+    <col min="1271" max="1271" width="11.44140625" style="1" hidden="1"/>
+    <col min="1272" max="1272" width="15.6640625" style="1" hidden="1"/>
+    <col min="1273" max="1273" width="21.88671875" style="1" hidden="1"/>
+    <col min="1274" max="1276" width="11.44140625" style="1" hidden="1"/>
     <col min="1277" max="1277" width="16" style="1" hidden="1"/>
-    <col min="1278" max="1278" width="20.42578125" style="1" hidden="1"/>
-    <col min="1279" max="1525" width="11.42578125" style="1" hidden="1"/>
-    <col min="1526" max="1526" width="15.42578125" style="1" hidden="1"/>
-    <col min="1527" max="1527" width="11.42578125" style="1" hidden="1"/>
-    <col min="1528" max="1528" width="15.7109375" style="1" hidden="1"/>
-    <col min="1529" max="1529" width="21.85546875" style="1" hidden="1"/>
-    <col min="1530" max="1532" width="11.42578125" style="1" hidden="1"/>
+    <col min="1278" max="1278" width="20.44140625" style="1" hidden="1"/>
+    <col min="1279" max="1525" width="11.44140625" style="1" hidden="1"/>
+    <col min="1526" max="1526" width="15.44140625" style="1" hidden="1"/>
+    <col min="1527" max="1527" width="11.44140625" style="1" hidden="1"/>
+    <col min="1528" max="1528" width="15.6640625" style="1" hidden="1"/>
+    <col min="1529" max="1529" width="21.88671875" style="1" hidden="1"/>
+    <col min="1530" max="1532" width="11.44140625" style="1" hidden="1"/>
     <col min="1533" max="1533" width="16" style="1" hidden="1"/>
-    <col min="1534" max="1534" width="20.42578125" style="1" hidden="1"/>
-    <col min="1535" max="1781" width="11.42578125" style="1" hidden="1"/>
-    <col min="1782" max="1782" width="15.42578125" style="1" hidden="1"/>
-    <col min="1783" max="1783" width="11.42578125" style="1" hidden="1"/>
-    <col min="1784" max="1784" width="15.7109375" style="1" hidden="1"/>
-    <col min="1785" max="1785" width="21.85546875" style="1" hidden="1"/>
-    <col min="1786" max="1788" width="11.42578125" style="1" hidden="1"/>
+    <col min="1534" max="1534" width="20.44140625" style="1" hidden="1"/>
+    <col min="1535" max="1781" width="11.44140625" style="1" hidden="1"/>
+    <col min="1782" max="1782" width="15.44140625" style="1" hidden="1"/>
+    <col min="1783" max="1783" width="11.44140625" style="1" hidden="1"/>
+    <col min="1784" max="1784" width="15.6640625" style="1" hidden="1"/>
+    <col min="1785" max="1785" width="21.88671875" style="1" hidden="1"/>
+    <col min="1786" max="1788" width="11.44140625" style="1" hidden="1"/>
     <col min="1789" max="1789" width="16" style="1" hidden="1"/>
-    <col min="1790" max="1790" width="20.42578125" style="1" hidden="1"/>
-    <col min="1791" max="2037" width="11.42578125" style="1" hidden="1"/>
-    <col min="2038" max="2038" width="15.42578125" style="1" hidden="1"/>
-    <col min="2039" max="2039" width="11.42578125" style="1" hidden="1"/>
-    <col min="2040" max="2040" width="15.7109375" style="1" hidden="1"/>
-    <col min="2041" max="2041" width="21.85546875" style="1" hidden="1"/>
-    <col min="2042" max="2044" width="11.42578125" style="1" hidden="1"/>
+    <col min="1790" max="1790" width="20.44140625" style="1" hidden="1"/>
+    <col min="1791" max="2037" width="11.44140625" style="1" hidden="1"/>
+    <col min="2038" max="2038" width="15.44140625" style="1" hidden="1"/>
+    <col min="2039" max="2039" width="11.44140625" style="1" hidden="1"/>
+    <col min="2040" max="2040" width="15.6640625" style="1" hidden="1"/>
+    <col min="2041" max="2041" width="21.88671875" style="1" hidden="1"/>
+    <col min="2042" max="2044" width="11.44140625" style="1" hidden="1"/>
     <col min="2045" max="2045" width="16" style="1" hidden="1"/>
-    <col min="2046" max="2046" width="20.42578125" style="1" hidden="1"/>
-    <col min="2047" max="2293" width="11.42578125" style="1" hidden="1"/>
-    <col min="2294" max="2294" width="15.42578125" style="1" hidden="1"/>
-    <col min="2295" max="2295" width="11.42578125" style="1" hidden="1"/>
-    <col min="2296" max="2296" width="15.7109375" style="1" hidden="1"/>
-    <col min="2297" max="2297" width="21.85546875" style="1" hidden="1"/>
-    <col min="2298" max="2300" width="11.42578125" style="1" hidden="1"/>
+    <col min="2046" max="2046" width="20.44140625" style="1" hidden="1"/>
+    <col min="2047" max="2293" width="11.44140625" style="1" hidden="1"/>
+    <col min="2294" max="2294" width="15.44140625" style="1" hidden="1"/>
+    <col min="2295" max="2295" width="11.44140625" style="1" hidden="1"/>
+    <col min="2296" max="2296" width="15.6640625" style="1" hidden="1"/>
+    <col min="2297" max="2297" width="21.88671875" style="1" hidden="1"/>
+    <col min="2298" max="2300" width="11.44140625" style="1" hidden="1"/>
     <col min="2301" max="2301" width="16" style="1" hidden="1"/>
-    <col min="2302" max="2302" width="20.42578125" style="1" hidden="1"/>
-    <col min="2303" max="2549" width="11.42578125" style="1" hidden="1"/>
-    <col min="2550" max="2550" width="15.42578125" style="1" hidden="1"/>
-    <col min="2551" max="2551" width="11.42578125" style="1" hidden="1"/>
-    <col min="2552" max="2552" width="15.7109375" style="1" hidden="1"/>
-    <col min="2553" max="2553" width="21.85546875" style="1" hidden="1"/>
-    <col min="2554" max="2556" width="11.42578125" style="1" hidden="1"/>
+    <col min="2302" max="2302" width="20.44140625" style="1" hidden="1"/>
+    <col min="2303" max="2549" width="11.44140625" style="1" hidden="1"/>
+    <col min="2550" max="2550" width="15.44140625" style="1" hidden="1"/>
+    <col min="2551" max="2551" width="11.44140625" style="1" hidden="1"/>
+    <col min="2552" max="2552" width="15.6640625" style="1" hidden="1"/>
+    <col min="2553" max="2553" width="21.88671875" style="1" hidden="1"/>
+    <col min="2554" max="2556" width="11.44140625" style="1" hidden="1"/>
     <col min="2557" max="2557" width="16" style="1" hidden="1"/>
-    <col min="2558" max="2558" width="20.42578125" style="1" hidden="1"/>
-    <col min="2559" max="2805" width="11.42578125" style="1" hidden="1"/>
-    <col min="2806" max="2806" width="15.42578125" style="1" hidden="1"/>
-    <col min="2807" max="2807" width="11.42578125" style="1" hidden="1"/>
-    <col min="2808" max="2808" width="15.7109375" style="1" hidden="1"/>
-    <col min="2809" max="2809" width="21.85546875" style="1" hidden="1"/>
-    <col min="2810" max="2812" width="11.42578125" style="1" hidden="1"/>
+    <col min="2558" max="2558" width="20.44140625" style="1" hidden="1"/>
+    <col min="2559" max="2805" width="11.44140625" style="1" hidden="1"/>
+    <col min="2806" max="2806" width="15.44140625" style="1" hidden="1"/>
+    <col min="2807" max="2807" width="11.44140625" style="1" hidden="1"/>
+    <col min="2808" max="2808" width="15.6640625" style="1" hidden="1"/>
+    <col min="2809" max="2809" width="21.88671875" style="1" hidden="1"/>
+    <col min="2810" max="2812" width="11.44140625" style="1" hidden="1"/>
     <col min="2813" max="2813" width="16" style="1" hidden="1"/>
-    <col min="2814" max="2814" width="20.42578125" style="1" hidden="1"/>
-    <col min="2815" max="3061" width="11.42578125" style="1" hidden="1"/>
-    <col min="3062" max="3062" width="15.42578125" style="1" hidden="1"/>
-    <col min="3063" max="3063" width="11.42578125" style="1" hidden="1"/>
-    <col min="3064" max="3064" width="15.7109375" style="1" hidden="1"/>
-    <col min="3065" max="3065" width="21.85546875" style="1" hidden="1"/>
-    <col min="3066" max="3068" width="11.42578125" style="1" hidden="1"/>
+    <col min="2814" max="2814" width="20.44140625" style="1" hidden="1"/>
+    <col min="2815" max="3061" width="11.44140625" style="1" hidden="1"/>
+    <col min="3062" max="3062" width="15.44140625" style="1" hidden="1"/>
+    <col min="3063" max="3063" width="11.44140625" style="1" hidden="1"/>
+    <col min="3064" max="3064" width="15.6640625" style="1" hidden="1"/>
+    <col min="3065" max="3065" width="21.88671875" style="1" hidden="1"/>
+    <col min="3066" max="3068" width="11.44140625" style="1" hidden="1"/>
     <col min="3069" max="3069" width="16" style="1" hidden="1"/>
-    <col min="3070" max="3070" width="20.42578125" style="1" hidden="1"/>
-    <col min="3071" max="3317" width="11.42578125" style="1" hidden="1"/>
-    <col min="3318" max="3318" width="15.42578125" style="1" hidden="1"/>
-    <col min="3319" max="3319" width="11.42578125" style="1" hidden="1"/>
-    <col min="3320" max="3320" width="15.7109375" style="1" hidden="1"/>
-    <col min="3321" max="3321" width="21.85546875" style="1" hidden="1"/>
-    <col min="3322" max="3324" width="11.42578125" style="1" hidden="1"/>
+    <col min="3070" max="3070" width="20.44140625" style="1" hidden="1"/>
+    <col min="3071" max="3317" width="11.44140625" style="1" hidden="1"/>
+    <col min="3318" max="3318" width="15.44140625" style="1" hidden="1"/>
+    <col min="3319" max="3319" width="11.44140625" style="1" hidden="1"/>
+    <col min="3320" max="3320" width="15.6640625" style="1" hidden="1"/>
+    <col min="3321" max="3321" width="21.88671875" style="1" hidden="1"/>
+    <col min="3322" max="3324" width="11.44140625" style="1" hidden="1"/>
     <col min="3325" max="3325" width="16" style="1" hidden="1"/>
-    <col min="3326" max="3326" width="20.42578125" style="1" hidden="1"/>
-    <col min="3327" max="3573" width="11.42578125" style="1" hidden="1"/>
-    <col min="3574" max="3574" width="15.42578125" style="1" hidden="1"/>
-    <col min="3575" max="3575" width="11.42578125" style="1" hidden="1"/>
-    <col min="3576" max="3576" width="15.7109375" style="1" hidden="1"/>
-    <col min="3577" max="3577" width="21.85546875" style="1" hidden="1"/>
-    <col min="3578" max="3580" width="11.42578125" style="1" hidden="1"/>
+    <col min="3326" max="3326" width="20.44140625" style="1" hidden="1"/>
+    <col min="3327" max="3573" width="11.44140625" style="1" hidden="1"/>
+    <col min="3574" max="3574" width="15.44140625" style="1" hidden="1"/>
+    <col min="3575" max="3575" width="11.44140625" style="1" hidden="1"/>
+    <col min="3576" max="3576" width="15.6640625" style="1" hidden="1"/>
+    <col min="3577" max="3577" width="21.88671875" style="1" hidden="1"/>
+    <col min="3578" max="3580" width="11.44140625" style="1" hidden="1"/>
     <col min="3581" max="3581" width="16" style="1" hidden="1"/>
-    <col min="3582" max="3582" width="20.42578125" style="1" hidden="1"/>
-    <col min="3583" max="3829" width="11.42578125" style="1" hidden="1"/>
-    <col min="3830" max="3830" width="15.42578125" style="1" hidden="1"/>
-    <col min="3831" max="3831" width="11.42578125" style="1" hidden="1"/>
-    <col min="3832" max="3832" width="15.7109375" style="1" hidden="1"/>
-    <col min="3833" max="3833" width="21.85546875" style="1" hidden="1"/>
-    <col min="3834" max="3836" width="11.42578125" style="1" hidden="1"/>
+    <col min="3582" max="3582" width="20.44140625" style="1" hidden="1"/>
+    <col min="3583" max="3829" width="11.44140625" style="1" hidden="1"/>
+    <col min="3830" max="3830" width="15.44140625" style="1" hidden="1"/>
+    <col min="3831" max="3831" width="11.44140625" style="1" hidden="1"/>
+    <col min="3832" max="3832" width="15.6640625" style="1" hidden="1"/>
+    <col min="3833" max="3833" width="21.88671875" style="1" hidden="1"/>
+    <col min="3834" max="3836" width="11.44140625" style="1" hidden="1"/>
     <col min="3837" max="3837" width="16" style="1" hidden="1"/>
-    <col min="3838" max="3838" width="20.42578125" style="1" hidden="1"/>
-    <col min="3839" max="4085" width="11.42578125" style="1" hidden="1"/>
-    <col min="4086" max="4086" width="15.42578125" style="1" hidden="1"/>
-    <col min="4087" max="4087" width="11.42578125" style="1" hidden="1"/>
-    <col min="4088" max="4088" width="15.7109375" style="1" hidden="1"/>
-    <col min="4089" max="4089" width="21.85546875" style="1" hidden="1"/>
-    <col min="4090" max="4092" width="11.42578125" style="1" hidden="1"/>
+    <col min="3838" max="3838" width="20.44140625" style="1" hidden="1"/>
+    <col min="3839" max="4085" width="11.44140625" style="1" hidden="1"/>
+    <col min="4086" max="4086" width="15.44140625" style="1" hidden="1"/>
+    <col min="4087" max="4087" width="11.44140625" style="1" hidden="1"/>
+    <col min="4088" max="4088" width="15.6640625" style="1" hidden="1"/>
+    <col min="4089" max="4089" width="21.88671875" style="1" hidden="1"/>
+    <col min="4090" max="4092" width="11.44140625" style="1" hidden="1"/>
     <col min="4093" max="4093" width="16" style="1" hidden="1"/>
-    <col min="4094" max="4094" width="20.42578125" style="1" hidden="1"/>
-    <col min="4095" max="4341" width="11.42578125" style="1" hidden="1"/>
-    <col min="4342" max="4342" width="15.42578125" style="1" hidden="1"/>
-    <col min="4343" max="4343" width="11.42578125" style="1" hidden="1"/>
-    <col min="4344" max="4344" width="15.7109375" style="1" hidden="1"/>
-    <col min="4345" max="4345" width="21.85546875" style="1" hidden="1"/>
-    <col min="4346" max="4348" width="11.42578125" style="1" hidden="1"/>
+    <col min="4094" max="4094" width="20.44140625" style="1" hidden="1"/>
+    <col min="4095" max="4341" width="11.44140625" style="1" hidden="1"/>
+    <col min="4342" max="4342" width="15.44140625" style="1" hidden="1"/>
+    <col min="4343" max="4343" width="11.44140625" style="1" hidden="1"/>
+    <col min="4344" max="4344" width="15.6640625" style="1" hidden="1"/>
+    <col min="4345" max="4345" width="21.88671875" style="1" hidden="1"/>
+    <col min="4346" max="4348" width="11.44140625" style="1" hidden="1"/>
     <col min="4349" max="4349" width="16" style="1" hidden="1"/>
-    <col min="4350" max="4350" width="20.42578125" style="1" hidden="1"/>
-    <col min="4351" max="4597" width="11.42578125" style="1" hidden="1"/>
-    <col min="4598" max="4598" width="15.42578125" style="1" hidden="1"/>
-    <col min="4599" max="4599" width="11.42578125" style="1" hidden="1"/>
-    <col min="4600" max="4600" width="15.7109375" style="1" hidden="1"/>
-    <col min="4601" max="4601" width="21.85546875" style="1" hidden="1"/>
-    <col min="4602" max="4604" width="11.42578125" style="1" hidden="1"/>
+    <col min="4350" max="4350" width="20.44140625" style="1" hidden="1"/>
+    <col min="4351" max="4597" width="11.44140625" style="1" hidden="1"/>
+    <col min="4598" max="4598" width="15.44140625" style="1" hidden="1"/>
+    <col min="4599" max="4599" width="11.44140625" style="1" hidden="1"/>
+    <col min="4600" max="4600" width="15.6640625" style="1" hidden="1"/>
+    <col min="4601" max="4601" width="21.88671875" style="1" hidden="1"/>
+    <col min="4602" max="4604" width="11.44140625" style="1" hidden="1"/>
     <col min="4605" max="4605" width="16" style="1" hidden="1"/>
-    <col min="4606" max="4606" width="20.42578125" style="1" hidden="1"/>
-    <col min="4607" max="4853" width="11.42578125" style="1" hidden="1"/>
-    <col min="4854" max="4854" width="15.42578125" style="1" hidden="1"/>
-    <col min="4855" max="4855" width="11.42578125" style="1" hidden="1"/>
-    <col min="4856" max="4856" width="15.7109375" style="1" hidden="1"/>
-    <col min="4857" max="4857" width="21.85546875" style="1" hidden="1"/>
-    <col min="4858" max="4860" width="11.42578125" style="1" hidden="1"/>
+    <col min="4606" max="4606" width="20.44140625" style="1" hidden="1"/>
+    <col min="4607" max="4853" width="11.44140625" style="1" hidden="1"/>
+    <col min="4854" max="4854" width="15.44140625" style="1" hidden="1"/>
+    <col min="4855" max="4855" width="11.44140625" style="1" hidden="1"/>
+    <col min="4856" max="4856" width="15.6640625" style="1" hidden="1"/>
+    <col min="4857" max="4857" width="21.88671875" style="1" hidden="1"/>
+    <col min="4858" max="4860" width="11.44140625" style="1" hidden="1"/>
     <col min="4861" max="4861" width="16" style="1" hidden="1"/>
-    <col min="4862" max="4862" width="20.42578125" style="1" hidden="1"/>
-    <col min="4863" max="5109" width="11.42578125" style="1" hidden="1"/>
-    <col min="5110" max="5110" width="15.42578125" style="1" hidden="1"/>
-    <col min="5111" max="5111" width="11.42578125" style="1" hidden="1"/>
-    <col min="5112" max="5112" width="15.7109375" style="1" hidden="1"/>
-    <col min="5113" max="5113" width="21.85546875" style="1" hidden="1"/>
-    <col min="5114" max="5116" width="11.42578125" style="1" hidden="1"/>
+    <col min="4862" max="4862" width="20.44140625" style="1" hidden="1"/>
+    <col min="4863" max="5109" width="11.44140625" style="1" hidden="1"/>
+    <col min="5110" max="5110" width="15.44140625" style="1" hidden="1"/>
+    <col min="5111" max="5111" width="11.44140625" style="1" hidden="1"/>
+    <col min="5112" max="5112" width="15.6640625" style="1" hidden="1"/>
+    <col min="5113" max="5113" width="21.88671875" style="1" hidden="1"/>
+    <col min="5114" max="5116" width="11.44140625" style="1" hidden="1"/>
     <col min="5117" max="5117" width="16" style="1" hidden="1"/>
-    <col min="5118" max="5118" width="20.42578125" style="1" hidden="1"/>
-    <col min="5119" max="5365" width="11.42578125" style="1" hidden="1"/>
-    <col min="5366" max="5366" width="15.42578125" style="1" hidden="1"/>
-    <col min="5367" max="5367" width="11.42578125" style="1" hidden="1"/>
-    <col min="5368" max="5368" width="15.7109375" style="1" hidden="1"/>
-    <col min="5369" max="5369" width="21.85546875" style="1" hidden="1"/>
-    <col min="5370" max="5372" width="11.42578125" style="1" hidden="1"/>
+    <col min="5118" max="5118" width="20.44140625" style="1" hidden="1"/>
+    <col min="5119" max="5365" width="11.44140625" style="1" hidden="1"/>
+    <col min="5366" max="5366" width="15.44140625" style="1" hidden="1"/>
+    <col min="5367" max="5367" width="11.44140625" style="1" hidden="1"/>
+    <col min="5368" max="5368" width="15.6640625" style="1" hidden="1"/>
+    <col min="5369" max="5369" width="21.88671875" style="1" hidden="1"/>
+    <col min="5370" max="5372" width="11.44140625" style="1" hidden="1"/>
     <col min="5373" max="5373" width="16" style="1" hidden="1"/>
-    <col min="5374" max="5374" width="20.42578125" style="1" hidden="1"/>
-    <col min="5375" max="5621" width="11.42578125" style="1" hidden="1"/>
-    <col min="5622" max="5622" width="15.42578125" style="1" hidden="1"/>
-    <col min="5623" max="5623" width="11.42578125" style="1" hidden="1"/>
-    <col min="5624" max="5624" width="15.7109375" style="1" hidden="1"/>
-    <col min="5625" max="5625" width="21.85546875" style="1" hidden="1"/>
-    <col min="5626" max="5628" width="11.42578125" style="1" hidden="1"/>
+    <col min="5374" max="5374" width="20.44140625" style="1" hidden="1"/>
+    <col min="5375" max="5621" width="11.44140625" style="1" hidden="1"/>
+    <col min="5622" max="5622" width="15.44140625" style="1" hidden="1"/>
+    <col min="5623" max="5623" width="11.44140625" style="1" hidden="1"/>
+    <col min="5624" max="5624" width="15.6640625" style="1" hidden="1"/>
+    <col min="5625" max="5625" width="21.88671875" style="1" hidden="1"/>
+    <col min="5626" max="5628" width="11.44140625" style="1" hidden="1"/>
     <col min="5629" max="5629" width="16" style="1" hidden="1"/>
-    <col min="5630" max="5630" width="20.42578125" style="1" hidden="1"/>
-    <col min="5631" max="5877" width="11.42578125" style="1" hidden="1"/>
-    <col min="5878" max="5878" width="15.42578125" style="1" hidden="1"/>
-    <col min="5879" max="5879" width="11.42578125" style="1" hidden="1"/>
-    <col min="5880" max="5880" width="15.7109375" style="1" hidden="1"/>
-    <col min="5881" max="5881" width="21.85546875" style="1" hidden="1"/>
-    <col min="5882" max="5884" width="11.42578125" style="1" hidden="1"/>
+    <col min="5630" max="5630" width="20.44140625" style="1" hidden="1"/>
+    <col min="5631" max="5877" width="11.44140625" style="1" hidden="1"/>
+    <col min="5878" max="5878" width="15.44140625" style="1" hidden="1"/>
+    <col min="5879" max="5879" width="11.44140625" style="1" hidden="1"/>
+    <col min="5880" max="5880" width="15.6640625" style="1" hidden="1"/>
+    <col min="5881" max="5881" width="21.88671875" style="1" hidden="1"/>
+    <col min="5882" max="5884" width="11.44140625" style="1" hidden="1"/>
     <col min="5885" max="5885" width="16" style="1" hidden="1"/>
-    <col min="5886" max="5886" width="20.42578125" style="1" hidden="1"/>
-    <col min="5887" max="6133" width="11.42578125" style="1" hidden="1"/>
-    <col min="6134" max="6134" width="15.42578125" style="1" hidden="1"/>
-    <col min="6135" max="6135" width="11.42578125" style="1" hidden="1"/>
-    <col min="6136" max="6136" width="15.7109375" style="1" hidden="1"/>
-    <col min="6137" max="6137" width="21.85546875" style="1" hidden="1"/>
-    <col min="6138" max="6140" width="11.42578125" style="1" hidden="1"/>
+    <col min="5886" max="5886" width="20.44140625" style="1" hidden="1"/>
+    <col min="5887" max="6133" width="11.44140625" style="1" hidden="1"/>
+    <col min="6134" max="6134" width="15.44140625" style="1" hidden="1"/>
+    <col min="6135" max="6135" width="11.44140625" style="1" hidden="1"/>
+    <col min="6136" max="6136" width="15.6640625" style="1" hidden="1"/>
+    <col min="6137" max="6137" width="21.88671875" style="1" hidden="1"/>
+    <col min="6138" max="6140" width="11.44140625" style="1" hidden="1"/>
     <col min="6141" max="6141" width="16" style="1" hidden="1"/>
-    <col min="6142" max="6142" width="20.42578125" style="1" hidden="1"/>
-    <col min="6143" max="6389" width="11.42578125" style="1" hidden="1"/>
-    <col min="6390" max="6390" width="15.42578125" style="1" hidden="1"/>
-    <col min="6391" max="6391" width="11.42578125" style="1" hidden="1"/>
-    <col min="6392" max="6392" width="15.7109375" style="1" hidden="1"/>
-    <col min="6393" max="6393" width="21.85546875" style="1" hidden="1"/>
-    <col min="6394" max="6396" width="11.42578125" style="1" hidden="1"/>
+    <col min="6142" max="6142" width="20.44140625" style="1" hidden="1"/>
+    <col min="6143" max="6389" width="11.44140625" style="1" hidden="1"/>
+    <col min="6390" max="6390" width="15.44140625" style="1" hidden="1"/>
+    <col min="6391" max="6391" width="11.44140625" style="1" hidden="1"/>
+    <col min="6392" max="6392" width="15.6640625" style="1" hidden="1"/>
+    <col min="6393" max="6393" width="21.88671875" style="1" hidden="1"/>
+    <col min="6394" max="6396" width="11.44140625" style="1" hidden="1"/>
     <col min="6397" max="6397" width="16" style="1" hidden="1"/>
-    <col min="6398" max="6398" width="20.42578125" style="1" hidden="1"/>
-    <col min="6399" max="6645" width="11.42578125" style="1" hidden="1"/>
-    <col min="6646" max="6646" width="15.42578125" style="1" hidden="1"/>
-    <col min="6647" max="6647" width="11.42578125" style="1" hidden="1"/>
-    <col min="6648" max="6648" width="15.7109375" style="1" hidden="1"/>
-    <col min="6649" max="6649" width="21.85546875" style="1" hidden="1"/>
-    <col min="6650" max="6652" width="11.42578125" style="1" hidden="1"/>
+    <col min="6398" max="6398" width="20.44140625" style="1" hidden="1"/>
+    <col min="6399" max="6645" width="11.44140625" style="1" hidden="1"/>
+    <col min="6646" max="6646" width="15.44140625" style="1" hidden="1"/>
+    <col min="6647" max="6647" width="11.44140625" style="1" hidden="1"/>
+    <col min="6648" max="6648" width="15.6640625" style="1" hidden="1"/>
+    <col min="6649" max="6649" width="21.88671875" style="1" hidden="1"/>
+    <col min="6650" max="6652" width="11.44140625" style="1" hidden="1"/>
     <col min="6653" max="6653" width="16" style="1" hidden="1"/>
-    <col min="6654" max="6654" width="20.42578125" style="1" hidden="1"/>
-    <col min="6655" max="6901" width="11.42578125" style="1" hidden="1"/>
-    <col min="6902" max="6902" width="15.42578125" style="1" hidden="1"/>
-    <col min="6903" max="6903" width="11.42578125" style="1" hidden="1"/>
-    <col min="6904" max="6904" width="15.7109375" style="1" hidden="1"/>
-    <col min="6905" max="6905" width="21.85546875" style="1" hidden="1"/>
-    <col min="6906" max="6908" width="11.42578125" style="1" hidden="1"/>
+    <col min="6654" max="6654" width="20.44140625" style="1" hidden="1"/>
+    <col min="6655" max="6901" width="11.44140625" style="1" hidden="1"/>
+    <col min="6902" max="6902" width="15.44140625" style="1" hidden="1"/>
+    <col min="6903" max="6903" width="11.44140625" style="1" hidden="1"/>
+    <col min="6904" max="6904" width="15.6640625" style="1" hidden="1"/>
+    <col min="6905" max="6905" width="21.88671875" style="1" hidden="1"/>
+    <col min="6906" max="6908" width="11.44140625" style="1" hidden="1"/>
     <col min="6909" max="6909" width="16" style="1" hidden="1"/>
-    <col min="6910" max="6910" width="20.42578125" style="1" hidden="1"/>
-    <col min="6911" max="7157" width="11.42578125" style="1" hidden="1"/>
-    <col min="7158" max="7158" width="15.42578125" style="1" hidden="1"/>
-    <col min="7159" max="7159" width="11.42578125" style="1" hidden="1"/>
-    <col min="7160" max="7160" width="15.7109375" style="1" hidden="1"/>
-    <col min="7161" max="7161" width="21.85546875" style="1" hidden="1"/>
-    <col min="7162" max="7164" width="11.42578125" style="1" hidden="1"/>
+    <col min="6910" max="6910" width="20.44140625" style="1" hidden="1"/>
+    <col min="6911" max="7157" width="11.44140625" style="1" hidden="1"/>
+    <col min="7158" max="7158" width="15.44140625" style="1" hidden="1"/>
+    <col min="7159" max="7159" width="11.44140625" style="1" hidden="1"/>
+    <col min="7160" max="7160" width="15.6640625" style="1" hidden="1"/>
+    <col min="7161" max="7161" width="21.88671875" style="1" hidden="1"/>
+    <col min="7162" max="7164" width="11.44140625" style="1" hidden="1"/>
     <col min="7165" max="7165" width="16" style="1" hidden="1"/>
-    <col min="7166" max="7166" width="20.42578125" style="1" hidden="1"/>
-    <col min="7167" max="7413" width="11.42578125" style="1" hidden="1"/>
-    <col min="7414" max="7414" width="15.42578125" style="1" hidden="1"/>
-    <col min="7415" max="7415" width="11.42578125" style="1" hidden="1"/>
-    <col min="7416" max="7416" width="15.7109375" style="1" hidden="1"/>
-    <col min="7417" max="7417" width="21.85546875" style="1" hidden="1"/>
-    <col min="7418" max="7420" width="11.42578125" style="1" hidden="1"/>
+    <col min="7166" max="7166" width="20.44140625" style="1" hidden="1"/>
+    <col min="7167" max="7413" width="11.44140625" style="1" hidden="1"/>
+    <col min="7414" max="7414" width="15.44140625" style="1" hidden="1"/>
+    <col min="7415" max="7415" width="11.44140625" style="1" hidden="1"/>
+    <col min="7416" max="7416" width="15.6640625" style="1" hidden="1"/>
+    <col min="7417" max="7417" width="21.88671875" style="1" hidden="1"/>
+    <col min="7418" max="7420" width="11.44140625" style="1" hidden="1"/>
     <col min="7421" max="7421" width="16" style="1" hidden="1"/>
-    <col min="7422" max="7422" width="20.42578125" style="1" hidden="1"/>
-    <col min="7423" max="7669" width="11.42578125" style="1" hidden="1"/>
-    <col min="7670" max="7670" width="15.42578125" style="1" hidden="1"/>
-    <col min="7671" max="7671" width="11.42578125" style="1" hidden="1"/>
-    <col min="7672" max="7672" width="15.7109375" style="1" hidden="1"/>
-    <col min="7673" max="7673" width="21.85546875" style="1" hidden="1"/>
-    <col min="7674" max="7676" width="11.42578125" style="1" hidden="1"/>
+    <col min="7422" max="7422" width="20.44140625" style="1" hidden="1"/>
+    <col min="7423" max="7669" width="11.44140625" style="1" hidden="1"/>
+    <col min="7670" max="7670" width="15.44140625" style="1" hidden="1"/>
+    <col min="7671" max="7671" width="11.44140625" style="1" hidden="1"/>
+    <col min="7672" max="7672" width="15.6640625" style="1" hidden="1"/>
+    <col min="7673" max="7673" width="21.88671875" style="1" hidden="1"/>
+    <col min="7674" max="7676" width="11.44140625" style="1" hidden="1"/>
     <col min="7677" max="7677" width="16" style="1" hidden="1"/>
-    <col min="7678" max="7678" width="20.42578125" style="1" hidden="1"/>
-    <col min="7679" max="7925" width="11.42578125" style="1" hidden="1"/>
-    <col min="7926" max="7926" width="15.42578125" style="1" hidden="1"/>
-    <col min="7927" max="7927" width="11.42578125" style="1" hidden="1"/>
-    <col min="7928" max="7928" width="15.7109375" style="1" hidden="1"/>
-    <col min="7929" max="7929" width="21.85546875" style="1" hidden="1"/>
-    <col min="7930" max="7932" width="11.42578125" style="1" hidden="1"/>
+    <col min="7678" max="7678" width="20.44140625" style="1" hidden="1"/>
+    <col min="7679" max="7925" width="11.44140625" style="1" hidden="1"/>
+    <col min="7926" max="7926" width="15.44140625" style="1" hidden="1"/>
+    <col min="7927" max="7927" width="11.44140625" style="1" hidden="1"/>
+    <col min="7928" max="7928" width="15.6640625" style="1" hidden="1"/>
+    <col min="7929" max="7929" width="21.88671875" style="1" hidden="1"/>
+    <col min="7930" max="7932" width="11.44140625" style="1" hidden="1"/>
     <col min="7933" max="7933" width="16" style="1" hidden="1"/>
-    <col min="7934" max="7934" width="20.42578125" style="1" hidden="1"/>
-    <col min="7935" max="8181" width="11.42578125" style="1" hidden="1"/>
-    <col min="8182" max="8182" width="15.42578125" style="1" hidden="1"/>
-    <col min="8183" max="8183" width="11.42578125" style="1" hidden="1"/>
-    <col min="8184" max="8184" width="15.7109375" style="1" hidden="1"/>
-    <col min="8185" max="8185" width="21.85546875" style="1" hidden="1"/>
-    <col min="8186" max="8188" width="11.42578125" style="1" hidden="1"/>
+    <col min="7934" max="7934" width="20.44140625" style="1" hidden="1"/>
+    <col min="7935" max="8181" width="11.44140625" style="1" hidden="1"/>
+    <col min="8182" max="8182" width="15.44140625" style="1" hidden="1"/>
+    <col min="8183" max="8183" width="11.44140625" style="1" hidden="1"/>
+    <col min="8184" max="8184" width="15.6640625" style="1" hidden="1"/>
+    <col min="8185" max="8185" width="21.88671875" style="1" hidden="1"/>
+    <col min="8186" max="8188" width="11.44140625" style="1" hidden="1"/>
     <col min="8189" max="8189" width="16" style="1" hidden="1"/>
-    <col min="8190" max="8190" width="20.42578125" style="1" hidden="1"/>
-    <col min="8191" max="8437" width="11.42578125" style="1" hidden="1"/>
-    <col min="8438" max="8438" width="15.42578125" style="1" hidden="1"/>
-    <col min="8439" max="8439" width="11.42578125" style="1" hidden="1"/>
-    <col min="8440" max="8440" width="15.7109375" style="1" hidden="1"/>
-    <col min="8441" max="8441" width="21.85546875" style="1" hidden="1"/>
-    <col min="8442" max="8444" width="11.42578125" style="1" hidden="1"/>
+    <col min="8190" max="8190" width="20.44140625" style="1" hidden="1"/>
+    <col min="8191" max="8437" width="11.44140625" style="1" hidden="1"/>
+    <col min="8438" max="8438" width="15.44140625" style="1" hidden="1"/>
+    <col min="8439" max="8439" width="11.44140625" style="1" hidden="1"/>
+    <col min="8440" max="8440" width="15.6640625" style="1" hidden="1"/>
+    <col min="8441" max="8441" width="21.88671875" style="1" hidden="1"/>
+    <col min="8442" max="8444" width="11.44140625" style="1" hidden="1"/>
     <col min="8445" max="8445" width="16" style="1" hidden="1"/>
-    <col min="8446" max="8446" width="20.42578125" style="1" hidden="1"/>
-    <col min="8447" max="8693" width="11.42578125" style="1" hidden="1"/>
-    <col min="8694" max="8694" width="15.42578125" style="1" hidden="1"/>
-    <col min="8695" max="8695" width="11.42578125" style="1" hidden="1"/>
-    <col min="8696" max="8696" width="15.7109375" style="1" hidden="1"/>
-    <col min="8697" max="8697" width="21.85546875" style="1" hidden="1"/>
-    <col min="8698" max="8700" width="11.42578125" style="1" hidden="1"/>
+    <col min="8446" max="8446" width="20.44140625" style="1" hidden="1"/>
+    <col min="8447" max="8693" width="11.44140625" style="1" hidden="1"/>
+    <col min="8694" max="8694" width="15.44140625" style="1" hidden="1"/>
+    <col min="8695" max="8695" width="11.44140625" style="1" hidden="1"/>
+    <col min="8696" max="8696" width="15.6640625" style="1" hidden="1"/>
+    <col min="8697" max="8697" width="21.88671875" style="1" hidden="1"/>
+    <col min="8698" max="8700" width="11.44140625" style="1" hidden="1"/>
     <col min="8701" max="8701" width="16" style="1" hidden="1"/>
-    <col min="8702" max="8702" width="20.42578125" style="1" hidden="1"/>
-    <col min="8703" max="8949" width="11.42578125" style="1" hidden="1"/>
-    <col min="8950" max="8950" width="15.42578125" style="1" hidden="1"/>
-    <col min="8951" max="8951" width="11.42578125" style="1" hidden="1"/>
-    <col min="8952" max="8952" width="15.7109375" style="1" hidden="1"/>
-    <col min="8953" max="8953" width="21.85546875" style="1" hidden="1"/>
-    <col min="8954" max="8956" width="11.42578125" style="1" hidden="1"/>
+    <col min="8702" max="8702" width="20.44140625" style="1" hidden="1"/>
+    <col min="8703" max="8949" width="11.44140625" style="1" hidden="1"/>
+    <col min="8950" max="8950" width="15.44140625" style="1" hidden="1"/>
+    <col min="8951" max="8951" width="11.44140625" style="1" hidden="1"/>
+    <col min="8952" max="8952" width="15.6640625" style="1" hidden="1"/>
+    <col min="8953" max="8953" width="21.88671875" style="1" hidden="1"/>
+    <col min="8954" max="8956" width="11.44140625" style="1" hidden="1"/>
     <col min="8957" max="8957" width="16" style="1" hidden="1"/>
-    <col min="8958" max="8958" width="20.42578125" style="1" hidden="1"/>
-    <col min="8959" max="9205" width="11.42578125" style="1" hidden="1"/>
-    <col min="9206" max="9206" width="15.42578125" style="1" hidden="1"/>
-    <col min="9207" max="9207" width="11.42578125" style="1" hidden="1"/>
-    <col min="9208" max="9208" width="15.7109375" style="1" hidden="1"/>
-    <col min="9209" max="9209" width="21.85546875" style="1" hidden="1"/>
-    <col min="9210" max="9212" width="11.42578125" style="1" hidden="1"/>
+    <col min="8958" max="8958" width="20.44140625" style="1" hidden="1"/>
+    <col min="8959" max="9205" width="11.44140625" style="1" hidden="1"/>
+    <col min="9206" max="9206" width="15.44140625" style="1" hidden="1"/>
+    <col min="9207" max="9207" width="11.44140625" style="1" hidden="1"/>
+    <col min="9208" max="9208" width="15.6640625" style="1" hidden="1"/>
+    <col min="9209" max="9209" width="21.88671875" style="1" hidden="1"/>
+    <col min="9210" max="9212" width="11.44140625" style="1" hidden="1"/>
     <col min="9213" max="9213" width="16" style="1" hidden="1"/>
-    <col min="9214" max="9214" width="20.42578125" style="1" hidden="1"/>
-    <col min="9215" max="9461" width="11.42578125" style="1" hidden="1"/>
-    <col min="9462" max="9462" width="15.42578125" style="1" hidden="1"/>
-    <col min="9463" max="9463" width="11.42578125" style="1" hidden="1"/>
-    <col min="9464" max="9464" width="15.7109375" style="1" hidden="1"/>
-    <col min="9465" max="9465" width="21.85546875" style="1" hidden="1"/>
-    <col min="9466" max="9468" width="11.42578125" style="1" hidden="1"/>
+    <col min="9214" max="9214" width="20.44140625" style="1" hidden="1"/>
+    <col min="9215" max="9461" width="11.44140625" style="1" hidden="1"/>
+    <col min="9462" max="9462" width="15.44140625" style="1" hidden="1"/>
+    <col min="9463" max="9463" width="11.44140625" style="1" hidden="1"/>
+    <col min="9464" max="9464" width="15.6640625" style="1" hidden="1"/>
+    <col min="9465" max="9465" width="21.88671875" style="1" hidden="1"/>
+    <col min="9466" max="9468" width="11.44140625" style="1" hidden="1"/>
     <col min="9469" max="9469" width="16" style="1" hidden="1"/>
-    <col min="9470" max="9470" width="20.42578125" style="1" hidden="1"/>
-    <col min="9471" max="9717" width="11.42578125" style="1" hidden="1"/>
-    <col min="9718" max="9718" width="15.42578125" style="1" hidden="1"/>
-    <col min="9719" max="9719" width="11.42578125" style="1" hidden="1"/>
-    <col min="9720" max="9720" width="15.7109375" style="1" hidden="1"/>
-    <col min="9721" max="9721" width="21.85546875" style="1" hidden="1"/>
-    <col min="9722" max="9724" width="11.42578125" style="1" hidden="1"/>
+    <col min="9470" max="9470" width="20.44140625" style="1" hidden="1"/>
+    <col min="9471" max="9717" width="11.44140625" style="1" hidden="1"/>
+    <col min="9718" max="9718" width="15.44140625" style="1" hidden="1"/>
+    <col min="9719" max="9719" width="11.44140625" style="1" hidden="1"/>
+    <col min="9720" max="9720" width="15.6640625" style="1" hidden="1"/>
+    <col min="9721" max="9721" width="21.88671875" style="1" hidden="1"/>
+    <col min="9722" max="9724" width="11.44140625" style="1" hidden="1"/>
     <col min="9725" max="9725" width="16" style="1" hidden="1"/>
-    <col min="9726" max="9726" width="20.42578125" style="1" hidden="1"/>
-    <col min="9727" max="9973" width="11.42578125" style="1" hidden="1"/>
-    <col min="9974" max="9974" width="15.42578125" style="1" hidden="1"/>
-    <col min="9975" max="9975" width="11.42578125" style="1" hidden="1"/>
-    <col min="9976" max="9976" width="15.7109375" style="1" hidden="1"/>
-    <col min="9977" max="9977" width="21.85546875" style="1" hidden="1"/>
-    <col min="9978" max="9980" width="11.42578125" style="1" hidden="1"/>
+    <col min="9726" max="9726" width="20.44140625" style="1" hidden="1"/>
+    <col min="9727" max="9973" width="11.44140625" style="1" hidden="1"/>
+    <col min="9974" max="9974" width="15.44140625" style="1" hidden="1"/>
+    <col min="9975" max="9975" width="11.44140625" style="1" hidden="1"/>
+    <col min="9976" max="9976" width="15.6640625" style="1" hidden="1"/>
+    <col min="9977" max="9977" width="21.88671875" style="1" hidden="1"/>
+    <col min="9978" max="9980" width="11.44140625" style="1" hidden="1"/>
     <col min="9981" max="9981" width="16" style="1" hidden="1"/>
-    <col min="9982" max="9982" width="20.42578125" style="1" hidden="1"/>
-    <col min="9983" max="10229" width="11.42578125" style="1" hidden="1"/>
-    <col min="10230" max="10230" width="15.42578125" style="1" hidden="1"/>
-    <col min="10231" max="10231" width="11.42578125" style="1" hidden="1"/>
-    <col min="10232" max="10232" width="15.7109375" style="1" hidden="1"/>
-    <col min="10233" max="10233" width="21.85546875" style="1" hidden="1"/>
-    <col min="10234" max="10236" width="11.42578125" style="1" hidden="1"/>
+    <col min="9982" max="9982" width="20.44140625" style="1" hidden="1"/>
+    <col min="9983" max="10229" width="11.44140625" style="1" hidden="1"/>
+    <col min="10230" max="10230" width="15.44140625" style="1" hidden="1"/>
+    <col min="10231" max="10231" width="11.44140625" style="1" hidden="1"/>
+    <col min="10232" max="10232" width="15.6640625" style="1" hidden="1"/>
+    <col min="10233" max="10233" width="21.88671875" style="1" hidden="1"/>
+    <col min="10234" max="10236" width="11.44140625" style="1" hidden="1"/>
     <col min="10237" max="10237" width="16" style="1" hidden="1"/>
-    <col min="10238" max="10238" width="20.42578125" style="1" hidden="1"/>
-    <col min="10239" max="10485" width="11.42578125" style="1" hidden="1"/>
-    <col min="10486" max="10486" width="15.42578125" style="1" hidden="1"/>
-    <col min="10487" max="10487" width="11.42578125" style="1" hidden="1"/>
-    <col min="10488" max="10488" width="15.7109375" style="1" hidden="1"/>
-    <col min="10489" max="10489" width="21.85546875" style="1" hidden="1"/>
-    <col min="10490" max="10492" width="11.42578125" style="1" hidden="1"/>
+    <col min="10238" max="10238" width="20.44140625" style="1" hidden="1"/>
+    <col min="10239" max="10485" width="11.44140625" style="1" hidden="1"/>
+    <col min="10486" max="10486" width="15.44140625" style="1" hidden="1"/>
+    <col min="10487" max="10487" width="11.44140625" style="1" hidden="1"/>
+    <col min="10488" max="10488" width="15.6640625" style="1" hidden="1"/>
+    <col min="10489" max="10489" width="21.88671875" style="1" hidden="1"/>
+    <col min="10490" max="10492" width="11.44140625" style="1" hidden="1"/>
     <col min="10493" max="10493" width="16" style="1" hidden="1"/>
-    <col min="10494" max="10494" width="20.42578125" style="1" hidden="1"/>
-    <col min="10495" max="10741" width="11.42578125" style="1" hidden="1"/>
-    <col min="10742" max="10742" width="15.42578125" style="1" hidden="1"/>
-    <col min="10743" max="10743" width="11.42578125" style="1" hidden="1"/>
-    <col min="10744" max="10744" width="15.7109375" style="1" hidden="1"/>
-    <col min="10745" max="10745" width="21.85546875" style="1" hidden="1"/>
-    <col min="10746" max="10748" width="11.42578125" style="1" hidden="1"/>
+    <col min="10494" max="10494" width="20.44140625" style="1" hidden="1"/>
+    <col min="10495" max="10741" width="11.44140625" style="1" hidden="1"/>
+    <col min="10742" max="10742" width="15.44140625" style="1" hidden="1"/>
+    <col min="10743" max="10743" width="11.44140625" style="1" hidden="1"/>
+    <col min="10744" max="10744" width="15.6640625" style="1" hidden="1"/>
+    <col min="10745" max="10745" width="21.88671875" style="1" hidden="1"/>
+    <col min="10746" max="10748" width="11.44140625" style="1" hidden="1"/>
     <col min="10749" max="10749" width="16" style="1" hidden="1"/>
-    <col min="10750" max="10750" width="20.42578125" style="1" hidden="1"/>
-    <col min="10751" max="10997" width="11.42578125" style="1" hidden="1"/>
-    <col min="10998" max="10998" width="15.42578125" style="1" hidden="1"/>
-    <col min="10999" max="10999" width="11.42578125" style="1" hidden="1"/>
-    <col min="11000" max="11000" width="15.7109375" style="1" hidden="1"/>
-    <col min="11001" max="11001" width="21.85546875" style="1" hidden="1"/>
-    <col min="11002" max="11004" width="11.42578125" style="1" hidden="1"/>
+    <col min="10750" max="10750" width="20.44140625" style="1" hidden="1"/>
+    <col min="10751" max="10997" width="11.44140625" style="1" hidden="1"/>
+    <col min="10998" max="10998" width="15.44140625" style="1" hidden="1"/>
+    <col min="10999" max="10999" width="11.44140625" style="1" hidden="1"/>
+    <col min="11000" max="11000" width="15.6640625" style="1" hidden="1"/>
+    <col min="11001" max="11001" width="21.88671875" style="1" hidden="1"/>
+    <col min="11002" max="11004" width="11.44140625" style="1" hidden="1"/>
     <col min="11005" max="11005" width="16" style="1" hidden="1"/>
-    <col min="11006" max="11006" width="20.42578125" style="1" hidden="1"/>
-    <col min="11007" max="11253" width="11.42578125" style="1" hidden="1"/>
-    <col min="11254" max="11254" width="15.42578125" style="1" hidden="1"/>
-    <col min="11255" max="11255" width="11.42578125" style="1" hidden="1"/>
-    <col min="11256" max="11256" width="15.7109375" style="1" hidden="1"/>
-    <col min="11257" max="11257" width="21.85546875" style="1" hidden="1"/>
-    <col min="11258" max="11260" width="11.42578125" style="1" hidden="1"/>
+    <col min="11006" max="11006" width="20.44140625" style="1" hidden="1"/>
+    <col min="11007" max="11253" width="11.44140625" style="1" hidden="1"/>
+    <col min="11254" max="11254" width="15.44140625" style="1" hidden="1"/>
+    <col min="11255" max="11255" width="11.44140625" style="1" hidden="1"/>
+    <col min="11256" max="11256" width="15.6640625" style="1" hidden="1"/>
+    <col min="11257" max="11257" width="21.88671875" style="1" hidden="1"/>
+    <col min="11258" max="11260" width="11.44140625" style="1" hidden="1"/>
     <col min="11261" max="11261" width="16" style="1" hidden="1"/>
-    <col min="11262" max="11262" width="20.42578125" style="1" hidden="1"/>
-    <col min="11263" max="11509" width="11.42578125" style="1" hidden="1"/>
-    <col min="11510" max="11510" width="15.42578125" style="1" hidden="1"/>
-    <col min="11511" max="11511" width="11.42578125" style="1" hidden="1"/>
-    <col min="11512" max="11512" width="15.7109375" style="1" hidden="1"/>
-    <col min="11513" max="11513" width="21.85546875" style="1" hidden="1"/>
-    <col min="11514" max="11516" width="11.42578125" style="1" hidden="1"/>
+    <col min="11262" max="11262" width="20.44140625" style="1" hidden="1"/>
+    <col min="11263" max="11509" width="11.44140625" style="1" hidden="1"/>
+    <col min="11510" max="11510" width="15.44140625" style="1" hidden="1"/>
+    <col min="11511" max="11511" width="11.44140625" style="1" hidden="1"/>
+    <col min="11512" max="11512" width="15.6640625" style="1" hidden="1"/>
+    <col min="11513" max="11513" width="21.88671875" style="1" hidden="1"/>
+    <col min="11514" max="11516" width="11.44140625" style="1" hidden="1"/>
     <col min="11517" max="11517" width="16" style="1" hidden="1"/>
-    <col min="11518" max="11518" width="20.42578125" style="1" hidden="1"/>
-    <col min="11519" max="11765" width="11.42578125" style="1" hidden="1"/>
-    <col min="11766" max="11766" width="15.42578125" style="1" hidden="1"/>
-    <col min="11767" max="11767" width="11.42578125" style="1" hidden="1"/>
-    <col min="11768" max="11768" width="15.7109375" style="1" hidden="1"/>
-    <col min="11769" max="11769" width="21.85546875" style="1" hidden="1"/>
-    <col min="11770" max="11772" width="11.42578125" style="1" hidden="1"/>
+    <col min="11518" max="11518" width="20.44140625" style="1" hidden="1"/>
+    <col min="11519" max="11765" width="11.44140625" style="1" hidden="1"/>
+    <col min="11766" max="11766" width="15.44140625" style="1" hidden="1"/>
+    <col min="11767" max="11767" width="11.44140625" style="1" hidden="1"/>
+    <col min="11768" max="11768" width="15.6640625" style="1" hidden="1"/>
+    <col min="11769" max="11769" width="21.88671875" style="1" hidden="1"/>
+    <col min="11770" max="11772" width="11.44140625" style="1" hidden="1"/>
     <col min="11773" max="11773" width="16" style="1" hidden="1"/>
-    <col min="11774" max="11774" width="20.42578125" style="1" hidden="1"/>
-    <col min="11775" max="12021" width="11.42578125" style="1" hidden="1"/>
-    <col min="12022" max="12022" width="15.42578125" style="1" hidden="1"/>
-    <col min="12023" max="12023" width="11.42578125" style="1" hidden="1"/>
-    <col min="12024" max="12024" width="15.7109375" style="1" hidden="1"/>
-    <col min="12025" max="12025" width="21.85546875" style="1" hidden="1"/>
-    <col min="12026" max="12028" width="11.42578125" style="1" hidden="1"/>
+    <col min="11774" max="11774" width="20.44140625" style="1" hidden="1"/>
+    <col min="11775" max="12021" width="11.44140625" style="1" hidden="1"/>
+    <col min="12022" max="12022" width="15.44140625" style="1" hidden="1"/>
+    <col min="12023" max="12023" width="11.44140625" style="1" hidden="1"/>
+    <col min="12024" max="12024" width="15.6640625" style="1" hidden="1"/>
+    <col min="12025" max="12025" width="21.88671875" style="1" hidden="1"/>
+    <col min="12026" max="12028" width="11.44140625" style="1" hidden="1"/>
     <col min="12029" max="12029" width="16" style="1" hidden="1"/>
-    <col min="12030" max="12030" width="20.42578125" style="1" hidden="1"/>
-    <col min="12031" max="12277" width="11.42578125" style="1" hidden="1"/>
-    <col min="12278" max="12278" width="15.42578125" style="1" hidden="1"/>
-    <col min="12279" max="12279" width="11.42578125" style="1" hidden="1"/>
-    <col min="12280" max="12280" width="15.7109375" style="1" hidden="1"/>
-    <col min="12281" max="12281" width="21.85546875" style="1" hidden="1"/>
-    <col min="12282" max="12284" width="11.42578125" style="1" hidden="1"/>
+    <col min="12030" max="12030" width="20.44140625" style="1" hidden="1"/>
+    <col min="12031" max="12277" width="11.44140625" style="1" hidden="1"/>
+    <col min="12278" max="12278" width="15.44140625" style="1" hidden="1"/>
+    <col min="12279" max="12279" width="11.44140625" style="1" hidden="1"/>
+    <col min="12280" max="12280" width="15.6640625" style="1" hidden="1"/>
+    <col min="12281" max="12281" width="21.88671875" style="1" hidden="1"/>
+    <col min="12282" max="12284" width="11.44140625" style="1" hidden="1"/>
     <col min="12285" max="12285" width="16" style="1" hidden="1"/>
-    <col min="12286" max="12286" width="20.42578125" style="1" hidden="1"/>
-    <col min="12287" max="12533" width="11.42578125" style="1" hidden="1"/>
-    <col min="12534" max="12534" width="15.42578125" style="1" hidden="1"/>
-    <col min="12535" max="12535" width="11.42578125" style="1" hidden="1"/>
-    <col min="12536" max="12536" width="15.7109375" style="1" hidden="1"/>
-    <col min="12537" max="12537" width="21.85546875" style="1" hidden="1"/>
-    <col min="12538" max="12540" width="11.42578125" style="1" hidden="1"/>
+    <col min="12286" max="12286" width="20.44140625" style="1" hidden="1"/>
+    <col min="12287" max="12533" width="11.44140625" style="1" hidden="1"/>
+    <col min="12534" max="12534" width="15.44140625" style="1" hidden="1"/>
+    <col min="12535" max="12535" width="11.44140625" style="1" hidden="1"/>
+    <col min="12536" max="12536" width="15.6640625" style="1" hidden="1"/>
+    <col min="12537" max="12537" width="21.88671875" style="1" hidden="1"/>
+    <col min="12538" max="12540" width="11.44140625" style="1" hidden="1"/>
     <col min="12541" max="12541" width="16" style="1" hidden="1"/>
-    <col min="12542" max="12542" width="20.42578125" style="1" hidden="1"/>
-    <col min="12543" max="12789" width="11.42578125" style="1" hidden="1"/>
-    <col min="12790" max="12790" width="15.42578125" style="1" hidden="1"/>
-    <col min="12791" max="12791" width="11.42578125" style="1" hidden="1"/>
-    <col min="12792" max="12792" width="15.7109375" style="1" hidden="1"/>
-    <col min="12793" max="12793" width="21.85546875" style="1" hidden="1"/>
-    <col min="12794" max="12796" width="11.42578125" style="1" hidden="1"/>
+    <col min="12542" max="12542" width="20.44140625" style="1" hidden="1"/>
+    <col min="12543" max="12789" width="11.44140625" style="1" hidden="1"/>
+    <col min="12790" max="12790" width="15.44140625" style="1" hidden="1"/>
+    <col min="12791" max="12791" width="11.44140625" style="1" hidden="1"/>
+    <col min="12792" max="12792" width="15.6640625" style="1" hidden="1"/>
+    <col min="12793" max="12793" width="21.88671875" style="1" hidden="1"/>
+    <col min="12794" max="12796" width="11.44140625" style="1" hidden="1"/>
     <col min="12797" max="12797" width="16" style="1" hidden="1"/>
-    <col min="12798" max="12798" width="20.42578125" style="1" hidden="1"/>
-    <col min="12799" max="13045" width="11.42578125" style="1" hidden="1"/>
-    <col min="13046" max="13046" width="15.42578125" style="1" hidden="1"/>
-    <col min="13047" max="13047" width="11.42578125" style="1" hidden="1"/>
-    <col min="13048" max="13048" width="15.7109375" style="1" hidden="1"/>
-    <col min="13049" max="13049" width="21.85546875" style="1" hidden="1"/>
-    <col min="13050" max="13052" width="11.42578125" style="1" hidden="1"/>
+    <col min="12798" max="12798" width="20.44140625" style="1" hidden="1"/>
+    <col min="12799" max="13045" width="11.44140625" style="1" hidden="1"/>
+    <col min="13046" max="13046" width="15.44140625" style="1" hidden="1"/>
+    <col min="13047" max="13047" width="11.44140625" style="1" hidden="1"/>
+    <col min="13048" max="13048" width="15.6640625" style="1" hidden="1"/>
+    <col min="13049" max="13049" width="21.88671875" style="1" hidden="1"/>
+    <col min="13050" max="13052" width="11.44140625" style="1" hidden="1"/>
     <col min="13053" max="13053" width="16" style="1" hidden="1"/>
-    <col min="13054" max="13054" width="20.42578125" style="1" hidden="1"/>
-    <col min="13055" max="13301" width="11.42578125" style="1" hidden="1"/>
-    <col min="13302" max="13302" width="15.42578125" style="1" hidden="1"/>
-    <col min="13303" max="13303" width="11.42578125" style="1" hidden="1"/>
-    <col min="13304" max="13304" width="15.7109375" style="1" hidden="1"/>
-    <col min="13305" max="13305" width="21.85546875" style="1" hidden="1"/>
-    <col min="13306" max="13308" width="11.42578125" style="1" hidden="1"/>
+    <col min="13054" max="13054" width="20.44140625" style="1" hidden="1"/>
+    <col min="13055" max="13301" width="11.44140625" style="1" hidden="1"/>
+    <col min="13302" max="13302" width="15.44140625" style="1" hidden="1"/>
+    <col min="13303" max="13303" width="11.44140625" style="1" hidden="1"/>
+    <col min="13304" max="13304" width="15.6640625" style="1" hidden="1"/>
+    <col min="13305" max="13305" width="21.88671875" style="1" hidden="1"/>
+    <col min="13306" max="13308" width="11.44140625" style="1" hidden="1"/>
     <col min="13309" max="13309" width="16" style="1" hidden="1"/>
-    <col min="13310" max="13310" width="20.42578125" style="1" hidden="1"/>
-    <col min="13311" max="13557" width="11.42578125" style="1" hidden="1"/>
-    <col min="13558" max="13558" width="15.42578125" style="1" hidden="1"/>
-    <col min="13559" max="13559" width="11.42578125" style="1" hidden="1"/>
-    <col min="13560" max="13560" width="15.7109375" style="1" hidden="1"/>
-    <col min="13561" max="13561" width="21.85546875" style="1" hidden="1"/>
-    <col min="13562" max="13564" width="11.42578125" style="1" hidden="1"/>
+    <col min="13310" max="13310" width="20.44140625" style="1" hidden="1"/>
+    <col min="13311" max="13557" width="11.44140625" style="1" hidden="1"/>
+    <col min="13558" max="13558" width="15.44140625" style="1" hidden="1"/>
+    <col min="13559" max="13559" width="11.44140625" style="1" hidden="1"/>
+    <col min="13560" max="13560" width="15.6640625" style="1" hidden="1"/>
+    <col min="13561" max="13561" width="21.88671875" style="1" hidden="1"/>
+    <col min="13562" max="13564" width="11.44140625" style="1" hidden="1"/>
     <col min="13565" max="13565" width="16" style="1" hidden="1"/>
-    <col min="13566" max="13566" width="20.42578125" style="1" hidden="1"/>
-    <col min="13567" max="13813" width="11.42578125" style="1" hidden="1"/>
-    <col min="13814" max="13814" width="15.42578125" style="1" hidden="1"/>
-    <col min="13815" max="13815" width="11.42578125" style="1" hidden="1"/>
-    <col min="13816" max="13816" width="15.7109375" style="1" hidden="1"/>
-    <col min="13817" max="13817" width="21.85546875" style="1" hidden="1"/>
-    <col min="13818" max="13820" width="11.42578125" style="1" hidden="1"/>
+    <col min="13566" max="13566" width="20.44140625" style="1" hidden="1"/>
+    <col min="13567" max="13813" width="11.44140625" style="1" hidden="1"/>
+    <col min="13814" max="13814" width="15.44140625" style="1" hidden="1"/>
+    <col min="13815" max="13815" width="11.44140625" style="1" hidden="1"/>
+    <col min="13816" max="13816" width="15.6640625" style="1" hidden="1"/>
+    <col min="13817" max="13817" width="21.88671875" style="1" hidden="1"/>
+    <col min="13818" max="13820" width="11.44140625" style="1" hidden="1"/>
     <col min="13821" max="13821" width="16" style="1" hidden="1"/>
-    <col min="13822" max="13822" width="20.42578125" style="1" hidden="1"/>
-    <col min="13823" max="14069" width="11.42578125" style="1" hidden="1"/>
-    <col min="14070" max="14070" width="15.42578125" style="1" hidden="1"/>
-    <col min="14071" max="14071" width="11.42578125" style="1" hidden="1"/>
-    <col min="14072" max="14072" width="15.7109375" style="1" hidden="1"/>
-    <col min="14073" max="14073" width="21.85546875" style="1" hidden="1"/>
-    <col min="14074" max="14076" width="11.42578125" style="1" hidden="1"/>
+    <col min="13822" max="13822" width="20.44140625" style="1" hidden="1"/>
+    <col min="13823" max="14069" width="11.44140625" style="1" hidden="1"/>
+    <col min="14070" max="14070" width="15.44140625" style="1" hidden="1"/>
+    <col min="14071" max="14071" width="11.44140625" style="1" hidden="1"/>
+    <col min="14072" max="14072" width="15.6640625" style="1" hidden="1"/>
+    <col min="14073" max="14073" width="21.88671875" style="1" hidden="1"/>
+    <col min="14074" max="14076" width="11.44140625" style="1" hidden="1"/>
     <col min="14077" max="14077" width="16" style="1" hidden="1"/>
-    <col min="14078" max="14078" width="20.42578125" style="1" hidden="1"/>
-    <col min="14079" max="14325" width="11.42578125" style="1" hidden="1"/>
-    <col min="14326" max="14326" width="15.42578125" style="1" hidden="1"/>
-    <col min="14327" max="14327" width="11.42578125" style="1" hidden="1"/>
-    <col min="14328" max="14328" width="15.7109375" style="1" hidden="1"/>
-    <col min="14329" max="14329" width="21.85546875" style="1" hidden="1"/>
-    <col min="14330" max="14332" width="11.42578125" style="1" hidden="1"/>
+    <col min="14078" max="14078" width="20.44140625" style="1" hidden="1"/>
+    <col min="14079" max="14325" width="11.44140625" style="1" hidden="1"/>
+    <col min="14326" max="14326" width="15.44140625" style="1" hidden="1"/>
+    <col min="14327" max="14327" width="11.44140625" style="1" hidden="1"/>
+    <col min="14328" max="14328" width="15.6640625" style="1" hidden="1"/>
+    <col min="14329" max="14329" width="21.88671875" style="1" hidden="1"/>
+    <col min="14330" max="14332" width="11.44140625" style="1" hidden="1"/>
     <col min="14333" max="14333" width="16" style="1" hidden="1"/>
-    <col min="14334" max="14334" width="20.42578125" style="1" hidden="1"/>
-    <col min="14335" max="14581" width="11.42578125" style="1" hidden="1"/>
-    <col min="14582" max="14582" width="15.42578125" style="1" hidden="1"/>
-    <col min="14583" max="14583" width="11.42578125" style="1" hidden="1"/>
-    <col min="14584" max="14584" width="15.7109375" style="1" hidden="1"/>
-    <col min="14585" max="14585" width="21.85546875" style="1" hidden="1"/>
-    <col min="14586" max="14588" width="11.42578125" style="1" hidden="1"/>
+    <col min="14334" max="14334" width="20.44140625" style="1" hidden="1"/>
+    <col min="14335" max="14581" width="11.44140625" style="1" hidden="1"/>
+    <col min="14582" max="14582" width="15.44140625" style="1" hidden="1"/>
+    <col min="14583" max="14583" width="11.44140625" style="1" hidden="1"/>
+    <col min="14584" max="14584" width="15.6640625" style="1" hidden="1"/>
+    <col min="14585" max="14585" width="21.88671875" style="1" hidden="1"/>
+    <col min="14586" max="14588" width="11.44140625" style="1" hidden="1"/>
     <col min="14589" max="14589" width="16" style="1" hidden="1"/>
-    <col min="14590" max="14590" width="20.42578125" style="1" hidden="1"/>
-    <col min="14591" max="14837" width="11.42578125" style="1" hidden="1"/>
-    <col min="14838" max="14838" width="15.42578125" style="1" hidden="1"/>
-    <col min="14839" max="14839" width="11.42578125" style="1" hidden="1"/>
-    <col min="14840" max="14840" width="15.7109375" style="1" hidden="1"/>
-    <col min="14841" max="14841" width="21.85546875" style="1" hidden="1"/>
-    <col min="14842" max="14844" width="11.42578125" style="1" hidden="1"/>
+    <col min="14590" max="14590" width="20.44140625" style="1" hidden="1"/>
+    <col min="14591" max="14837" width="11.44140625" style="1" hidden="1"/>
+    <col min="14838" max="14838" width="15.44140625" style="1" hidden="1"/>
+    <col min="14839" max="14839" width="11.44140625" style="1" hidden="1"/>
+    <col min="14840" max="14840" width="15.6640625" style="1" hidden="1"/>
+    <col min="14841" max="14841" width="21.88671875" style="1" hidden="1"/>
+    <col min="14842" max="14844" width="11.44140625" style="1" hidden="1"/>
     <col min="14845" max="14845" width="16" style="1" hidden="1"/>
-    <col min="14846" max="14846" width="20.42578125" style="1" hidden="1"/>
-    <col min="14847" max="15093" width="11.42578125" style="1" hidden="1"/>
-    <col min="15094" max="15094" width="15.42578125" style="1" hidden="1"/>
-    <col min="15095" max="15095" width="11.42578125" style="1" hidden="1"/>
-    <col min="15096" max="15096" width="15.7109375" style="1" hidden="1"/>
-    <col min="15097" max="15097" width="21.85546875" style="1" hidden="1"/>
-    <col min="15098" max="15100" width="11.42578125" style="1" hidden="1"/>
+    <col min="14846" max="14846" width="20.44140625" style="1" hidden="1"/>
+    <col min="14847" max="15093" width="11.44140625" style="1" hidden="1"/>
+    <col min="15094" max="15094" width="15.44140625" style="1" hidden="1"/>
+    <col min="15095" max="15095" width="11.44140625" style="1" hidden="1"/>
+    <col min="15096" max="15096" width="15.6640625" style="1" hidden="1"/>
+    <col min="15097" max="15097" width="21.88671875" style="1" hidden="1"/>
+    <col min="15098" max="15100" width="11.44140625" style="1" hidden="1"/>
     <col min="15101" max="15101" width="16" style="1" hidden="1"/>
-    <col min="15102" max="15102" width="20.42578125" style="1" hidden="1"/>
-    <col min="15103" max="15349" width="11.42578125" style="1" hidden="1"/>
-    <col min="15350" max="15350" width="15.42578125" style="1" hidden="1"/>
-    <col min="15351" max="15351" width="11.42578125" style="1" hidden="1"/>
-    <col min="15352" max="15352" width="15.7109375" style="1" hidden="1"/>
-    <col min="15353" max="15353" width="21.85546875" style="1" hidden="1"/>
-    <col min="15354" max="15356" width="11.42578125" style="1" hidden="1"/>
+    <col min="15102" max="15102" width="20.44140625" style="1" hidden="1"/>
+    <col min="15103" max="15349" width="11.44140625" style="1" hidden="1"/>
+    <col min="15350" max="15350" width="15.44140625" style="1" hidden="1"/>
+    <col min="15351" max="15351" width="11.44140625" style="1" hidden="1"/>
+    <col min="15352" max="15352" width="15.6640625" style="1" hidden="1"/>
+    <col min="15353" max="15353" width="21.88671875" style="1" hidden="1"/>
+    <col min="15354" max="15356" width="11.44140625" style="1" hidden="1"/>
     <col min="15357" max="15357" width="16" style="1" hidden="1"/>
-    <col min="15358" max="15358" width="20.42578125" style="1" hidden="1"/>
-    <col min="15359" max="15605" width="11.42578125" style="1" hidden="1"/>
-    <col min="15606" max="15606" width="15.42578125" style="1" hidden="1"/>
-    <col min="15607" max="15607" width="11.42578125" style="1" hidden="1"/>
-    <col min="15608" max="15608" width="15.7109375" style="1" hidden="1"/>
-    <col min="15609" max="15609" width="21.85546875" style="1" hidden="1"/>
-    <col min="15610" max="15612" width="11.42578125" style="1" hidden="1"/>
+    <col min="15358" max="15358" width="20.44140625" style="1" hidden="1"/>
+    <col min="15359" max="15605" width="11.44140625" style="1" hidden="1"/>
+    <col min="15606" max="15606" width="15.44140625" style="1" hidden="1"/>
+    <col min="15607" max="15607" width="11.44140625" style="1" hidden="1"/>
+    <col min="15608" max="15608" width="15.6640625" style="1" hidden="1"/>
+    <col min="15609" max="15609" width="21.88671875" style="1" hidden="1"/>
+    <col min="15610" max="15612" width="11.44140625" style="1" hidden="1"/>
     <col min="15613" max="15613" width="16" style="1" hidden="1"/>
-    <col min="15614" max="15614" width="20.42578125" style="1" hidden="1"/>
-    <col min="15615" max="15861" width="11.42578125" style="1" hidden="1"/>
-    <col min="15862" max="15862" width="15.42578125" style="1" hidden="1"/>
-    <col min="15863" max="15863" width="11.42578125" style="1" hidden="1"/>
-    <col min="15864" max="15864" width="15.7109375" style="1" hidden="1"/>
-    <col min="15865" max="15865" width="21.85546875" style="1" hidden="1"/>
-    <col min="15866" max="15868" width="11.42578125" style="1" hidden="1"/>
+    <col min="15614" max="15614" width="20.44140625" style="1" hidden="1"/>
+    <col min="15615" max="15861" width="11.44140625" style="1" hidden="1"/>
+    <col min="15862" max="15862" width="15.44140625" style="1" hidden="1"/>
+    <col min="15863" max="15863" width="11.44140625" style="1" hidden="1"/>
+    <col min="15864" max="15864" width="15.6640625" style="1" hidden="1"/>
+    <col min="15865" max="15865" width="21.88671875" style="1" hidden="1"/>
+    <col min="15866" max="15868" width="11.44140625" style="1" hidden="1"/>
     <col min="15869" max="15869" width="16" style="1" hidden="1"/>
-    <col min="15870" max="15870" width="20.42578125" style="1" hidden="1"/>
-    <col min="15871" max="16117" width="11.42578125" style="1" hidden="1"/>
-    <col min="16118" max="16118" width="15.42578125" style="1" hidden="1"/>
-    <col min="16119" max="16119" width="11.42578125" style="1" hidden="1"/>
-    <col min="16120" max="16120" width="15.7109375" style="1" hidden="1"/>
-    <col min="16121" max="16121" width="21.85546875" style="1" hidden="1"/>
-    <col min="16122" max="16124" width="11.42578125" style="1" hidden="1"/>
+    <col min="15870" max="15870" width="20.44140625" style="1" hidden="1"/>
+    <col min="15871" max="16117" width="11.44140625" style="1" hidden="1"/>
+    <col min="16118" max="16118" width="15.44140625" style="1" hidden="1"/>
+    <col min="16119" max="16119" width="11.44140625" style="1" hidden="1"/>
+    <col min="16120" max="16120" width="15.6640625" style="1" hidden="1"/>
+    <col min="16121" max="16121" width="21.88671875" style="1" hidden="1"/>
+    <col min="16122" max="16124" width="11.44140625" style="1" hidden="1"/>
     <col min="16125" max="16125" width="16" style="1" hidden="1"/>
-    <col min="16126" max="16126" width="20.42578125" style="1" hidden="1"/>
-    <col min="16127" max="16129" width="11.42578125" style="1" hidden="1"/>
-    <col min="16130" max="16130" width="15.42578125" style="1" hidden="1"/>
-    <col min="16131" max="16131" width="11.42578125" style="1" hidden="1"/>
-    <col min="16132" max="16132" width="15.7109375" style="1" hidden="1"/>
-    <col min="16133" max="16133" width="21.85546875" style="1" hidden="1"/>
-    <col min="16134" max="16136" width="11.42578125" style="1" hidden="1"/>
+    <col min="16126" max="16126" width="20.44140625" style="1" hidden="1"/>
+    <col min="16127" max="16129" width="11.44140625" style="1" hidden="1"/>
+    <col min="16130" max="16130" width="15.44140625" style="1" hidden="1"/>
+    <col min="16131" max="16131" width="11.44140625" style="1" hidden="1"/>
+    <col min="16132" max="16132" width="15.6640625" style="1" hidden="1"/>
+    <col min="16133" max="16133" width="21.88671875" style="1" hidden="1"/>
+    <col min="16134" max="16136" width="11.44140625" style="1" hidden="1"/>
     <col min="16137" max="16137" width="16" style="1" hidden="1"/>
-    <col min="16138" max="16139" width="20.42578125" style="1" hidden="1"/>
-    <col min="16140" max="16141" width="11.42578125" style="1" hidden="1"/>
+    <col min="16138" max="16139" width="20.44140625" style="1" hidden="1"/>
+    <col min="16140" max="16141" width="11.44140625" style="1" hidden="1"/>
     <col min="16142" max="16142" width="16" style="1" hidden="1"/>
-    <col min="16143" max="16145" width="20.42578125" style="1" hidden="1"/>
-    <col min="16146" max="16384" width="11.42578125" style="1" hidden="1"/>
+    <col min="16143" max="16145" width="20.44140625" style="1" hidden="1"/>
+    <col min="16146" max="16384" width="11.44140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="str">
         <f>RAWDATA!B2</f>
         <v>applicant.last_name</v>
@@ -2619,7 +2620,7 @@
         <v>course.teacher_name</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <f>RAWDATA!B3</f>
         <v>0</v>
@@ -2688,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <f>RAWDATA!B4</f>
         <v>0</v>
@@ -2757,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <f>RAWDATA!B5</f>
         <v>0</v>
@@ -2826,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <f>RAWDATA!B6</f>
         <v>0</v>
@@ -2895,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <f>RAWDATA!B7</f>
         <v>0</v>
@@ -2964,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <f>RAWDATA!B8</f>
         <v>0</v>
@@ -3033,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <f>RAWDATA!B9</f>
         <v>0</v>
@@ -3102,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <f>RAWDATA!B10</f>
         <v>0</v>
@@ -3171,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <f>RAWDATA!B11</f>
         <v>0</v>
@@ -3240,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <f>RAWDATA!B12</f>
         <v>0</v>
@@ -3309,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <f>RAWDATA!B13</f>
         <v>0</v>
@@ -3378,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <f>RAWDATA!B14</f>
         <v>0</v>
@@ -3447,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <f>RAWDATA!B15</f>
         <v>0</v>
@@ -3516,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <f>RAWDATA!B16</f>
         <v>0</v>
@@ -3585,7 +3586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <f>RAWDATA!B17</f>
         <v>0</v>
@@ -3654,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <f>RAWDATA!B18</f>
         <v>0</v>
@@ -3723,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <f>RAWDATA!B19</f>
         <v>0</v>
@@ -3792,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <f>RAWDATA!B20</f>
         <v>0</v>
@@ -3861,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <f>RAWDATA!B21</f>
         <v>0</v>
@@ -3930,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <f>RAWDATA!B22</f>
         <v>0</v>
@@ -3999,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <f>RAWDATA!B23</f>
         <v>0</v>
@@ -4068,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <f>RAWDATA!B24</f>
         <v>0</v>
@@ -4137,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <f>RAWDATA!B25</f>
         <v>0</v>
@@ -4189,7 +4190,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="11"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <f>RAWDATA!B26</f>
         <v>0</v>
@@ -4241,7 +4242,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="11"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <f>RAWDATA!B27</f>
         <v>0</v>
@@ -4293,7 +4294,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="11"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <f>RAWDATA!B28</f>
         <v>0</v>
@@ -4345,7 +4346,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="11"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <f>RAWDATA!B29</f>
         <v>0</v>
@@ -4397,7 +4398,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="11"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <f>RAWDATA!B30</f>
         <v>0</v>
@@ -4449,7 +4450,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="11"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <f>RAWDATA!B31</f>
         <v>0</v>
@@ -4501,7 +4502,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="11"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <f>RAWDATA!B32</f>
         <v>0</v>
@@ -4553,7 +4554,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="11"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <f>RAWDATA!B33</f>
         <v>0</v>
@@ -4605,7 +4606,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="11"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
         <f>RAWDATA!B34</f>
         <v>0</v>
@@ -4657,7 +4658,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="11"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="29">
         <f>RAWDATA!B35</f>
         <v>0</v>
@@ -4726,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <f>RAWDATA!B36</f>
         <v>0</v>
@@ -4795,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>10</v>
@@ -4815,7 +4816,7 @@
       <c r="M37" s="4"/>
       <c r="N37" s="22"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -4832,7 +4833,7 @@
       <c r="M38" s="4"/>
       <c r="N38" s="22"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
@@ -4853,7 +4854,7 @@
       <c r="M39" s="4"/>
       <c r="N39" s="22"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
@@ -4869,7 +4870,7 @@
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
@@ -4891,7 +4892,7 @@
       <c r="M41" s="31"/>
       <c r="N41" s="22"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
@@ -4911,7 +4912,7 @@
       <c r="M42" s="31"/>
       <c r="N42" s="22"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -4931,7 +4932,7 @@
       <c r="M43" s="31"/>
       <c r="N43" s="22"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -4951,7 +4952,7 @@
       <c r="M44" s="31"/>
       <c r="N44" s="22"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -4971,7 +4972,7 @@
       <c r="M45" s="31"/>
       <c r="N45" s="22"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>51</v>
       </c>
@@ -4991,7 +4992,7 @@
       <c r="M46" s="31"/>
       <c r="N46" s="22"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
@@ -5011,7 +5012,7 @@
       <c r="M47" s="31"/>
       <c r="N47" s="22"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>44</v>
       </c>
@@ -5031,55 +5032,55 @@
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
     </row>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="53"/>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="53"/>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="53"/>
     </row>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="53"/>
     </row>
-    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="53"/>
     </row>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="53"/>
     </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="53"/>
     </row>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="53"/>
     </row>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="53"/>
     </row>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="53"/>
     </row>
-    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="53"/>
     </row>
-    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="53"/>
     </row>
-    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="53"/>
     </row>
-    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="53"/>
     </row>
-    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="53"/>
     </row>
-    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="53"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
   <dataConsolidate/>
@@ -5087,7 +5088,7 @@
     <mergeCell ref="D41:G48"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Inkorrekte Semesterangabe" error="Bitte wählen Sie aus der Dropdown-Liste aus._x000a__x000a_Ihre Eingabe wird nicht automatisch korrigiert." promptTitle="Semester" prompt="Bitte geben Sie das entsprechende Semester an. Wählen Sie aus der Dropdown-Liste." sqref="B47"/>
+    <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Inkorrekte Semesterangabe" error="Bitte wählen Sie aus der Dropdown-Liste aus._x000a__x000a_Ihre Eingabe wird nicht automatisch korrigiert." promptTitle="Semester" prompt="Bitte geben Sie das entsprechende Semester an. Wählen Sie aus der Dropdown-Liste." sqref="B47" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.2598425196850394" bottom="1.0629921259842521" header="0.59055118110236227" footer="0.78740157480314965"/>
   <pageSetup paperSize="9" scale="82" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5100,7 +5101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5110,15 +5111,15 @@
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="7" customWidth="1"/>
-    <col min="3" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" hidden="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="7" customWidth="1"/>
+    <col min="3" max="8" width="11.44140625" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="70" t="str">
         <f>Notenliste!B44</f>
         <v>course.name</v>
@@ -5132,7 +5133,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -5149,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1.3</v>
       </c>
@@ -5158,7 +5159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1.7</v>
       </c>
@@ -5167,7 +5168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -5176,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2.7</v>
       </c>
@@ -5194,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -5203,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>3.3</v>
       </c>
@@ -5212,7 +5213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>3.7</v>
       </c>
@@ -5221,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>4</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -5251,32 +5252,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView showZeros="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" style="20" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="14" width="8.7109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="1.7109375" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" hidden="1"/>
+    <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="8.6640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="1.6640625" customWidth="1"/>
+    <col min="17" max="16384" width="11.44140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="58" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="58" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>course.namecourse.alternative</v>
@@ -5296,7 +5297,7 @@
       <c r="N1" s="71"/>
       <c r="O1" s="71"/>
     </row>
-    <row r="2" spans="1:15" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
         <v>Dozent/in: course.teacher_name</v>
@@ -5319,7 +5320,7 @@
       <c r="N2" s="73"/>
       <c r="O2" s="73"/>
     </row>
-    <row r="3" spans="1:15" s="59" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="59" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -5366,7 +5367,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -5427,7 +5428,7 @@
         <v>ATTENDANCE.TS_RECEIVED_STR</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>2</v>
       </c>
@@ -5452,7 +5453,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="18">
-        <f>RAWDATA!L3</f>
+        <f>RAWDATA!I3</f>
         <v>0</v>
       </c>
       <c r="H5" s="19" t="str">
@@ -5488,7 +5489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>3</v>
       </c>
@@ -5513,7 +5514,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="18">
-        <f>RAWDATA!L4</f>
+        <f>RAWDATA!I4</f>
         <v>0</v>
       </c>
       <c r="H6" s="19" t="str">
@@ -5549,7 +5550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>4</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="18">
-        <f>RAWDATA!L5</f>
+        <f>RAWDATA!I5</f>
         <v>0</v>
       </c>
       <c r="H7" s="19" t="str">
@@ -5610,7 +5611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>5</v>
       </c>
@@ -5635,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="18">
-        <f>RAWDATA!L6</f>
+        <f>RAWDATA!I6</f>
         <v>0</v>
       </c>
       <c r="H8" s="19" t="str">
@@ -5671,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>6</v>
       </c>
@@ -5696,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="18">
-        <f>RAWDATA!L7</f>
+        <f>RAWDATA!I7</f>
         <v>0</v>
       </c>
       <c r="H9" s="19" t="str">
@@ -5732,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>7</v>
       </c>
@@ -5757,7 +5758,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="18">
-        <f>RAWDATA!L8</f>
+        <f>RAWDATA!I8</f>
         <v>0</v>
       </c>
       <c r="H10" s="19" t="str">
@@ -5793,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>8</v>
       </c>
@@ -5818,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="18">
-        <f>RAWDATA!L9</f>
+        <f>RAWDATA!I9</f>
         <v>0</v>
       </c>
       <c r="H11" s="19" t="str">
@@ -5854,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>9</v>
       </c>
@@ -5879,7 +5880,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="18">
-        <f>RAWDATA!L10</f>
+        <f>RAWDATA!I10</f>
         <v>0</v>
       </c>
       <c r="H12" s="19" t="str">
@@ -5915,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>10</v>
       </c>
@@ -5940,7 +5941,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="18">
-        <f>RAWDATA!L11</f>
+        <f>RAWDATA!I11</f>
         <v>0</v>
       </c>
       <c r="H13" s="19" t="str">
@@ -5976,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>11</v>
       </c>
@@ -6001,7 +6002,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="18">
-        <f>RAWDATA!L12</f>
+        <f>RAWDATA!I12</f>
         <v>0</v>
       </c>
       <c r="H14" s="19" t="str">
@@ -6037,7 +6038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>12</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="18">
-        <f>RAWDATA!L13</f>
+        <f>RAWDATA!I13</f>
         <v>0</v>
       </c>
       <c r="H15" s="19" t="str">
@@ -6098,7 +6099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>13</v>
       </c>
@@ -6123,7 +6124,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="18">
-        <f>RAWDATA!L14</f>
+        <f>RAWDATA!I14</f>
         <v>0</v>
       </c>
       <c r="H16" s="19" t="str">
@@ -6159,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>14</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="18">
-        <f>RAWDATA!L15</f>
+        <f>RAWDATA!I15</f>
         <v>0</v>
       </c>
       <c r="H17" s="19" t="str">
@@ -6220,7 +6221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>15</v>
       </c>
@@ -6245,7 +6246,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="18">
-        <f>RAWDATA!L16</f>
+        <f>RAWDATA!I16</f>
         <v>0</v>
       </c>
       <c r="H18" s="19" t="str">
@@ -6281,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>16</v>
       </c>
@@ -6306,7 +6307,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="18">
-        <f>RAWDATA!L17</f>
+        <f>RAWDATA!I17</f>
         <v>0</v>
       </c>
       <c r="H19" s="19" t="str">
@@ -6342,7 +6343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>17</v>
       </c>
@@ -6367,7 +6368,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="18">
-        <f>RAWDATA!L18</f>
+        <f>RAWDATA!I18</f>
         <v>0</v>
       </c>
       <c r="H20" s="19" t="str">
@@ -6403,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>18</v>
       </c>
@@ -6428,7 +6429,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="18">
-        <f>RAWDATA!L19</f>
+        <f>RAWDATA!I19</f>
         <v>0</v>
       </c>
       <c r="H21" s="19" t="str">
@@ -6464,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>19</v>
       </c>
@@ -6489,7 +6490,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="18">
-        <f>RAWDATA!L20</f>
+        <f>RAWDATA!I20</f>
         <v>0</v>
       </c>
       <c r="H22" s="19" t="str">
@@ -6525,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>20</v>
       </c>
@@ -6550,7 +6551,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="18">
-        <f>RAWDATA!L21</f>
+        <f>RAWDATA!I21</f>
         <v>0</v>
       </c>
       <c r="H23" s="19" t="str">
@@ -6586,7 +6587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>21</v>
       </c>
@@ -6611,7 +6612,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="18">
-        <f>RAWDATA!L22</f>
+        <f>RAWDATA!I22</f>
         <v>0</v>
       </c>
       <c r="H24" s="19" t="str">
@@ -6647,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>22</v>
       </c>
@@ -6672,7 +6673,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="18">
-        <f>RAWDATA!L23</f>
+        <f>RAWDATA!I23</f>
         <v>0</v>
       </c>
       <c r="H25" s="19" t="str">
@@ -6708,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>23</v>
       </c>
@@ -6733,7 +6734,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="18">
-        <f>RAWDATA!L24</f>
+        <f>RAWDATA!I24</f>
         <v>0</v>
       </c>
       <c r="H26" s="19" t="str">
@@ -6769,7 +6770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>24</v>
       </c>
@@ -6794,7 +6795,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="18">
-        <f>RAWDATA!L25</f>
+        <f>RAWDATA!I25</f>
         <v>0</v>
       </c>
       <c r="H27" s="19">
@@ -6830,7 +6831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>25</v>
       </c>
@@ -6855,7 +6856,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="18">
-        <f>RAWDATA!L26</f>
+        <f>RAWDATA!I26</f>
         <v>0</v>
       </c>
       <c r="H28" s="19">
@@ -6891,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>26</v>
       </c>
@@ -6916,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="18">
-        <f>RAWDATA!L27</f>
+        <f>RAWDATA!I27</f>
         <v>0</v>
       </c>
       <c r="H29" s="19">
@@ -6952,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>27</v>
       </c>
@@ -6977,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="18">
-        <f>RAWDATA!L28</f>
+        <f>RAWDATA!I28</f>
         <v>0</v>
       </c>
       <c r="H30" s="19">
@@ -7013,7 +7014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>28</v>
       </c>
@@ -7038,7 +7039,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="18">
-        <f>RAWDATA!L29</f>
+        <f>RAWDATA!I29</f>
         <v>0</v>
       </c>
       <c r="H31" s="19">
@@ -7074,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
         <v>29</v>
       </c>
@@ -7099,7 +7100,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="18">
-        <f>RAWDATA!L30</f>
+        <f>RAWDATA!I30</f>
         <v>0</v>
       </c>
       <c r="H32" s="19">
@@ -7135,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17">
         <v>30</v>
       </c>
@@ -7160,7 +7161,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="18">
-        <f>RAWDATA!L31</f>
+        <f>RAWDATA!I31</f>
         <v>0</v>
       </c>
       <c r="H33" s="19">
@@ -7196,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17">
         <v>31</v>
       </c>
@@ -7221,7 +7222,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="18">
-        <f>RAWDATA!L32</f>
+        <f>RAWDATA!I32</f>
         <v>0</v>
       </c>
       <c r="H34" s="19">
@@ -7257,7 +7258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
         <v>32</v>
       </c>
@@ -7282,7 +7283,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="18">
-        <f>RAWDATA!L33</f>
+        <f>RAWDATA!I33</f>
         <v>0</v>
       </c>
       <c r="H35" s="19">
@@ -7318,7 +7319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>33</v>
       </c>
@@ -7343,7 +7344,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="18">
-        <f>RAWDATA!L34</f>
+        <f>RAWDATA!I34</f>
         <v>0</v>
       </c>
       <c r="H36" s="19">
@@ -7379,7 +7380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>34</v>
       </c>
@@ -7404,7 +7405,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="18">
-        <f>RAWDATA!L35</f>
+        <f>RAWDATA!I35</f>
         <v>0</v>
       </c>
       <c r="H37" s="19">
@@ -7440,7 +7441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
         <v>35</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="18">
-        <f>RAWDATA!L36</f>
+        <f>RAWDATA!I36</f>
         <v>0</v>
       </c>
       <c r="H38" s="19">
@@ -7501,7 +7502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="55"/>
       <c r="B39" s="56"/>
       <c r="C39" s="56"/>
@@ -7524,7 +7525,7 @@
       <c r="N39" s="55"/>
       <c r="O39" s="57"/>
     </row>
-    <row r="40" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="74" t="s">
         <v>42</v>
       </c>
@@ -7543,7 +7544,7 @@
       <c r="N40" s="74"/>
       <c r="O40" s="74"/>
     </row>
-    <row r="41" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="74"/>
       <c r="B41" s="74"/>
       <c r="C41" s="74"/>
@@ -7560,7 +7561,7 @@
       <c r="N41" s="74"/>
       <c r="O41" s="74"/>
     </row>
-    <row r="42" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="74"/>
       <c r="B42" s="74"/>
       <c r="C42" s="74"/>
@@ -7577,7 +7578,7 @@
       <c r="N42" s="74"/>
       <c r="O42" s="74"/>
     </row>
-    <row r="43" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="74"/>
       <c r="B43" s="74"/>
       <c r="C43" s="74"/>
@@ -7594,7 +7595,7 @@
       <c r="N43" s="74"/>
       <c r="O43" s="74"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="74"/>
       <c r="B44" s="74"/>
       <c r="C44" s="74"/>
@@ -7631,7 +7632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7641,24 +7642,24 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="20" customWidth="1"/>
-    <col min="6" max="6" width="0.85546875" style="20" customWidth="1"/>
-    <col min="7" max="20" width="7.7109375" style="20" customWidth="1"/>
-    <col min="21" max="21" width="0.85546875" style="20" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="51" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" style="52" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="0.88671875" style="20" customWidth="1"/>
+    <col min="7" max="20" width="7.6640625" style="20" customWidth="1"/>
+    <col min="21" max="21" width="0.88671875" style="20" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="51" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" style="52" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" style="39" customWidth="1"/>
     <col min="25" max="31" width="0" hidden="1" customWidth="1"/>
-    <col min="32" max="16384" width="11.42578125" hidden="1"/>
+    <col min="32" max="16384" width="11.44140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>course.namecourse.alternative</v>
@@ -7687,7 +7688,7 @@
       <c r="W1" s="77"/>
       <c r="X1" s="77"/>
     </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>40</v>
       </c>
@@ -7715,7 +7716,7 @@
       <c r="W2" s="77"/>
       <c r="X2" s="77"/>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="78" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
         <v>Dozent/in: course.teacher_name</v>
@@ -7744,7 +7745,7 @@
       <c r="W3" s="79"/>
       <c r="X3" s="79"/>
     </row>
-    <row r="4" spans="1:24" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80" t="s">
         <v>26</v>
       </c>
@@ -7786,7 +7787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="81"/>
       <c r="B5" s="81"/>
       <c r="C5" s="81"/>
@@ -7840,7 +7841,7 @@
       <c r="W5" s="76"/>
       <c r="X5" s="76"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -7880,7 +7881,7 @@
       <c r="W6" s="50"/>
       <c r="X6" s="50"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>2</v>
       </c>
@@ -7920,7 +7921,7 @@
       <c r="W7" s="50"/>
       <c r="X7" s="50"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>3</v>
       </c>
@@ -7960,7 +7961,7 @@
       <c r="W8" s="50"/>
       <c r="X8" s="50"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>4</v>
       </c>
@@ -8000,7 +8001,7 @@
       <c r="W9" s="50"/>
       <c r="X9" s="50"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>5</v>
       </c>
@@ -8040,7 +8041,7 @@
       <c r="W10" s="50"/>
       <c r="X10" s="50"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>6</v>
       </c>
@@ -8080,7 +8081,7 @@
       <c r="W11" s="50"/>
       <c r="X11" s="50"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>7</v>
       </c>
@@ -8120,7 +8121,7 @@
       <c r="W12" s="50"/>
       <c r="X12" s="50"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>8</v>
       </c>
@@ -8160,7 +8161,7 @@
       <c r="W13" s="50"/>
       <c r="X13" s="50"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>9</v>
       </c>
@@ -8200,7 +8201,7 @@
       <c r="W14" s="50"/>
       <c r="X14" s="50"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>10</v>
       </c>
@@ -8240,7 +8241,7 @@
       <c r="W15" s="50"/>
       <c r="X15" s="50"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>11</v>
       </c>
@@ -8280,7 +8281,7 @@
       <c r="W16" s="50"/>
       <c r="X16" s="50"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>12</v>
       </c>
@@ -8320,7 +8321,7 @@
       <c r="W17" s="50"/>
       <c r="X17" s="50"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>13</v>
       </c>
@@ -8360,7 +8361,7 @@
       <c r="W18" s="50"/>
       <c r="X18" s="50"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>14</v>
       </c>
@@ -8400,7 +8401,7 @@
       <c r="W19" s="50"/>
       <c r="X19" s="50"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>15</v>
       </c>
@@ -8440,7 +8441,7 @@
       <c r="W20" s="50"/>
       <c r="X20" s="50"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>16</v>
       </c>
@@ -8480,7 +8481,7 @@
       <c r="W21" s="50"/>
       <c r="X21" s="50"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>17</v>
       </c>
@@ -8520,7 +8521,7 @@
       <c r="W22" s="50"/>
       <c r="X22" s="50"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>18</v>
       </c>
@@ -8560,7 +8561,7 @@
       <c r="W23" s="50"/>
       <c r="X23" s="50"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>19</v>
       </c>
@@ -8600,7 +8601,7 @@
       <c r="W24" s="50"/>
       <c r="X24" s="50"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>20</v>
       </c>
@@ -8640,7 +8641,7 @@
       <c r="W25" s="50"/>
       <c r="X25" s="50"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>21</v>
       </c>
@@ -8680,7 +8681,7 @@
       <c r="W26" s="50"/>
       <c r="X26" s="50"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>22</v>
       </c>
@@ -8720,7 +8721,7 @@
       <c r="W27" s="50"/>
       <c r="X27" s="50"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>23</v>
       </c>
@@ -8760,7 +8761,7 @@
       <c r="W28" s="50"/>
       <c r="X28" s="50"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>24</v>
       </c>
@@ -8800,7 +8801,7 @@
       <c r="W29" s="50"/>
       <c r="X29" s="50"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>25</v>
       </c>
@@ -8840,7 +8841,7 @@
       <c r="W30" s="50"/>
       <c r="X30" s="50"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>26</v>
       </c>
@@ -8880,7 +8881,7 @@
       <c r="W31" s="50"/>
       <c r="X31" s="50"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
         <v>27</v>
       </c>
@@ -8920,7 +8921,7 @@
       <c r="W32" s="50"/>
       <c r="X32" s="50"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="17">
         <v>28</v>
       </c>
@@ -8960,7 +8961,7 @@
       <c r="W33" s="50"/>
       <c r="X33" s="50"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="17">
         <v>29</v>
       </c>
@@ -9000,7 +9001,7 @@
       <c r="W34" s="50"/>
       <c r="X34" s="50"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
         <v>30</v>
       </c>
@@ -9040,7 +9041,7 @@
       <c r="W35" s="50"/>
       <c r="X35" s="50"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>31</v>
       </c>
@@ -9080,7 +9081,7 @@
       <c r="W36" s="50"/>
       <c r="X36" s="50"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>32</v>
       </c>
@@ -9120,7 +9121,7 @@
       <c r="W37" s="50"/>
       <c r="X37" s="50"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
         <v>33</v>
       </c>
@@ -9160,7 +9161,7 @@
       <c r="W38" s="50"/>
       <c r="X38" s="50"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
         <v>34</v>
       </c>
@@ -9200,7 +9201,7 @@
       <c r="W39" s="50"/>
       <c r="X39" s="50"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="17">
         <v>35</v>
       </c>
@@ -9267,25 +9268,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="61" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="64" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="63" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="64" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="63" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
         <v>27</v>
       </c>
@@ -9311,7 +9312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="str">
         <f>IF(Notenliste!D2=0," ",Notenliste!D2)</f>
         <v>applicant.tag</v>
@@ -9333,7 +9334,7 @@
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="str">
         <f>IF(Notenliste!D3=0," ",Notenliste!D3)</f>
         <v xml:space="preserve"> </v>
@@ -9355,7 +9356,7 @@
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="str">
         <f>IF(Notenliste!D4=0," ",Notenliste!D4)</f>
         <v xml:space="preserve"> </v>
@@ -9377,7 +9378,7 @@
       <c r="G4" s="39"/>
       <c r="H4" s="39"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="40" t="str">
         <f>IF(Notenliste!D5=0," ",Notenliste!D5)</f>
         <v xml:space="preserve"> </v>
@@ -9399,7 +9400,7 @@
       <c r="G5" s="39"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="str">
         <f>IF(Notenliste!D6=0," ",Notenliste!D6)</f>
         <v xml:space="preserve"> </v>
@@ -9421,7 +9422,7 @@
       <c r="G6" s="39"/>
       <c r="H6" s="39"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="40" t="str">
         <f>IF(Notenliste!D7=0," ",Notenliste!D7)</f>
         <v xml:space="preserve"> </v>
@@ -9443,7 +9444,7 @@
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="40" t="str">
         <f>IF(Notenliste!D8=0," ",Notenliste!D8)</f>
         <v xml:space="preserve"> </v>
@@ -9465,7 +9466,7 @@
       <c r="G8" s="39"/>
       <c r="H8" s="39"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="str">
         <f>IF(Notenliste!D9=0," ",Notenliste!D9)</f>
         <v xml:space="preserve"> </v>
@@ -9487,7 +9488,7 @@
       <c r="G9" s="39"/>
       <c r="H9" s="39"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="str">
         <f>IF(Notenliste!D10=0," ",Notenliste!D10)</f>
         <v xml:space="preserve"> </v>
@@ -9509,7 +9510,7 @@
       <c r="G10" s="39"/>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="str">
         <f>IF(Notenliste!D11=0," ",Notenliste!D11)</f>
         <v xml:space="preserve"> </v>
@@ -9531,7 +9532,7 @@
       <c r="G11" s="39"/>
       <c r="H11" s="39"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="str">
         <f>IF(Notenliste!D12=0," ",Notenliste!D12)</f>
         <v xml:space="preserve"> </v>
@@ -9553,7 +9554,7 @@
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="40" t="str">
         <f>IF(Notenliste!D13=0," ",Notenliste!D13)</f>
         <v xml:space="preserve"> </v>
@@ -9575,7 +9576,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="40" t="str">
         <f>IF(Notenliste!D14=0," ",Notenliste!D14)</f>
         <v xml:space="preserve"> </v>
@@ -9597,7 +9598,7 @@
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="str">
         <f>IF(Notenliste!D15=0," ",Notenliste!D15)</f>
         <v xml:space="preserve"> </v>
@@ -9619,7 +9620,7 @@
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="str">
         <f>IF(Notenliste!D16=0," ",Notenliste!D16)</f>
         <v xml:space="preserve"> </v>
@@ -9641,7 +9642,7 @@
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="str">
         <f>IF(Notenliste!D17=0," ",Notenliste!D17)</f>
         <v xml:space="preserve"> </v>
@@ -9663,7 +9664,7 @@
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="str">
         <f>IF(Notenliste!D18=0," ",Notenliste!D18)</f>
         <v xml:space="preserve"> </v>
@@ -9685,7 +9686,7 @@
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="str">
         <f>IF(Notenliste!D19=0," ",Notenliste!D19)</f>
         <v xml:space="preserve"> </v>
@@ -9707,7 +9708,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="40" t="str">
         <f>IF(Notenliste!D20=0," ",Notenliste!D20)</f>
         <v xml:space="preserve"> </v>
@@ -9729,7 +9730,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="40" t="str">
         <f>IF(Notenliste!D21=0," ",Notenliste!D21)</f>
         <v xml:space="preserve"> </v>
@@ -9751,7 +9752,7 @@
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="40" t="str">
         <f>IF(Notenliste!D22=0," ",Notenliste!D22)</f>
         <v xml:space="preserve"> </v>
@@ -9773,7 +9774,7 @@
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="40" t="str">
         <f>IF(Notenliste!D23=0," ",Notenliste!D23)</f>
         <v xml:space="preserve"> </v>
@@ -9795,7 +9796,7 @@
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="40" t="str">
         <f>IF(Notenliste!D24=0," ",Notenliste!D24)</f>
         <v xml:space="preserve"> </v>
@@ -9817,7 +9818,7 @@
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="40" t="str">
         <f>IF(Notenliste!D25=0," ",Notenliste!D25)</f>
         <v xml:space="preserve"> </v>
@@ -9839,7 +9840,7 @@
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="40" t="str">
         <f>IF(Notenliste!D26=0," ",Notenliste!D26)</f>
         <v xml:space="preserve"> </v>
@@ -9861,7 +9862,7 @@
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="40" t="str">
         <f>IF(Notenliste!D27=0," ",Notenliste!D27)</f>
         <v xml:space="preserve"> </v>
@@ -9883,7 +9884,7 @@
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="40" t="str">
         <f>IF(Notenliste!D28=0," ",Notenliste!D28)</f>
         <v xml:space="preserve"> </v>
@@ -9905,7 +9906,7 @@
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="40" t="str">
         <f>IF(Notenliste!D29=0," ",Notenliste!D29)</f>
         <v xml:space="preserve"> </v>
@@ -9927,7 +9928,7 @@
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="40" t="str">
         <f>IF(Notenliste!D30=0," ",Notenliste!D30)</f>
         <v xml:space="preserve"> </v>
@@ -9949,7 +9950,7 @@
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="str">
         <f>IF(Notenliste!D31=0," ",Notenliste!D31)</f>
         <v xml:space="preserve"> </v>
@@ -9971,7 +9972,7 @@
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="str">
         <f>IF(Notenliste!D32=0," ",Notenliste!D32)</f>
         <v xml:space="preserve"> </v>
@@ -9993,7 +9994,7 @@
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="str">
         <f>IF(Notenliste!D33=0," ",Notenliste!D33)</f>
         <v xml:space="preserve"> </v>
@@ -10015,7 +10016,7 @@
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="str">
         <f>IF(Notenliste!D34=0," ",Notenliste!D34)</f>
         <v xml:space="preserve"> </v>
@@ -10037,7 +10038,7 @@
       <c r="G34" s="39"/>
       <c r="H34" s="39"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="str">
         <f>IF(Notenliste!D35=0," ",Notenliste!D35)</f>
         <v xml:space="preserve"> </v>
@@ -10059,7 +10060,7 @@
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="str">
         <f>IF(Notenliste!D36=0," ",Notenliste!D36)</f>
         <v xml:space="preserve"> </v>
@@ -10084,21 +10085,21 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>Anmeldestatus</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>Notenskala</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C37:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C37:C1048576" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>0</formula1>
       <formula2>120</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E37:E1048576">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E37:E1048576" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>41275</formula1>
       <formula2>73050</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A37:A1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A37:A1048576" xr:uid="{00000000-0002-0000-0500-000004000000}">
       <formula1>0</formula1>
       <formula2>99999999</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
update rounding in excel templates
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\04_Hiwi\Datenbank\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s_hiwi\Documents\Datenbank\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE68B1A-E018-44D6-A0A0-7EC7505C1079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <definedName name="kursname">Notenliste!$A$52:$A$60</definedName>
     <definedName name="semester">Notenliste!$D$52:$D$62</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -340,7 +339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -834,8 +833,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -945,7 +944,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -973,6 +972,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1195,54 +1195,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DATA" displayName="DATA" ref="B1:L2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B1:L2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DATA" displayName="DATA" ref="B1:L2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B1:L2"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vorname" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hochschule" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Matrikelnummer" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Note" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="LP" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E-Mail" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Telefon" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="bestanden" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Teilnahmeschein" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Schein erhalten" dataDxfId="11"/>
+    <tableColumn id="1" name="Nachname" dataDxfId="21"/>
+    <tableColumn id="2" name="Vorname" dataDxfId="20"/>
+    <tableColumn id="3" name="Hochschule" dataDxfId="19"/>
+    <tableColumn id="4" name="Matrikelnummer" dataDxfId="18"/>
+    <tableColumn id="8" name="Note" dataDxfId="17"/>
+    <tableColumn id="7" name="LP" dataDxfId="16"/>
+    <tableColumn id="5" name="E-Mail" dataDxfId="15"/>
+    <tableColumn id="9" name="Telefon" dataDxfId="14"/>
+    <tableColumn id="11" name="bestanden" dataDxfId="13"/>
+    <tableColumn id="10" name="Teilnahmeschein" dataDxfId="12"/>
+    <tableColumn id="6" name="Schein erhalten" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="10">
-  <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="A1:H36"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Matrikelnummer" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="1" name="Matrikelnummer" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>IF(Notenliste!D2=0," ",Notenliste!D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Status" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="LP" dataDxfId="6">
+    <tableColumn id="2" name="Status" dataDxfId="7"/>
+    <tableColumn id="3" name="LP" dataDxfId="6">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,IF(Notenliste!I2&lt;&gt;0,Notenliste!I2,Notenliste!$B$33)," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Note" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="4" name="Note" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(Notenliste!D2=0," ",IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Datum" dataDxfId="3">
+    <tableColumn id="5" name="Datum" dataDxfId="3">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$48," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Individueller Titel deutsch" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Individueller Titel englisch" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Anmerkungen" dataDxfId="0"/>
+    <tableColumn id="6" name="Individueller Titel deutsch" dataDxfId="2"/>
+    <tableColumn id="7" name="Individueller Titel englisch" dataDxfId="1"/>
+    <tableColumn id="8" name="Anmerkungen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1280,9 +1280,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1317,7 +1317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1352,7 +1352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1525,32 +1525,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" style="39" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="40" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="40" customWidth="1"/>
     <col min="6" max="7" width="9" style="40" customWidth="1"/>
-    <col min="8" max="8" width="31.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.88671875" style="39" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="39" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" style="39" customWidth="1"/>
-    <col min="12" max="12" width="22.44140625" style="39" customWidth="1"/>
-    <col min="13" max="13" width="45.109375" style="39" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="39" hidden="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.44140625" hidden="1"/>
+    <col min="8" max="8" width="31.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" style="39" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="39" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="39" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="39" customWidth="1"/>
+    <col min="13" max="13" width="45.140625" style="39" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="39" hidden="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1877,62 +1877,62 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1948,557 +1948,557 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:WVY71"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.44140625" style="1" hidden="1"/>
-    <col min="16" max="16" width="5.109375" style="1" hidden="1"/>
-    <col min="17" max="17" width="6.88671875" style="2" hidden="1"/>
-    <col min="18" max="18" width="17.6640625" style="1" hidden="1"/>
+    <col min="15" max="15" width="6.42578125" style="1" hidden="1"/>
+    <col min="16" max="16" width="5.140625" style="1" hidden="1"/>
+    <col min="17" max="17" width="6.85546875" style="2" hidden="1"/>
+    <col min="18" max="18" width="17.7109375" style="1" hidden="1"/>
     <col min="19" max="19" width="16" style="1" hidden="1"/>
-    <col min="20" max="20" width="17.6640625" style="1" hidden="1"/>
-    <col min="21" max="245" width="11.44140625" style="1" hidden="1"/>
-    <col min="246" max="246" width="15.44140625" style="1" hidden="1"/>
-    <col min="247" max="247" width="11.44140625" style="1" hidden="1"/>
-    <col min="248" max="248" width="15.6640625" style="1" hidden="1"/>
-    <col min="249" max="249" width="21.88671875" style="1" hidden="1"/>
-    <col min="250" max="252" width="11.44140625" style="1" hidden="1"/>
+    <col min="20" max="20" width="17.7109375" style="1" hidden="1"/>
+    <col min="21" max="245" width="11.42578125" style="1" hidden="1"/>
+    <col min="246" max="246" width="15.42578125" style="1" hidden="1"/>
+    <col min="247" max="247" width="11.42578125" style="1" hidden="1"/>
+    <col min="248" max="248" width="15.7109375" style="1" hidden="1"/>
+    <col min="249" max="249" width="21.85546875" style="1" hidden="1"/>
+    <col min="250" max="252" width="11.42578125" style="1" hidden="1"/>
     <col min="253" max="253" width="16" style="1" hidden="1"/>
-    <col min="254" max="254" width="20.44140625" style="1" hidden="1"/>
-    <col min="255" max="501" width="11.44140625" style="1" hidden="1"/>
-    <col min="502" max="502" width="15.44140625" style="1" hidden="1"/>
-    <col min="503" max="503" width="11.44140625" style="1" hidden="1"/>
-    <col min="504" max="504" width="15.6640625" style="1" hidden="1"/>
-    <col min="505" max="505" width="21.88671875" style="1" hidden="1"/>
-    <col min="506" max="508" width="11.44140625" style="1" hidden="1"/>
+    <col min="254" max="254" width="20.42578125" style="1" hidden="1"/>
+    <col min="255" max="501" width="11.42578125" style="1" hidden="1"/>
+    <col min="502" max="502" width="15.42578125" style="1" hidden="1"/>
+    <col min="503" max="503" width="11.42578125" style="1" hidden="1"/>
+    <col min="504" max="504" width="15.7109375" style="1" hidden="1"/>
+    <col min="505" max="505" width="21.85546875" style="1" hidden="1"/>
+    <col min="506" max="508" width="11.42578125" style="1" hidden="1"/>
     <col min="509" max="509" width="16" style="1" hidden="1"/>
-    <col min="510" max="510" width="20.44140625" style="1" hidden="1"/>
-    <col min="511" max="757" width="11.44140625" style="1" hidden="1"/>
-    <col min="758" max="758" width="15.44140625" style="1" hidden="1"/>
-    <col min="759" max="759" width="11.44140625" style="1" hidden="1"/>
-    <col min="760" max="760" width="15.6640625" style="1" hidden="1"/>
-    <col min="761" max="761" width="21.88671875" style="1" hidden="1"/>
-    <col min="762" max="764" width="11.44140625" style="1" hidden="1"/>
+    <col min="510" max="510" width="20.42578125" style="1" hidden="1"/>
+    <col min="511" max="757" width="11.42578125" style="1" hidden="1"/>
+    <col min="758" max="758" width="15.42578125" style="1" hidden="1"/>
+    <col min="759" max="759" width="11.42578125" style="1" hidden="1"/>
+    <col min="760" max="760" width="15.7109375" style="1" hidden="1"/>
+    <col min="761" max="761" width="21.85546875" style="1" hidden="1"/>
+    <col min="762" max="764" width="11.42578125" style="1" hidden="1"/>
     <col min="765" max="765" width="16" style="1" hidden="1"/>
-    <col min="766" max="766" width="20.44140625" style="1" hidden="1"/>
-    <col min="767" max="1013" width="11.44140625" style="1" hidden="1"/>
-    <col min="1014" max="1014" width="15.44140625" style="1" hidden="1"/>
-    <col min="1015" max="1015" width="11.44140625" style="1" hidden="1"/>
-    <col min="1016" max="1016" width="15.6640625" style="1" hidden="1"/>
-    <col min="1017" max="1017" width="21.88671875" style="1" hidden="1"/>
-    <col min="1018" max="1020" width="11.44140625" style="1" hidden="1"/>
+    <col min="766" max="766" width="20.42578125" style="1" hidden="1"/>
+    <col min="767" max="1013" width="11.42578125" style="1" hidden="1"/>
+    <col min="1014" max="1014" width="15.42578125" style="1" hidden="1"/>
+    <col min="1015" max="1015" width="11.42578125" style="1" hidden="1"/>
+    <col min="1016" max="1016" width="15.7109375" style="1" hidden="1"/>
+    <col min="1017" max="1017" width="21.85546875" style="1" hidden="1"/>
+    <col min="1018" max="1020" width="11.42578125" style="1" hidden="1"/>
     <col min="1021" max="1021" width="16" style="1" hidden="1"/>
-    <col min="1022" max="1022" width="20.44140625" style="1" hidden="1"/>
-    <col min="1023" max="1269" width="11.44140625" style="1" hidden="1"/>
-    <col min="1270" max="1270" width="15.44140625" style="1" hidden="1"/>
-    <col min="1271" max="1271" width="11.44140625" style="1" hidden="1"/>
-    <col min="1272" max="1272" width="15.6640625" style="1" hidden="1"/>
-    <col min="1273" max="1273" width="21.88671875" style="1" hidden="1"/>
-    <col min="1274" max="1276" width="11.44140625" style="1" hidden="1"/>
+    <col min="1022" max="1022" width="20.42578125" style="1" hidden="1"/>
+    <col min="1023" max="1269" width="11.42578125" style="1" hidden="1"/>
+    <col min="1270" max="1270" width="15.42578125" style="1" hidden="1"/>
+    <col min="1271" max="1271" width="11.42578125" style="1" hidden="1"/>
+    <col min="1272" max="1272" width="15.7109375" style="1" hidden="1"/>
+    <col min="1273" max="1273" width="21.85546875" style="1" hidden="1"/>
+    <col min="1274" max="1276" width="11.42578125" style="1" hidden="1"/>
     <col min="1277" max="1277" width="16" style="1" hidden="1"/>
-    <col min="1278" max="1278" width="20.44140625" style="1" hidden="1"/>
-    <col min="1279" max="1525" width="11.44140625" style="1" hidden="1"/>
-    <col min="1526" max="1526" width="15.44140625" style="1" hidden="1"/>
-    <col min="1527" max="1527" width="11.44140625" style="1" hidden="1"/>
-    <col min="1528" max="1528" width="15.6640625" style="1" hidden="1"/>
-    <col min="1529" max="1529" width="21.88671875" style="1" hidden="1"/>
-    <col min="1530" max="1532" width="11.44140625" style="1" hidden="1"/>
+    <col min="1278" max="1278" width="20.42578125" style="1" hidden="1"/>
+    <col min="1279" max="1525" width="11.42578125" style="1" hidden="1"/>
+    <col min="1526" max="1526" width="15.42578125" style="1" hidden="1"/>
+    <col min="1527" max="1527" width="11.42578125" style="1" hidden="1"/>
+    <col min="1528" max="1528" width="15.7109375" style="1" hidden="1"/>
+    <col min="1529" max="1529" width="21.85546875" style="1" hidden="1"/>
+    <col min="1530" max="1532" width="11.42578125" style="1" hidden="1"/>
     <col min="1533" max="1533" width="16" style="1" hidden="1"/>
-    <col min="1534" max="1534" width="20.44140625" style="1" hidden="1"/>
-    <col min="1535" max="1781" width="11.44140625" style="1" hidden="1"/>
-    <col min="1782" max="1782" width="15.44140625" style="1" hidden="1"/>
-    <col min="1783" max="1783" width="11.44140625" style="1" hidden="1"/>
-    <col min="1784" max="1784" width="15.6640625" style="1" hidden="1"/>
-    <col min="1785" max="1785" width="21.88671875" style="1" hidden="1"/>
-    <col min="1786" max="1788" width="11.44140625" style="1" hidden="1"/>
+    <col min="1534" max="1534" width="20.42578125" style="1" hidden="1"/>
+    <col min="1535" max="1781" width="11.42578125" style="1" hidden="1"/>
+    <col min="1782" max="1782" width="15.42578125" style="1" hidden="1"/>
+    <col min="1783" max="1783" width="11.42578125" style="1" hidden="1"/>
+    <col min="1784" max="1784" width="15.7109375" style="1" hidden="1"/>
+    <col min="1785" max="1785" width="21.85546875" style="1" hidden="1"/>
+    <col min="1786" max="1788" width="11.42578125" style="1" hidden="1"/>
     <col min="1789" max="1789" width="16" style="1" hidden="1"/>
-    <col min="1790" max="1790" width="20.44140625" style="1" hidden="1"/>
-    <col min="1791" max="2037" width="11.44140625" style="1" hidden="1"/>
-    <col min="2038" max="2038" width="15.44140625" style="1" hidden="1"/>
-    <col min="2039" max="2039" width="11.44140625" style="1" hidden="1"/>
-    <col min="2040" max="2040" width="15.6640625" style="1" hidden="1"/>
-    <col min="2041" max="2041" width="21.88671875" style="1" hidden="1"/>
-    <col min="2042" max="2044" width="11.44140625" style="1" hidden="1"/>
+    <col min="1790" max="1790" width="20.42578125" style="1" hidden="1"/>
+    <col min="1791" max="2037" width="11.42578125" style="1" hidden="1"/>
+    <col min="2038" max="2038" width="15.42578125" style="1" hidden="1"/>
+    <col min="2039" max="2039" width="11.42578125" style="1" hidden="1"/>
+    <col min="2040" max="2040" width="15.7109375" style="1" hidden="1"/>
+    <col min="2041" max="2041" width="21.85546875" style="1" hidden="1"/>
+    <col min="2042" max="2044" width="11.42578125" style="1" hidden="1"/>
     <col min="2045" max="2045" width="16" style="1" hidden="1"/>
-    <col min="2046" max="2046" width="20.44140625" style="1" hidden="1"/>
-    <col min="2047" max="2293" width="11.44140625" style="1" hidden="1"/>
-    <col min="2294" max="2294" width="15.44140625" style="1" hidden="1"/>
-    <col min="2295" max="2295" width="11.44140625" style="1" hidden="1"/>
-    <col min="2296" max="2296" width="15.6640625" style="1" hidden="1"/>
-    <col min="2297" max="2297" width="21.88671875" style="1" hidden="1"/>
-    <col min="2298" max="2300" width="11.44140625" style="1" hidden="1"/>
+    <col min="2046" max="2046" width="20.42578125" style="1" hidden="1"/>
+    <col min="2047" max="2293" width="11.42578125" style="1" hidden="1"/>
+    <col min="2294" max="2294" width="15.42578125" style="1" hidden="1"/>
+    <col min="2295" max="2295" width="11.42578125" style="1" hidden="1"/>
+    <col min="2296" max="2296" width="15.7109375" style="1" hidden="1"/>
+    <col min="2297" max="2297" width="21.85546875" style="1" hidden="1"/>
+    <col min="2298" max="2300" width="11.42578125" style="1" hidden="1"/>
     <col min="2301" max="2301" width="16" style="1" hidden="1"/>
-    <col min="2302" max="2302" width="20.44140625" style="1" hidden="1"/>
-    <col min="2303" max="2549" width="11.44140625" style="1" hidden="1"/>
-    <col min="2550" max="2550" width="15.44140625" style="1" hidden="1"/>
-    <col min="2551" max="2551" width="11.44140625" style="1" hidden="1"/>
-    <col min="2552" max="2552" width="15.6640625" style="1" hidden="1"/>
-    <col min="2553" max="2553" width="21.88671875" style="1" hidden="1"/>
-    <col min="2554" max="2556" width="11.44140625" style="1" hidden="1"/>
+    <col min="2302" max="2302" width="20.42578125" style="1" hidden="1"/>
+    <col min="2303" max="2549" width="11.42578125" style="1" hidden="1"/>
+    <col min="2550" max="2550" width="15.42578125" style="1" hidden="1"/>
+    <col min="2551" max="2551" width="11.42578125" style="1" hidden="1"/>
+    <col min="2552" max="2552" width="15.7109375" style="1" hidden="1"/>
+    <col min="2553" max="2553" width="21.85546875" style="1" hidden="1"/>
+    <col min="2554" max="2556" width="11.42578125" style="1" hidden="1"/>
     <col min="2557" max="2557" width="16" style="1" hidden="1"/>
-    <col min="2558" max="2558" width="20.44140625" style="1" hidden="1"/>
-    <col min="2559" max="2805" width="11.44140625" style="1" hidden="1"/>
-    <col min="2806" max="2806" width="15.44140625" style="1" hidden="1"/>
-    <col min="2807" max="2807" width="11.44140625" style="1" hidden="1"/>
-    <col min="2808" max="2808" width="15.6640625" style="1" hidden="1"/>
-    <col min="2809" max="2809" width="21.88671875" style="1" hidden="1"/>
-    <col min="2810" max="2812" width="11.44140625" style="1" hidden="1"/>
+    <col min="2558" max="2558" width="20.42578125" style="1" hidden="1"/>
+    <col min="2559" max="2805" width="11.42578125" style="1" hidden="1"/>
+    <col min="2806" max="2806" width="15.42578125" style="1" hidden="1"/>
+    <col min="2807" max="2807" width="11.42578125" style="1" hidden="1"/>
+    <col min="2808" max="2808" width="15.7109375" style="1" hidden="1"/>
+    <col min="2809" max="2809" width="21.85546875" style="1" hidden="1"/>
+    <col min="2810" max="2812" width="11.42578125" style="1" hidden="1"/>
     <col min="2813" max="2813" width="16" style="1" hidden="1"/>
-    <col min="2814" max="2814" width="20.44140625" style="1" hidden="1"/>
-    <col min="2815" max="3061" width="11.44140625" style="1" hidden="1"/>
-    <col min="3062" max="3062" width="15.44140625" style="1" hidden="1"/>
-    <col min="3063" max="3063" width="11.44140625" style="1" hidden="1"/>
-    <col min="3064" max="3064" width="15.6640625" style="1" hidden="1"/>
-    <col min="3065" max="3065" width="21.88671875" style="1" hidden="1"/>
-    <col min="3066" max="3068" width="11.44140625" style="1" hidden="1"/>
+    <col min="2814" max="2814" width="20.42578125" style="1" hidden="1"/>
+    <col min="2815" max="3061" width="11.42578125" style="1" hidden="1"/>
+    <col min="3062" max="3062" width="15.42578125" style="1" hidden="1"/>
+    <col min="3063" max="3063" width="11.42578125" style="1" hidden="1"/>
+    <col min="3064" max="3064" width="15.7109375" style="1" hidden="1"/>
+    <col min="3065" max="3065" width="21.85546875" style="1" hidden="1"/>
+    <col min="3066" max="3068" width="11.42578125" style="1" hidden="1"/>
     <col min="3069" max="3069" width="16" style="1" hidden="1"/>
-    <col min="3070" max="3070" width="20.44140625" style="1" hidden="1"/>
-    <col min="3071" max="3317" width="11.44140625" style="1" hidden="1"/>
-    <col min="3318" max="3318" width="15.44140625" style="1" hidden="1"/>
-    <col min="3319" max="3319" width="11.44140625" style="1" hidden="1"/>
-    <col min="3320" max="3320" width="15.6640625" style="1" hidden="1"/>
-    <col min="3321" max="3321" width="21.88671875" style="1" hidden="1"/>
-    <col min="3322" max="3324" width="11.44140625" style="1" hidden="1"/>
+    <col min="3070" max="3070" width="20.42578125" style="1" hidden="1"/>
+    <col min="3071" max="3317" width="11.42578125" style="1" hidden="1"/>
+    <col min="3318" max="3318" width="15.42578125" style="1" hidden="1"/>
+    <col min="3319" max="3319" width="11.42578125" style="1" hidden="1"/>
+    <col min="3320" max="3320" width="15.7109375" style="1" hidden="1"/>
+    <col min="3321" max="3321" width="21.85546875" style="1" hidden="1"/>
+    <col min="3322" max="3324" width="11.42578125" style="1" hidden="1"/>
     <col min="3325" max="3325" width="16" style="1" hidden="1"/>
-    <col min="3326" max="3326" width="20.44140625" style="1" hidden="1"/>
-    <col min="3327" max="3573" width="11.44140625" style="1" hidden="1"/>
-    <col min="3574" max="3574" width="15.44140625" style="1" hidden="1"/>
-    <col min="3575" max="3575" width="11.44140625" style="1" hidden="1"/>
-    <col min="3576" max="3576" width="15.6640625" style="1" hidden="1"/>
-    <col min="3577" max="3577" width="21.88671875" style="1" hidden="1"/>
-    <col min="3578" max="3580" width="11.44140625" style="1" hidden="1"/>
+    <col min="3326" max="3326" width="20.42578125" style="1" hidden="1"/>
+    <col min="3327" max="3573" width="11.42578125" style="1" hidden="1"/>
+    <col min="3574" max="3574" width="15.42578125" style="1" hidden="1"/>
+    <col min="3575" max="3575" width="11.42578125" style="1" hidden="1"/>
+    <col min="3576" max="3576" width="15.7109375" style="1" hidden="1"/>
+    <col min="3577" max="3577" width="21.85546875" style="1" hidden="1"/>
+    <col min="3578" max="3580" width="11.42578125" style="1" hidden="1"/>
     <col min="3581" max="3581" width="16" style="1" hidden="1"/>
-    <col min="3582" max="3582" width="20.44140625" style="1" hidden="1"/>
-    <col min="3583" max="3829" width="11.44140625" style="1" hidden="1"/>
-    <col min="3830" max="3830" width="15.44140625" style="1" hidden="1"/>
-    <col min="3831" max="3831" width="11.44140625" style="1" hidden="1"/>
-    <col min="3832" max="3832" width="15.6640625" style="1" hidden="1"/>
-    <col min="3833" max="3833" width="21.88671875" style="1" hidden="1"/>
-    <col min="3834" max="3836" width="11.44140625" style="1" hidden="1"/>
+    <col min="3582" max="3582" width="20.42578125" style="1" hidden="1"/>
+    <col min="3583" max="3829" width="11.42578125" style="1" hidden="1"/>
+    <col min="3830" max="3830" width="15.42578125" style="1" hidden="1"/>
+    <col min="3831" max="3831" width="11.42578125" style="1" hidden="1"/>
+    <col min="3832" max="3832" width="15.7109375" style="1" hidden="1"/>
+    <col min="3833" max="3833" width="21.85546875" style="1" hidden="1"/>
+    <col min="3834" max="3836" width="11.42578125" style="1" hidden="1"/>
     <col min="3837" max="3837" width="16" style="1" hidden="1"/>
-    <col min="3838" max="3838" width="20.44140625" style="1" hidden="1"/>
-    <col min="3839" max="4085" width="11.44140625" style="1" hidden="1"/>
-    <col min="4086" max="4086" width="15.44140625" style="1" hidden="1"/>
-    <col min="4087" max="4087" width="11.44140625" style="1" hidden="1"/>
-    <col min="4088" max="4088" width="15.6640625" style="1" hidden="1"/>
-    <col min="4089" max="4089" width="21.88671875" style="1" hidden="1"/>
-    <col min="4090" max="4092" width="11.44140625" style="1" hidden="1"/>
+    <col min="3838" max="3838" width="20.42578125" style="1" hidden="1"/>
+    <col min="3839" max="4085" width="11.42578125" style="1" hidden="1"/>
+    <col min="4086" max="4086" width="15.42578125" style="1" hidden="1"/>
+    <col min="4087" max="4087" width="11.42578125" style="1" hidden="1"/>
+    <col min="4088" max="4088" width="15.7109375" style="1" hidden="1"/>
+    <col min="4089" max="4089" width="21.85546875" style="1" hidden="1"/>
+    <col min="4090" max="4092" width="11.42578125" style="1" hidden="1"/>
     <col min="4093" max="4093" width="16" style="1" hidden="1"/>
-    <col min="4094" max="4094" width="20.44140625" style="1" hidden="1"/>
-    <col min="4095" max="4341" width="11.44140625" style="1" hidden="1"/>
-    <col min="4342" max="4342" width="15.44140625" style="1" hidden="1"/>
-    <col min="4343" max="4343" width="11.44140625" style="1" hidden="1"/>
-    <col min="4344" max="4344" width="15.6640625" style="1" hidden="1"/>
-    <col min="4345" max="4345" width="21.88671875" style="1" hidden="1"/>
-    <col min="4346" max="4348" width="11.44140625" style="1" hidden="1"/>
+    <col min="4094" max="4094" width="20.42578125" style="1" hidden="1"/>
+    <col min="4095" max="4341" width="11.42578125" style="1" hidden="1"/>
+    <col min="4342" max="4342" width="15.42578125" style="1" hidden="1"/>
+    <col min="4343" max="4343" width="11.42578125" style="1" hidden="1"/>
+    <col min="4344" max="4344" width="15.7109375" style="1" hidden="1"/>
+    <col min="4345" max="4345" width="21.85546875" style="1" hidden="1"/>
+    <col min="4346" max="4348" width="11.42578125" style="1" hidden="1"/>
     <col min="4349" max="4349" width="16" style="1" hidden="1"/>
-    <col min="4350" max="4350" width="20.44140625" style="1" hidden="1"/>
-    <col min="4351" max="4597" width="11.44140625" style="1" hidden="1"/>
-    <col min="4598" max="4598" width="15.44140625" style="1" hidden="1"/>
-    <col min="4599" max="4599" width="11.44140625" style="1" hidden="1"/>
-    <col min="4600" max="4600" width="15.6640625" style="1" hidden="1"/>
-    <col min="4601" max="4601" width="21.88671875" style="1" hidden="1"/>
-    <col min="4602" max="4604" width="11.44140625" style="1" hidden="1"/>
+    <col min="4350" max="4350" width="20.42578125" style="1" hidden="1"/>
+    <col min="4351" max="4597" width="11.42578125" style="1" hidden="1"/>
+    <col min="4598" max="4598" width="15.42578125" style="1" hidden="1"/>
+    <col min="4599" max="4599" width="11.42578125" style="1" hidden="1"/>
+    <col min="4600" max="4600" width="15.7109375" style="1" hidden="1"/>
+    <col min="4601" max="4601" width="21.85546875" style="1" hidden="1"/>
+    <col min="4602" max="4604" width="11.42578125" style="1" hidden="1"/>
     <col min="4605" max="4605" width="16" style="1" hidden="1"/>
-    <col min="4606" max="4606" width="20.44140625" style="1" hidden="1"/>
-    <col min="4607" max="4853" width="11.44140625" style="1" hidden="1"/>
-    <col min="4854" max="4854" width="15.44140625" style="1" hidden="1"/>
-    <col min="4855" max="4855" width="11.44140625" style="1" hidden="1"/>
-    <col min="4856" max="4856" width="15.6640625" style="1" hidden="1"/>
-    <col min="4857" max="4857" width="21.88671875" style="1" hidden="1"/>
-    <col min="4858" max="4860" width="11.44140625" style="1" hidden="1"/>
+    <col min="4606" max="4606" width="20.42578125" style="1" hidden="1"/>
+    <col min="4607" max="4853" width="11.42578125" style="1" hidden="1"/>
+    <col min="4854" max="4854" width="15.42578125" style="1" hidden="1"/>
+    <col min="4855" max="4855" width="11.42578125" style="1" hidden="1"/>
+    <col min="4856" max="4856" width="15.7109375" style="1" hidden="1"/>
+    <col min="4857" max="4857" width="21.85546875" style="1" hidden="1"/>
+    <col min="4858" max="4860" width="11.42578125" style="1" hidden="1"/>
     <col min="4861" max="4861" width="16" style="1" hidden="1"/>
-    <col min="4862" max="4862" width="20.44140625" style="1" hidden="1"/>
-    <col min="4863" max="5109" width="11.44140625" style="1" hidden="1"/>
-    <col min="5110" max="5110" width="15.44140625" style="1" hidden="1"/>
-    <col min="5111" max="5111" width="11.44140625" style="1" hidden="1"/>
-    <col min="5112" max="5112" width="15.6640625" style="1" hidden="1"/>
-    <col min="5113" max="5113" width="21.88671875" style="1" hidden="1"/>
-    <col min="5114" max="5116" width="11.44140625" style="1" hidden="1"/>
+    <col min="4862" max="4862" width="20.42578125" style="1" hidden="1"/>
+    <col min="4863" max="5109" width="11.42578125" style="1" hidden="1"/>
+    <col min="5110" max="5110" width="15.42578125" style="1" hidden="1"/>
+    <col min="5111" max="5111" width="11.42578125" style="1" hidden="1"/>
+    <col min="5112" max="5112" width="15.7109375" style="1" hidden="1"/>
+    <col min="5113" max="5113" width="21.85546875" style="1" hidden="1"/>
+    <col min="5114" max="5116" width="11.42578125" style="1" hidden="1"/>
     <col min="5117" max="5117" width="16" style="1" hidden="1"/>
-    <col min="5118" max="5118" width="20.44140625" style="1" hidden="1"/>
-    <col min="5119" max="5365" width="11.44140625" style="1" hidden="1"/>
-    <col min="5366" max="5366" width="15.44140625" style="1" hidden="1"/>
-    <col min="5367" max="5367" width="11.44140625" style="1" hidden="1"/>
-    <col min="5368" max="5368" width="15.6640625" style="1" hidden="1"/>
-    <col min="5369" max="5369" width="21.88671875" style="1" hidden="1"/>
-    <col min="5370" max="5372" width="11.44140625" style="1" hidden="1"/>
+    <col min="5118" max="5118" width="20.42578125" style="1" hidden="1"/>
+    <col min="5119" max="5365" width="11.42578125" style="1" hidden="1"/>
+    <col min="5366" max="5366" width="15.42578125" style="1" hidden="1"/>
+    <col min="5367" max="5367" width="11.42578125" style="1" hidden="1"/>
+    <col min="5368" max="5368" width="15.7109375" style="1" hidden="1"/>
+    <col min="5369" max="5369" width="21.85546875" style="1" hidden="1"/>
+    <col min="5370" max="5372" width="11.42578125" style="1" hidden="1"/>
     <col min="5373" max="5373" width="16" style="1" hidden="1"/>
-    <col min="5374" max="5374" width="20.44140625" style="1" hidden="1"/>
-    <col min="5375" max="5621" width="11.44140625" style="1" hidden="1"/>
-    <col min="5622" max="5622" width="15.44140625" style="1" hidden="1"/>
-    <col min="5623" max="5623" width="11.44140625" style="1" hidden="1"/>
-    <col min="5624" max="5624" width="15.6640625" style="1" hidden="1"/>
-    <col min="5625" max="5625" width="21.88671875" style="1" hidden="1"/>
-    <col min="5626" max="5628" width="11.44140625" style="1" hidden="1"/>
+    <col min="5374" max="5374" width="20.42578125" style="1" hidden="1"/>
+    <col min="5375" max="5621" width="11.42578125" style="1" hidden="1"/>
+    <col min="5622" max="5622" width="15.42578125" style="1" hidden="1"/>
+    <col min="5623" max="5623" width="11.42578125" style="1" hidden="1"/>
+    <col min="5624" max="5624" width="15.7109375" style="1" hidden="1"/>
+    <col min="5625" max="5625" width="21.85546875" style="1" hidden="1"/>
+    <col min="5626" max="5628" width="11.42578125" style="1" hidden="1"/>
     <col min="5629" max="5629" width="16" style="1" hidden="1"/>
-    <col min="5630" max="5630" width="20.44140625" style="1" hidden="1"/>
-    <col min="5631" max="5877" width="11.44140625" style="1" hidden="1"/>
-    <col min="5878" max="5878" width="15.44140625" style="1" hidden="1"/>
-    <col min="5879" max="5879" width="11.44140625" style="1" hidden="1"/>
-    <col min="5880" max="5880" width="15.6640625" style="1" hidden="1"/>
-    <col min="5881" max="5881" width="21.88671875" style="1" hidden="1"/>
-    <col min="5882" max="5884" width="11.44140625" style="1" hidden="1"/>
+    <col min="5630" max="5630" width="20.42578125" style="1" hidden="1"/>
+    <col min="5631" max="5877" width="11.42578125" style="1" hidden="1"/>
+    <col min="5878" max="5878" width="15.42578125" style="1" hidden="1"/>
+    <col min="5879" max="5879" width="11.42578125" style="1" hidden="1"/>
+    <col min="5880" max="5880" width="15.7109375" style="1" hidden="1"/>
+    <col min="5881" max="5881" width="21.85546875" style="1" hidden="1"/>
+    <col min="5882" max="5884" width="11.42578125" style="1" hidden="1"/>
     <col min="5885" max="5885" width="16" style="1" hidden="1"/>
-    <col min="5886" max="5886" width="20.44140625" style="1" hidden="1"/>
-    <col min="5887" max="6133" width="11.44140625" style="1" hidden="1"/>
-    <col min="6134" max="6134" width="15.44140625" style="1" hidden="1"/>
-    <col min="6135" max="6135" width="11.44140625" style="1" hidden="1"/>
-    <col min="6136" max="6136" width="15.6640625" style="1" hidden="1"/>
-    <col min="6137" max="6137" width="21.88671875" style="1" hidden="1"/>
-    <col min="6138" max="6140" width="11.44140625" style="1" hidden="1"/>
+    <col min="5886" max="5886" width="20.42578125" style="1" hidden="1"/>
+    <col min="5887" max="6133" width="11.42578125" style="1" hidden="1"/>
+    <col min="6134" max="6134" width="15.42578125" style="1" hidden="1"/>
+    <col min="6135" max="6135" width="11.42578125" style="1" hidden="1"/>
+    <col min="6136" max="6136" width="15.7109375" style="1" hidden="1"/>
+    <col min="6137" max="6137" width="21.85546875" style="1" hidden="1"/>
+    <col min="6138" max="6140" width="11.42578125" style="1" hidden="1"/>
     <col min="6141" max="6141" width="16" style="1" hidden="1"/>
-    <col min="6142" max="6142" width="20.44140625" style="1" hidden="1"/>
-    <col min="6143" max="6389" width="11.44140625" style="1" hidden="1"/>
-    <col min="6390" max="6390" width="15.44140625" style="1" hidden="1"/>
-    <col min="6391" max="6391" width="11.44140625" style="1" hidden="1"/>
-    <col min="6392" max="6392" width="15.6640625" style="1" hidden="1"/>
-    <col min="6393" max="6393" width="21.88671875" style="1" hidden="1"/>
-    <col min="6394" max="6396" width="11.44140625" style="1" hidden="1"/>
+    <col min="6142" max="6142" width="20.42578125" style="1" hidden="1"/>
+    <col min="6143" max="6389" width="11.42578125" style="1" hidden="1"/>
+    <col min="6390" max="6390" width="15.42578125" style="1" hidden="1"/>
+    <col min="6391" max="6391" width="11.42578125" style="1" hidden="1"/>
+    <col min="6392" max="6392" width="15.7109375" style="1" hidden="1"/>
+    <col min="6393" max="6393" width="21.85546875" style="1" hidden="1"/>
+    <col min="6394" max="6396" width="11.42578125" style="1" hidden="1"/>
     <col min="6397" max="6397" width="16" style="1" hidden="1"/>
-    <col min="6398" max="6398" width="20.44140625" style="1" hidden="1"/>
-    <col min="6399" max="6645" width="11.44140625" style="1" hidden="1"/>
-    <col min="6646" max="6646" width="15.44140625" style="1" hidden="1"/>
-    <col min="6647" max="6647" width="11.44140625" style="1" hidden="1"/>
-    <col min="6648" max="6648" width="15.6640625" style="1" hidden="1"/>
-    <col min="6649" max="6649" width="21.88671875" style="1" hidden="1"/>
-    <col min="6650" max="6652" width="11.44140625" style="1" hidden="1"/>
+    <col min="6398" max="6398" width="20.42578125" style="1" hidden="1"/>
+    <col min="6399" max="6645" width="11.42578125" style="1" hidden="1"/>
+    <col min="6646" max="6646" width="15.42578125" style="1" hidden="1"/>
+    <col min="6647" max="6647" width="11.42578125" style="1" hidden="1"/>
+    <col min="6648" max="6648" width="15.7109375" style="1" hidden="1"/>
+    <col min="6649" max="6649" width="21.85546875" style="1" hidden="1"/>
+    <col min="6650" max="6652" width="11.42578125" style="1" hidden="1"/>
     <col min="6653" max="6653" width="16" style="1" hidden="1"/>
-    <col min="6654" max="6654" width="20.44140625" style="1" hidden="1"/>
-    <col min="6655" max="6901" width="11.44140625" style="1" hidden="1"/>
-    <col min="6902" max="6902" width="15.44140625" style="1" hidden="1"/>
-    <col min="6903" max="6903" width="11.44140625" style="1" hidden="1"/>
-    <col min="6904" max="6904" width="15.6640625" style="1" hidden="1"/>
-    <col min="6905" max="6905" width="21.88671875" style="1" hidden="1"/>
-    <col min="6906" max="6908" width="11.44140625" style="1" hidden="1"/>
+    <col min="6654" max="6654" width="20.42578125" style="1" hidden="1"/>
+    <col min="6655" max="6901" width="11.42578125" style="1" hidden="1"/>
+    <col min="6902" max="6902" width="15.42578125" style="1" hidden="1"/>
+    <col min="6903" max="6903" width="11.42578125" style="1" hidden="1"/>
+    <col min="6904" max="6904" width="15.7109375" style="1" hidden="1"/>
+    <col min="6905" max="6905" width="21.85546875" style="1" hidden="1"/>
+    <col min="6906" max="6908" width="11.42578125" style="1" hidden="1"/>
     <col min="6909" max="6909" width="16" style="1" hidden="1"/>
-    <col min="6910" max="6910" width="20.44140625" style="1" hidden="1"/>
-    <col min="6911" max="7157" width="11.44140625" style="1" hidden="1"/>
-    <col min="7158" max="7158" width="15.44140625" style="1" hidden="1"/>
-    <col min="7159" max="7159" width="11.44140625" style="1" hidden="1"/>
-    <col min="7160" max="7160" width="15.6640625" style="1" hidden="1"/>
-    <col min="7161" max="7161" width="21.88671875" style="1" hidden="1"/>
-    <col min="7162" max="7164" width="11.44140625" style="1" hidden="1"/>
+    <col min="6910" max="6910" width="20.42578125" style="1" hidden="1"/>
+    <col min="6911" max="7157" width="11.42578125" style="1" hidden="1"/>
+    <col min="7158" max="7158" width="15.42578125" style="1" hidden="1"/>
+    <col min="7159" max="7159" width="11.42578125" style="1" hidden="1"/>
+    <col min="7160" max="7160" width="15.7109375" style="1" hidden="1"/>
+    <col min="7161" max="7161" width="21.85546875" style="1" hidden="1"/>
+    <col min="7162" max="7164" width="11.42578125" style="1" hidden="1"/>
     <col min="7165" max="7165" width="16" style="1" hidden="1"/>
-    <col min="7166" max="7166" width="20.44140625" style="1" hidden="1"/>
-    <col min="7167" max="7413" width="11.44140625" style="1" hidden="1"/>
-    <col min="7414" max="7414" width="15.44140625" style="1" hidden="1"/>
-    <col min="7415" max="7415" width="11.44140625" style="1" hidden="1"/>
-    <col min="7416" max="7416" width="15.6640625" style="1" hidden="1"/>
-    <col min="7417" max="7417" width="21.88671875" style="1" hidden="1"/>
-    <col min="7418" max="7420" width="11.44140625" style="1" hidden="1"/>
+    <col min="7166" max="7166" width="20.42578125" style="1" hidden="1"/>
+    <col min="7167" max="7413" width="11.42578125" style="1" hidden="1"/>
+    <col min="7414" max="7414" width="15.42578125" style="1" hidden="1"/>
+    <col min="7415" max="7415" width="11.42578125" style="1" hidden="1"/>
+    <col min="7416" max="7416" width="15.7109375" style="1" hidden="1"/>
+    <col min="7417" max="7417" width="21.85546875" style="1" hidden="1"/>
+    <col min="7418" max="7420" width="11.42578125" style="1" hidden="1"/>
     <col min="7421" max="7421" width="16" style="1" hidden="1"/>
-    <col min="7422" max="7422" width="20.44140625" style="1" hidden="1"/>
-    <col min="7423" max="7669" width="11.44140625" style="1" hidden="1"/>
-    <col min="7670" max="7670" width="15.44140625" style="1" hidden="1"/>
-    <col min="7671" max="7671" width="11.44140625" style="1" hidden="1"/>
-    <col min="7672" max="7672" width="15.6640625" style="1" hidden="1"/>
-    <col min="7673" max="7673" width="21.88671875" style="1" hidden="1"/>
-    <col min="7674" max="7676" width="11.44140625" style="1" hidden="1"/>
+    <col min="7422" max="7422" width="20.42578125" style="1" hidden="1"/>
+    <col min="7423" max="7669" width="11.42578125" style="1" hidden="1"/>
+    <col min="7670" max="7670" width="15.42578125" style="1" hidden="1"/>
+    <col min="7671" max="7671" width="11.42578125" style="1" hidden="1"/>
+    <col min="7672" max="7672" width="15.7109375" style="1" hidden="1"/>
+    <col min="7673" max="7673" width="21.85546875" style="1" hidden="1"/>
+    <col min="7674" max="7676" width="11.42578125" style="1" hidden="1"/>
     <col min="7677" max="7677" width="16" style="1" hidden="1"/>
-    <col min="7678" max="7678" width="20.44140625" style="1" hidden="1"/>
-    <col min="7679" max="7925" width="11.44140625" style="1" hidden="1"/>
-    <col min="7926" max="7926" width="15.44140625" style="1" hidden="1"/>
-    <col min="7927" max="7927" width="11.44140625" style="1" hidden="1"/>
-    <col min="7928" max="7928" width="15.6640625" style="1" hidden="1"/>
-    <col min="7929" max="7929" width="21.88671875" style="1" hidden="1"/>
-    <col min="7930" max="7932" width="11.44140625" style="1" hidden="1"/>
+    <col min="7678" max="7678" width="20.42578125" style="1" hidden="1"/>
+    <col min="7679" max="7925" width="11.42578125" style="1" hidden="1"/>
+    <col min="7926" max="7926" width="15.42578125" style="1" hidden="1"/>
+    <col min="7927" max="7927" width="11.42578125" style="1" hidden="1"/>
+    <col min="7928" max="7928" width="15.7109375" style="1" hidden="1"/>
+    <col min="7929" max="7929" width="21.85546875" style="1" hidden="1"/>
+    <col min="7930" max="7932" width="11.42578125" style="1" hidden="1"/>
     <col min="7933" max="7933" width="16" style="1" hidden="1"/>
-    <col min="7934" max="7934" width="20.44140625" style="1" hidden="1"/>
-    <col min="7935" max="8181" width="11.44140625" style="1" hidden="1"/>
-    <col min="8182" max="8182" width="15.44140625" style="1" hidden="1"/>
-    <col min="8183" max="8183" width="11.44140625" style="1" hidden="1"/>
-    <col min="8184" max="8184" width="15.6640625" style="1" hidden="1"/>
-    <col min="8185" max="8185" width="21.88671875" style="1" hidden="1"/>
-    <col min="8186" max="8188" width="11.44140625" style="1" hidden="1"/>
+    <col min="7934" max="7934" width="20.42578125" style="1" hidden="1"/>
+    <col min="7935" max="8181" width="11.42578125" style="1" hidden="1"/>
+    <col min="8182" max="8182" width="15.42578125" style="1" hidden="1"/>
+    <col min="8183" max="8183" width="11.42578125" style="1" hidden="1"/>
+    <col min="8184" max="8184" width="15.7109375" style="1" hidden="1"/>
+    <col min="8185" max="8185" width="21.85546875" style="1" hidden="1"/>
+    <col min="8186" max="8188" width="11.42578125" style="1" hidden="1"/>
     <col min="8189" max="8189" width="16" style="1" hidden="1"/>
-    <col min="8190" max="8190" width="20.44140625" style="1" hidden="1"/>
-    <col min="8191" max="8437" width="11.44140625" style="1" hidden="1"/>
-    <col min="8438" max="8438" width="15.44140625" style="1" hidden="1"/>
-    <col min="8439" max="8439" width="11.44140625" style="1" hidden="1"/>
-    <col min="8440" max="8440" width="15.6640625" style="1" hidden="1"/>
-    <col min="8441" max="8441" width="21.88671875" style="1" hidden="1"/>
-    <col min="8442" max="8444" width="11.44140625" style="1" hidden="1"/>
+    <col min="8190" max="8190" width="20.42578125" style="1" hidden="1"/>
+    <col min="8191" max="8437" width="11.42578125" style="1" hidden="1"/>
+    <col min="8438" max="8438" width="15.42578125" style="1" hidden="1"/>
+    <col min="8439" max="8439" width="11.42578125" style="1" hidden="1"/>
+    <col min="8440" max="8440" width="15.7109375" style="1" hidden="1"/>
+    <col min="8441" max="8441" width="21.85546875" style="1" hidden="1"/>
+    <col min="8442" max="8444" width="11.42578125" style="1" hidden="1"/>
     <col min="8445" max="8445" width="16" style="1" hidden="1"/>
-    <col min="8446" max="8446" width="20.44140625" style="1" hidden="1"/>
-    <col min="8447" max="8693" width="11.44140625" style="1" hidden="1"/>
-    <col min="8694" max="8694" width="15.44140625" style="1" hidden="1"/>
-    <col min="8695" max="8695" width="11.44140625" style="1" hidden="1"/>
-    <col min="8696" max="8696" width="15.6640625" style="1" hidden="1"/>
-    <col min="8697" max="8697" width="21.88671875" style="1" hidden="1"/>
-    <col min="8698" max="8700" width="11.44140625" style="1" hidden="1"/>
+    <col min="8446" max="8446" width="20.42578125" style="1" hidden="1"/>
+    <col min="8447" max="8693" width="11.42578125" style="1" hidden="1"/>
+    <col min="8694" max="8694" width="15.42578125" style="1" hidden="1"/>
+    <col min="8695" max="8695" width="11.42578125" style="1" hidden="1"/>
+    <col min="8696" max="8696" width="15.7109375" style="1" hidden="1"/>
+    <col min="8697" max="8697" width="21.85546875" style="1" hidden="1"/>
+    <col min="8698" max="8700" width="11.42578125" style="1" hidden="1"/>
     <col min="8701" max="8701" width="16" style="1" hidden="1"/>
-    <col min="8702" max="8702" width="20.44140625" style="1" hidden="1"/>
-    <col min="8703" max="8949" width="11.44140625" style="1" hidden="1"/>
-    <col min="8950" max="8950" width="15.44140625" style="1" hidden="1"/>
-    <col min="8951" max="8951" width="11.44140625" style="1" hidden="1"/>
-    <col min="8952" max="8952" width="15.6640625" style="1" hidden="1"/>
-    <col min="8953" max="8953" width="21.88671875" style="1" hidden="1"/>
-    <col min="8954" max="8956" width="11.44140625" style="1" hidden="1"/>
+    <col min="8702" max="8702" width="20.42578125" style="1" hidden="1"/>
+    <col min="8703" max="8949" width="11.42578125" style="1" hidden="1"/>
+    <col min="8950" max="8950" width="15.42578125" style="1" hidden="1"/>
+    <col min="8951" max="8951" width="11.42578125" style="1" hidden="1"/>
+    <col min="8952" max="8952" width="15.7109375" style="1" hidden="1"/>
+    <col min="8953" max="8953" width="21.85546875" style="1" hidden="1"/>
+    <col min="8954" max="8956" width="11.42578125" style="1" hidden="1"/>
     <col min="8957" max="8957" width="16" style="1" hidden="1"/>
-    <col min="8958" max="8958" width="20.44140625" style="1" hidden="1"/>
-    <col min="8959" max="9205" width="11.44140625" style="1" hidden="1"/>
-    <col min="9206" max="9206" width="15.44140625" style="1" hidden="1"/>
-    <col min="9207" max="9207" width="11.44140625" style="1" hidden="1"/>
-    <col min="9208" max="9208" width="15.6640625" style="1" hidden="1"/>
-    <col min="9209" max="9209" width="21.88671875" style="1" hidden="1"/>
-    <col min="9210" max="9212" width="11.44140625" style="1" hidden="1"/>
+    <col min="8958" max="8958" width="20.42578125" style="1" hidden="1"/>
+    <col min="8959" max="9205" width="11.42578125" style="1" hidden="1"/>
+    <col min="9206" max="9206" width="15.42578125" style="1" hidden="1"/>
+    <col min="9207" max="9207" width="11.42578125" style="1" hidden="1"/>
+    <col min="9208" max="9208" width="15.7109375" style="1" hidden="1"/>
+    <col min="9209" max="9209" width="21.85546875" style="1" hidden="1"/>
+    <col min="9210" max="9212" width="11.42578125" style="1" hidden="1"/>
     <col min="9213" max="9213" width="16" style="1" hidden="1"/>
-    <col min="9214" max="9214" width="20.44140625" style="1" hidden="1"/>
-    <col min="9215" max="9461" width="11.44140625" style="1" hidden="1"/>
-    <col min="9462" max="9462" width="15.44140625" style="1" hidden="1"/>
-    <col min="9463" max="9463" width="11.44140625" style="1" hidden="1"/>
-    <col min="9464" max="9464" width="15.6640625" style="1" hidden="1"/>
-    <col min="9465" max="9465" width="21.88671875" style="1" hidden="1"/>
-    <col min="9466" max="9468" width="11.44140625" style="1" hidden="1"/>
+    <col min="9214" max="9214" width="20.42578125" style="1" hidden="1"/>
+    <col min="9215" max="9461" width="11.42578125" style="1" hidden="1"/>
+    <col min="9462" max="9462" width="15.42578125" style="1" hidden="1"/>
+    <col min="9463" max="9463" width="11.42578125" style="1" hidden="1"/>
+    <col min="9464" max="9464" width="15.7109375" style="1" hidden="1"/>
+    <col min="9465" max="9465" width="21.85546875" style="1" hidden="1"/>
+    <col min="9466" max="9468" width="11.42578125" style="1" hidden="1"/>
     <col min="9469" max="9469" width="16" style="1" hidden="1"/>
-    <col min="9470" max="9470" width="20.44140625" style="1" hidden="1"/>
-    <col min="9471" max="9717" width="11.44140625" style="1" hidden="1"/>
-    <col min="9718" max="9718" width="15.44140625" style="1" hidden="1"/>
-    <col min="9719" max="9719" width="11.44140625" style="1" hidden="1"/>
-    <col min="9720" max="9720" width="15.6640625" style="1" hidden="1"/>
-    <col min="9721" max="9721" width="21.88671875" style="1" hidden="1"/>
-    <col min="9722" max="9724" width="11.44140625" style="1" hidden="1"/>
+    <col min="9470" max="9470" width="20.42578125" style="1" hidden="1"/>
+    <col min="9471" max="9717" width="11.42578125" style="1" hidden="1"/>
+    <col min="9718" max="9718" width="15.42578125" style="1" hidden="1"/>
+    <col min="9719" max="9719" width="11.42578125" style="1" hidden="1"/>
+    <col min="9720" max="9720" width="15.7109375" style="1" hidden="1"/>
+    <col min="9721" max="9721" width="21.85546875" style="1" hidden="1"/>
+    <col min="9722" max="9724" width="11.42578125" style="1" hidden="1"/>
     <col min="9725" max="9725" width="16" style="1" hidden="1"/>
-    <col min="9726" max="9726" width="20.44140625" style="1" hidden="1"/>
-    <col min="9727" max="9973" width="11.44140625" style="1" hidden="1"/>
-    <col min="9974" max="9974" width="15.44140625" style="1" hidden="1"/>
-    <col min="9975" max="9975" width="11.44140625" style="1" hidden="1"/>
-    <col min="9976" max="9976" width="15.6640625" style="1" hidden="1"/>
-    <col min="9977" max="9977" width="21.88671875" style="1" hidden="1"/>
-    <col min="9978" max="9980" width="11.44140625" style="1" hidden="1"/>
+    <col min="9726" max="9726" width="20.42578125" style="1" hidden="1"/>
+    <col min="9727" max="9973" width="11.42578125" style="1" hidden="1"/>
+    <col min="9974" max="9974" width="15.42578125" style="1" hidden="1"/>
+    <col min="9975" max="9975" width="11.42578125" style="1" hidden="1"/>
+    <col min="9976" max="9976" width="15.7109375" style="1" hidden="1"/>
+    <col min="9977" max="9977" width="21.85546875" style="1" hidden="1"/>
+    <col min="9978" max="9980" width="11.42578125" style="1" hidden="1"/>
     <col min="9981" max="9981" width="16" style="1" hidden="1"/>
-    <col min="9982" max="9982" width="20.44140625" style="1" hidden="1"/>
-    <col min="9983" max="10229" width="11.44140625" style="1" hidden="1"/>
-    <col min="10230" max="10230" width="15.44140625" style="1" hidden="1"/>
-    <col min="10231" max="10231" width="11.44140625" style="1" hidden="1"/>
-    <col min="10232" max="10232" width="15.6640625" style="1" hidden="1"/>
-    <col min="10233" max="10233" width="21.88671875" style="1" hidden="1"/>
-    <col min="10234" max="10236" width="11.44140625" style="1" hidden="1"/>
+    <col min="9982" max="9982" width="20.42578125" style="1" hidden="1"/>
+    <col min="9983" max="10229" width="11.42578125" style="1" hidden="1"/>
+    <col min="10230" max="10230" width="15.42578125" style="1" hidden="1"/>
+    <col min="10231" max="10231" width="11.42578125" style="1" hidden="1"/>
+    <col min="10232" max="10232" width="15.7109375" style="1" hidden="1"/>
+    <col min="10233" max="10233" width="21.85546875" style="1" hidden="1"/>
+    <col min="10234" max="10236" width="11.42578125" style="1" hidden="1"/>
     <col min="10237" max="10237" width="16" style="1" hidden="1"/>
-    <col min="10238" max="10238" width="20.44140625" style="1" hidden="1"/>
-    <col min="10239" max="10485" width="11.44140625" style="1" hidden="1"/>
-    <col min="10486" max="10486" width="15.44140625" style="1" hidden="1"/>
-    <col min="10487" max="10487" width="11.44140625" style="1" hidden="1"/>
-    <col min="10488" max="10488" width="15.6640625" style="1" hidden="1"/>
-    <col min="10489" max="10489" width="21.88671875" style="1" hidden="1"/>
-    <col min="10490" max="10492" width="11.44140625" style="1" hidden="1"/>
+    <col min="10238" max="10238" width="20.42578125" style="1" hidden="1"/>
+    <col min="10239" max="10485" width="11.42578125" style="1" hidden="1"/>
+    <col min="10486" max="10486" width="15.42578125" style="1" hidden="1"/>
+    <col min="10487" max="10487" width="11.42578125" style="1" hidden="1"/>
+    <col min="10488" max="10488" width="15.7109375" style="1" hidden="1"/>
+    <col min="10489" max="10489" width="21.85546875" style="1" hidden="1"/>
+    <col min="10490" max="10492" width="11.42578125" style="1" hidden="1"/>
     <col min="10493" max="10493" width="16" style="1" hidden="1"/>
-    <col min="10494" max="10494" width="20.44140625" style="1" hidden="1"/>
-    <col min="10495" max="10741" width="11.44140625" style="1" hidden="1"/>
-    <col min="10742" max="10742" width="15.44140625" style="1" hidden="1"/>
-    <col min="10743" max="10743" width="11.44140625" style="1" hidden="1"/>
-    <col min="10744" max="10744" width="15.6640625" style="1" hidden="1"/>
-    <col min="10745" max="10745" width="21.88671875" style="1" hidden="1"/>
-    <col min="10746" max="10748" width="11.44140625" style="1" hidden="1"/>
+    <col min="10494" max="10494" width="20.42578125" style="1" hidden="1"/>
+    <col min="10495" max="10741" width="11.42578125" style="1" hidden="1"/>
+    <col min="10742" max="10742" width="15.42578125" style="1" hidden="1"/>
+    <col min="10743" max="10743" width="11.42578125" style="1" hidden="1"/>
+    <col min="10744" max="10744" width="15.7109375" style="1" hidden="1"/>
+    <col min="10745" max="10745" width="21.85546875" style="1" hidden="1"/>
+    <col min="10746" max="10748" width="11.42578125" style="1" hidden="1"/>
     <col min="10749" max="10749" width="16" style="1" hidden="1"/>
-    <col min="10750" max="10750" width="20.44140625" style="1" hidden="1"/>
-    <col min="10751" max="10997" width="11.44140625" style="1" hidden="1"/>
-    <col min="10998" max="10998" width="15.44140625" style="1" hidden="1"/>
-    <col min="10999" max="10999" width="11.44140625" style="1" hidden="1"/>
-    <col min="11000" max="11000" width="15.6640625" style="1" hidden="1"/>
-    <col min="11001" max="11001" width="21.88671875" style="1" hidden="1"/>
-    <col min="11002" max="11004" width="11.44140625" style="1" hidden="1"/>
+    <col min="10750" max="10750" width="20.42578125" style="1" hidden="1"/>
+    <col min="10751" max="10997" width="11.42578125" style="1" hidden="1"/>
+    <col min="10998" max="10998" width="15.42578125" style="1" hidden="1"/>
+    <col min="10999" max="10999" width="11.42578125" style="1" hidden="1"/>
+    <col min="11000" max="11000" width="15.7109375" style="1" hidden="1"/>
+    <col min="11001" max="11001" width="21.85546875" style="1" hidden="1"/>
+    <col min="11002" max="11004" width="11.42578125" style="1" hidden="1"/>
     <col min="11005" max="11005" width="16" style="1" hidden="1"/>
-    <col min="11006" max="11006" width="20.44140625" style="1" hidden="1"/>
-    <col min="11007" max="11253" width="11.44140625" style="1" hidden="1"/>
-    <col min="11254" max="11254" width="15.44140625" style="1" hidden="1"/>
-    <col min="11255" max="11255" width="11.44140625" style="1" hidden="1"/>
-    <col min="11256" max="11256" width="15.6640625" style="1" hidden="1"/>
-    <col min="11257" max="11257" width="21.88671875" style="1" hidden="1"/>
-    <col min="11258" max="11260" width="11.44140625" style="1" hidden="1"/>
+    <col min="11006" max="11006" width="20.42578125" style="1" hidden="1"/>
+    <col min="11007" max="11253" width="11.42578125" style="1" hidden="1"/>
+    <col min="11254" max="11254" width="15.42578125" style="1" hidden="1"/>
+    <col min="11255" max="11255" width="11.42578125" style="1" hidden="1"/>
+    <col min="11256" max="11256" width="15.7109375" style="1" hidden="1"/>
+    <col min="11257" max="11257" width="21.85546875" style="1" hidden="1"/>
+    <col min="11258" max="11260" width="11.42578125" style="1" hidden="1"/>
     <col min="11261" max="11261" width="16" style="1" hidden="1"/>
-    <col min="11262" max="11262" width="20.44140625" style="1" hidden="1"/>
-    <col min="11263" max="11509" width="11.44140625" style="1" hidden="1"/>
-    <col min="11510" max="11510" width="15.44140625" style="1" hidden="1"/>
-    <col min="11511" max="11511" width="11.44140625" style="1" hidden="1"/>
-    <col min="11512" max="11512" width="15.6640625" style="1" hidden="1"/>
-    <col min="11513" max="11513" width="21.88671875" style="1" hidden="1"/>
-    <col min="11514" max="11516" width="11.44140625" style="1" hidden="1"/>
+    <col min="11262" max="11262" width="20.42578125" style="1" hidden="1"/>
+    <col min="11263" max="11509" width="11.42578125" style="1" hidden="1"/>
+    <col min="11510" max="11510" width="15.42578125" style="1" hidden="1"/>
+    <col min="11511" max="11511" width="11.42578125" style="1" hidden="1"/>
+    <col min="11512" max="11512" width="15.7109375" style="1" hidden="1"/>
+    <col min="11513" max="11513" width="21.85546875" style="1" hidden="1"/>
+    <col min="11514" max="11516" width="11.42578125" style="1" hidden="1"/>
     <col min="11517" max="11517" width="16" style="1" hidden="1"/>
-    <col min="11518" max="11518" width="20.44140625" style="1" hidden="1"/>
-    <col min="11519" max="11765" width="11.44140625" style="1" hidden="1"/>
-    <col min="11766" max="11766" width="15.44140625" style="1" hidden="1"/>
-    <col min="11767" max="11767" width="11.44140625" style="1" hidden="1"/>
-    <col min="11768" max="11768" width="15.6640625" style="1" hidden="1"/>
-    <col min="11769" max="11769" width="21.88671875" style="1" hidden="1"/>
-    <col min="11770" max="11772" width="11.44140625" style="1" hidden="1"/>
+    <col min="11518" max="11518" width="20.42578125" style="1" hidden="1"/>
+    <col min="11519" max="11765" width="11.42578125" style="1" hidden="1"/>
+    <col min="11766" max="11766" width="15.42578125" style="1" hidden="1"/>
+    <col min="11767" max="11767" width="11.42578125" style="1" hidden="1"/>
+    <col min="11768" max="11768" width="15.7109375" style="1" hidden="1"/>
+    <col min="11769" max="11769" width="21.85546875" style="1" hidden="1"/>
+    <col min="11770" max="11772" width="11.42578125" style="1" hidden="1"/>
     <col min="11773" max="11773" width="16" style="1" hidden="1"/>
-    <col min="11774" max="11774" width="20.44140625" style="1" hidden="1"/>
-    <col min="11775" max="12021" width="11.44140625" style="1" hidden="1"/>
-    <col min="12022" max="12022" width="15.44140625" style="1" hidden="1"/>
-    <col min="12023" max="12023" width="11.44140625" style="1" hidden="1"/>
-    <col min="12024" max="12024" width="15.6640625" style="1" hidden="1"/>
-    <col min="12025" max="12025" width="21.88671875" style="1" hidden="1"/>
-    <col min="12026" max="12028" width="11.44140625" style="1" hidden="1"/>
+    <col min="11774" max="11774" width="20.42578125" style="1" hidden="1"/>
+    <col min="11775" max="12021" width="11.42578125" style="1" hidden="1"/>
+    <col min="12022" max="12022" width="15.42578125" style="1" hidden="1"/>
+    <col min="12023" max="12023" width="11.42578125" style="1" hidden="1"/>
+    <col min="12024" max="12024" width="15.7109375" style="1" hidden="1"/>
+    <col min="12025" max="12025" width="21.85546875" style="1" hidden="1"/>
+    <col min="12026" max="12028" width="11.42578125" style="1" hidden="1"/>
     <col min="12029" max="12029" width="16" style="1" hidden="1"/>
-    <col min="12030" max="12030" width="20.44140625" style="1" hidden="1"/>
-    <col min="12031" max="12277" width="11.44140625" style="1" hidden="1"/>
-    <col min="12278" max="12278" width="15.44140625" style="1" hidden="1"/>
-    <col min="12279" max="12279" width="11.44140625" style="1" hidden="1"/>
-    <col min="12280" max="12280" width="15.6640625" style="1" hidden="1"/>
-    <col min="12281" max="12281" width="21.88671875" style="1" hidden="1"/>
-    <col min="12282" max="12284" width="11.44140625" style="1" hidden="1"/>
+    <col min="12030" max="12030" width="20.42578125" style="1" hidden="1"/>
+    <col min="12031" max="12277" width="11.42578125" style="1" hidden="1"/>
+    <col min="12278" max="12278" width="15.42578125" style="1" hidden="1"/>
+    <col min="12279" max="12279" width="11.42578125" style="1" hidden="1"/>
+    <col min="12280" max="12280" width="15.7109375" style="1" hidden="1"/>
+    <col min="12281" max="12281" width="21.85546875" style="1" hidden="1"/>
+    <col min="12282" max="12284" width="11.42578125" style="1" hidden="1"/>
     <col min="12285" max="12285" width="16" style="1" hidden="1"/>
-    <col min="12286" max="12286" width="20.44140625" style="1" hidden="1"/>
-    <col min="12287" max="12533" width="11.44140625" style="1" hidden="1"/>
-    <col min="12534" max="12534" width="15.44140625" style="1" hidden="1"/>
-    <col min="12535" max="12535" width="11.44140625" style="1" hidden="1"/>
-    <col min="12536" max="12536" width="15.6640625" style="1" hidden="1"/>
-    <col min="12537" max="12537" width="21.88671875" style="1" hidden="1"/>
-    <col min="12538" max="12540" width="11.44140625" style="1" hidden="1"/>
+    <col min="12286" max="12286" width="20.42578125" style="1" hidden="1"/>
+    <col min="12287" max="12533" width="11.42578125" style="1" hidden="1"/>
+    <col min="12534" max="12534" width="15.42578125" style="1" hidden="1"/>
+    <col min="12535" max="12535" width="11.42578125" style="1" hidden="1"/>
+    <col min="12536" max="12536" width="15.7109375" style="1" hidden="1"/>
+    <col min="12537" max="12537" width="21.85546875" style="1" hidden="1"/>
+    <col min="12538" max="12540" width="11.42578125" style="1" hidden="1"/>
     <col min="12541" max="12541" width="16" style="1" hidden="1"/>
-    <col min="12542" max="12542" width="20.44140625" style="1" hidden="1"/>
-    <col min="12543" max="12789" width="11.44140625" style="1" hidden="1"/>
-    <col min="12790" max="12790" width="15.44140625" style="1" hidden="1"/>
-    <col min="12791" max="12791" width="11.44140625" style="1" hidden="1"/>
-    <col min="12792" max="12792" width="15.6640625" style="1" hidden="1"/>
-    <col min="12793" max="12793" width="21.88671875" style="1" hidden="1"/>
-    <col min="12794" max="12796" width="11.44140625" style="1" hidden="1"/>
+    <col min="12542" max="12542" width="20.42578125" style="1" hidden="1"/>
+    <col min="12543" max="12789" width="11.42578125" style="1" hidden="1"/>
+    <col min="12790" max="12790" width="15.42578125" style="1" hidden="1"/>
+    <col min="12791" max="12791" width="11.42578125" style="1" hidden="1"/>
+    <col min="12792" max="12792" width="15.7109375" style="1" hidden="1"/>
+    <col min="12793" max="12793" width="21.85546875" style="1" hidden="1"/>
+    <col min="12794" max="12796" width="11.42578125" style="1" hidden="1"/>
     <col min="12797" max="12797" width="16" style="1" hidden="1"/>
-    <col min="12798" max="12798" width="20.44140625" style="1" hidden="1"/>
-    <col min="12799" max="13045" width="11.44140625" style="1" hidden="1"/>
-    <col min="13046" max="13046" width="15.44140625" style="1" hidden="1"/>
-    <col min="13047" max="13047" width="11.44140625" style="1" hidden="1"/>
-    <col min="13048" max="13048" width="15.6640625" style="1" hidden="1"/>
-    <col min="13049" max="13049" width="21.88671875" style="1" hidden="1"/>
-    <col min="13050" max="13052" width="11.44140625" style="1" hidden="1"/>
+    <col min="12798" max="12798" width="20.42578125" style="1" hidden="1"/>
+    <col min="12799" max="13045" width="11.42578125" style="1" hidden="1"/>
+    <col min="13046" max="13046" width="15.42578125" style="1" hidden="1"/>
+    <col min="13047" max="13047" width="11.42578125" style="1" hidden="1"/>
+    <col min="13048" max="13048" width="15.7109375" style="1" hidden="1"/>
+    <col min="13049" max="13049" width="21.85546875" style="1" hidden="1"/>
+    <col min="13050" max="13052" width="11.42578125" style="1" hidden="1"/>
     <col min="13053" max="13053" width="16" style="1" hidden="1"/>
-    <col min="13054" max="13054" width="20.44140625" style="1" hidden="1"/>
-    <col min="13055" max="13301" width="11.44140625" style="1" hidden="1"/>
-    <col min="13302" max="13302" width="15.44140625" style="1" hidden="1"/>
-    <col min="13303" max="13303" width="11.44140625" style="1" hidden="1"/>
-    <col min="13304" max="13304" width="15.6640625" style="1" hidden="1"/>
-    <col min="13305" max="13305" width="21.88671875" style="1" hidden="1"/>
-    <col min="13306" max="13308" width="11.44140625" style="1" hidden="1"/>
+    <col min="13054" max="13054" width="20.42578125" style="1" hidden="1"/>
+    <col min="13055" max="13301" width="11.42578125" style="1" hidden="1"/>
+    <col min="13302" max="13302" width="15.42578125" style="1" hidden="1"/>
+    <col min="13303" max="13303" width="11.42578125" style="1" hidden="1"/>
+    <col min="13304" max="13304" width="15.7109375" style="1" hidden="1"/>
+    <col min="13305" max="13305" width="21.85546875" style="1" hidden="1"/>
+    <col min="13306" max="13308" width="11.42578125" style="1" hidden="1"/>
     <col min="13309" max="13309" width="16" style="1" hidden="1"/>
-    <col min="13310" max="13310" width="20.44140625" style="1" hidden="1"/>
-    <col min="13311" max="13557" width="11.44140625" style="1" hidden="1"/>
-    <col min="13558" max="13558" width="15.44140625" style="1" hidden="1"/>
-    <col min="13559" max="13559" width="11.44140625" style="1" hidden="1"/>
-    <col min="13560" max="13560" width="15.6640625" style="1" hidden="1"/>
-    <col min="13561" max="13561" width="21.88671875" style="1" hidden="1"/>
-    <col min="13562" max="13564" width="11.44140625" style="1" hidden="1"/>
+    <col min="13310" max="13310" width="20.42578125" style="1" hidden="1"/>
+    <col min="13311" max="13557" width="11.42578125" style="1" hidden="1"/>
+    <col min="13558" max="13558" width="15.42578125" style="1" hidden="1"/>
+    <col min="13559" max="13559" width="11.42578125" style="1" hidden="1"/>
+    <col min="13560" max="13560" width="15.7109375" style="1" hidden="1"/>
+    <col min="13561" max="13561" width="21.85546875" style="1" hidden="1"/>
+    <col min="13562" max="13564" width="11.42578125" style="1" hidden="1"/>
     <col min="13565" max="13565" width="16" style="1" hidden="1"/>
-    <col min="13566" max="13566" width="20.44140625" style="1" hidden="1"/>
-    <col min="13567" max="13813" width="11.44140625" style="1" hidden="1"/>
-    <col min="13814" max="13814" width="15.44140625" style="1" hidden="1"/>
-    <col min="13815" max="13815" width="11.44140625" style="1" hidden="1"/>
-    <col min="13816" max="13816" width="15.6640625" style="1" hidden="1"/>
-    <col min="13817" max="13817" width="21.88671875" style="1" hidden="1"/>
-    <col min="13818" max="13820" width="11.44140625" style="1" hidden="1"/>
+    <col min="13566" max="13566" width="20.42578125" style="1" hidden="1"/>
+    <col min="13567" max="13813" width="11.42578125" style="1" hidden="1"/>
+    <col min="13814" max="13814" width="15.42578125" style="1" hidden="1"/>
+    <col min="13815" max="13815" width="11.42578125" style="1" hidden="1"/>
+    <col min="13816" max="13816" width="15.7109375" style="1" hidden="1"/>
+    <col min="13817" max="13817" width="21.85546875" style="1" hidden="1"/>
+    <col min="13818" max="13820" width="11.42578125" style="1" hidden="1"/>
     <col min="13821" max="13821" width="16" style="1" hidden="1"/>
-    <col min="13822" max="13822" width="20.44140625" style="1" hidden="1"/>
-    <col min="13823" max="14069" width="11.44140625" style="1" hidden="1"/>
-    <col min="14070" max="14070" width="15.44140625" style="1" hidden="1"/>
-    <col min="14071" max="14071" width="11.44140625" style="1" hidden="1"/>
-    <col min="14072" max="14072" width="15.6640625" style="1" hidden="1"/>
-    <col min="14073" max="14073" width="21.88671875" style="1" hidden="1"/>
-    <col min="14074" max="14076" width="11.44140625" style="1" hidden="1"/>
+    <col min="13822" max="13822" width="20.42578125" style="1" hidden="1"/>
+    <col min="13823" max="14069" width="11.42578125" style="1" hidden="1"/>
+    <col min="14070" max="14070" width="15.42578125" style="1" hidden="1"/>
+    <col min="14071" max="14071" width="11.42578125" style="1" hidden="1"/>
+    <col min="14072" max="14072" width="15.7109375" style="1" hidden="1"/>
+    <col min="14073" max="14073" width="21.85546875" style="1" hidden="1"/>
+    <col min="14074" max="14076" width="11.42578125" style="1" hidden="1"/>
     <col min="14077" max="14077" width="16" style="1" hidden="1"/>
-    <col min="14078" max="14078" width="20.44140625" style="1" hidden="1"/>
-    <col min="14079" max="14325" width="11.44140625" style="1" hidden="1"/>
-    <col min="14326" max="14326" width="15.44140625" style="1" hidden="1"/>
-    <col min="14327" max="14327" width="11.44140625" style="1" hidden="1"/>
-    <col min="14328" max="14328" width="15.6640625" style="1" hidden="1"/>
-    <col min="14329" max="14329" width="21.88671875" style="1" hidden="1"/>
-    <col min="14330" max="14332" width="11.44140625" style="1" hidden="1"/>
+    <col min="14078" max="14078" width="20.42578125" style="1" hidden="1"/>
+    <col min="14079" max="14325" width="11.42578125" style="1" hidden="1"/>
+    <col min="14326" max="14326" width="15.42578125" style="1" hidden="1"/>
+    <col min="14327" max="14327" width="11.42578125" style="1" hidden="1"/>
+    <col min="14328" max="14328" width="15.7109375" style="1" hidden="1"/>
+    <col min="14329" max="14329" width="21.85546875" style="1" hidden="1"/>
+    <col min="14330" max="14332" width="11.42578125" style="1" hidden="1"/>
     <col min="14333" max="14333" width="16" style="1" hidden="1"/>
-    <col min="14334" max="14334" width="20.44140625" style="1" hidden="1"/>
-    <col min="14335" max="14581" width="11.44140625" style="1" hidden="1"/>
-    <col min="14582" max="14582" width="15.44140625" style="1" hidden="1"/>
-    <col min="14583" max="14583" width="11.44140625" style="1" hidden="1"/>
-    <col min="14584" max="14584" width="15.6640625" style="1" hidden="1"/>
-    <col min="14585" max="14585" width="21.88671875" style="1" hidden="1"/>
-    <col min="14586" max="14588" width="11.44140625" style="1" hidden="1"/>
+    <col min="14334" max="14334" width="20.42578125" style="1" hidden="1"/>
+    <col min="14335" max="14581" width="11.42578125" style="1" hidden="1"/>
+    <col min="14582" max="14582" width="15.42578125" style="1" hidden="1"/>
+    <col min="14583" max="14583" width="11.42578125" style="1" hidden="1"/>
+    <col min="14584" max="14584" width="15.7109375" style="1" hidden="1"/>
+    <col min="14585" max="14585" width="21.85546875" style="1" hidden="1"/>
+    <col min="14586" max="14588" width="11.42578125" style="1" hidden="1"/>
     <col min="14589" max="14589" width="16" style="1" hidden="1"/>
-    <col min="14590" max="14590" width="20.44140625" style="1" hidden="1"/>
-    <col min="14591" max="14837" width="11.44140625" style="1" hidden="1"/>
-    <col min="14838" max="14838" width="15.44140625" style="1" hidden="1"/>
-    <col min="14839" max="14839" width="11.44140625" style="1" hidden="1"/>
-    <col min="14840" max="14840" width="15.6640625" style="1" hidden="1"/>
-    <col min="14841" max="14841" width="21.88671875" style="1" hidden="1"/>
-    <col min="14842" max="14844" width="11.44140625" style="1" hidden="1"/>
+    <col min="14590" max="14590" width="20.42578125" style="1" hidden="1"/>
+    <col min="14591" max="14837" width="11.42578125" style="1" hidden="1"/>
+    <col min="14838" max="14838" width="15.42578125" style="1" hidden="1"/>
+    <col min="14839" max="14839" width="11.42578125" style="1" hidden="1"/>
+    <col min="14840" max="14840" width="15.7109375" style="1" hidden="1"/>
+    <col min="14841" max="14841" width="21.85546875" style="1" hidden="1"/>
+    <col min="14842" max="14844" width="11.42578125" style="1" hidden="1"/>
     <col min="14845" max="14845" width="16" style="1" hidden="1"/>
-    <col min="14846" max="14846" width="20.44140625" style="1" hidden="1"/>
-    <col min="14847" max="15093" width="11.44140625" style="1" hidden="1"/>
-    <col min="15094" max="15094" width="15.44140625" style="1" hidden="1"/>
-    <col min="15095" max="15095" width="11.44140625" style="1" hidden="1"/>
-    <col min="15096" max="15096" width="15.6640625" style="1" hidden="1"/>
-    <col min="15097" max="15097" width="21.88671875" style="1" hidden="1"/>
-    <col min="15098" max="15100" width="11.44140625" style="1" hidden="1"/>
+    <col min="14846" max="14846" width="20.42578125" style="1" hidden="1"/>
+    <col min="14847" max="15093" width="11.42578125" style="1" hidden="1"/>
+    <col min="15094" max="15094" width="15.42578125" style="1" hidden="1"/>
+    <col min="15095" max="15095" width="11.42578125" style="1" hidden="1"/>
+    <col min="15096" max="15096" width="15.7109375" style="1" hidden="1"/>
+    <col min="15097" max="15097" width="21.85546875" style="1" hidden="1"/>
+    <col min="15098" max="15100" width="11.42578125" style="1" hidden="1"/>
     <col min="15101" max="15101" width="16" style="1" hidden="1"/>
-    <col min="15102" max="15102" width="20.44140625" style="1" hidden="1"/>
-    <col min="15103" max="15349" width="11.44140625" style="1" hidden="1"/>
-    <col min="15350" max="15350" width="15.44140625" style="1" hidden="1"/>
-    <col min="15351" max="15351" width="11.44140625" style="1" hidden="1"/>
-    <col min="15352" max="15352" width="15.6640625" style="1" hidden="1"/>
-    <col min="15353" max="15353" width="21.88671875" style="1" hidden="1"/>
-    <col min="15354" max="15356" width="11.44140625" style="1" hidden="1"/>
+    <col min="15102" max="15102" width="20.42578125" style="1" hidden="1"/>
+    <col min="15103" max="15349" width="11.42578125" style="1" hidden="1"/>
+    <col min="15350" max="15350" width="15.42578125" style="1" hidden="1"/>
+    <col min="15351" max="15351" width="11.42578125" style="1" hidden="1"/>
+    <col min="15352" max="15352" width="15.7109375" style="1" hidden="1"/>
+    <col min="15353" max="15353" width="21.85546875" style="1" hidden="1"/>
+    <col min="15354" max="15356" width="11.42578125" style="1" hidden="1"/>
     <col min="15357" max="15357" width="16" style="1" hidden="1"/>
-    <col min="15358" max="15358" width="20.44140625" style="1" hidden="1"/>
-    <col min="15359" max="15605" width="11.44140625" style="1" hidden="1"/>
-    <col min="15606" max="15606" width="15.44140625" style="1" hidden="1"/>
-    <col min="15607" max="15607" width="11.44140625" style="1" hidden="1"/>
-    <col min="15608" max="15608" width="15.6640625" style="1" hidden="1"/>
-    <col min="15609" max="15609" width="21.88671875" style="1" hidden="1"/>
-    <col min="15610" max="15612" width="11.44140625" style="1" hidden="1"/>
+    <col min="15358" max="15358" width="20.42578125" style="1" hidden="1"/>
+    <col min="15359" max="15605" width="11.42578125" style="1" hidden="1"/>
+    <col min="15606" max="15606" width="15.42578125" style="1" hidden="1"/>
+    <col min="15607" max="15607" width="11.42578125" style="1" hidden="1"/>
+    <col min="15608" max="15608" width="15.7109375" style="1" hidden="1"/>
+    <col min="15609" max="15609" width="21.85546875" style="1" hidden="1"/>
+    <col min="15610" max="15612" width="11.42578125" style="1" hidden="1"/>
     <col min="15613" max="15613" width="16" style="1" hidden="1"/>
-    <col min="15614" max="15614" width="20.44140625" style="1" hidden="1"/>
-    <col min="15615" max="15861" width="11.44140625" style="1" hidden="1"/>
-    <col min="15862" max="15862" width="15.44140625" style="1" hidden="1"/>
-    <col min="15863" max="15863" width="11.44140625" style="1" hidden="1"/>
-    <col min="15864" max="15864" width="15.6640625" style="1" hidden="1"/>
-    <col min="15865" max="15865" width="21.88671875" style="1" hidden="1"/>
-    <col min="15866" max="15868" width="11.44140625" style="1" hidden="1"/>
+    <col min="15614" max="15614" width="20.42578125" style="1" hidden="1"/>
+    <col min="15615" max="15861" width="11.42578125" style="1" hidden="1"/>
+    <col min="15862" max="15862" width="15.42578125" style="1" hidden="1"/>
+    <col min="15863" max="15863" width="11.42578125" style="1" hidden="1"/>
+    <col min="15864" max="15864" width="15.7109375" style="1" hidden="1"/>
+    <col min="15865" max="15865" width="21.85546875" style="1" hidden="1"/>
+    <col min="15866" max="15868" width="11.42578125" style="1" hidden="1"/>
     <col min="15869" max="15869" width="16" style="1" hidden="1"/>
-    <col min="15870" max="15870" width="20.44140625" style="1" hidden="1"/>
-    <col min="15871" max="16117" width="11.44140625" style="1" hidden="1"/>
-    <col min="16118" max="16118" width="15.44140625" style="1" hidden="1"/>
-    <col min="16119" max="16119" width="11.44140625" style="1" hidden="1"/>
-    <col min="16120" max="16120" width="15.6640625" style="1" hidden="1"/>
-    <col min="16121" max="16121" width="21.88671875" style="1" hidden="1"/>
-    <col min="16122" max="16124" width="11.44140625" style="1" hidden="1"/>
+    <col min="15870" max="15870" width="20.42578125" style="1" hidden="1"/>
+    <col min="15871" max="16117" width="11.42578125" style="1" hidden="1"/>
+    <col min="16118" max="16118" width="15.42578125" style="1" hidden="1"/>
+    <col min="16119" max="16119" width="11.42578125" style="1" hidden="1"/>
+    <col min="16120" max="16120" width="15.7109375" style="1" hidden="1"/>
+    <col min="16121" max="16121" width="21.85546875" style="1" hidden="1"/>
+    <col min="16122" max="16124" width="11.42578125" style="1" hidden="1"/>
     <col min="16125" max="16125" width="16" style="1" hidden="1"/>
-    <col min="16126" max="16126" width="20.44140625" style="1" hidden="1"/>
-    <col min="16127" max="16129" width="11.44140625" style="1" hidden="1"/>
-    <col min="16130" max="16130" width="15.44140625" style="1" hidden="1"/>
-    <col min="16131" max="16131" width="11.44140625" style="1" hidden="1"/>
-    <col min="16132" max="16132" width="15.6640625" style="1" hidden="1"/>
-    <col min="16133" max="16133" width="21.88671875" style="1" hidden="1"/>
-    <col min="16134" max="16136" width="11.44140625" style="1" hidden="1"/>
+    <col min="16126" max="16126" width="20.42578125" style="1" hidden="1"/>
+    <col min="16127" max="16129" width="11.42578125" style="1" hidden="1"/>
+    <col min="16130" max="16130" width="15.42578125" style="1" hidden="1"/>
+    <col min="16131" max="16131" width="11.42578125" style="1" hidden="1"/>
+    <col min="16132" max="16132" width="15.7109375" style="1" hidden="1"/>
+    <col min="16133" max="16133" width="21.85546875" style="1" hidden="1"/>
+    <col min="16134" max="16136" width="11.42578125" style="1" hidden="1"/>
     <col min="16137" max="16137" width="16" style="1" hidden="1"/>
-    <col min="16138" max="16139" width="20.44140625" style="1" hidden="1"/>
-    <col min="16140" max="16141" width="11.44140625" style="1" hidden="1"/>
+    <col min="16138" max="16139" width="20.42578125" style="1" hidden="1"/>
+    <col min="16140" max="16141" width="11.42578125" style="1" hidden="1"/>
     <col min="16142" max="16142" width="16" style="1" hidden="1"/>
-    <col min="16143" max="16145" width="20.44140625" style="1" hidden="1"/>
-    <col min="16146" max="16384" width="11.44140625" style="1" hidden="1"/>
+    <col min="16143" max="16145" width="20.42578125" style="1" hidden="1"/>
+    <col min="16146" max="16384" width="11.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="str">
         <f>RAWDATA!B2</f>
         <v>applicant.last_name</v>
@@ -2573,7 +2573,7 @@
         <v>attendance.sanitized_grade</v>
       </c>
       <c r="F2" s="30" t="e">
-        <f>LOOKUP(E2,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E2,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>#N/A</v>
       </c>
       <c r="G2" s="4"/>
@@ -2620,7 +2620,7 @@
         <v>course.teacher_name</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <f>RAWDATA!B3</f>
         <v>0</v>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="30" t="str">
-        <f>LOOKUP(E3,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E3,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G3" s="4"/>
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <f>RAWDATA!B4</f>
         <v>0</v>
@@ -2711,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="30" t="str">
-        <f>LOOKUP(E4,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E4,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G4" s="4"/>
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="29">
         <f>RAWDATA!B5</f>
         <v>0</v>
@@ -2780,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="30" t="str">
-        <f>LOOKUP(E5,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E5,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G5" s="4"/>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="29">
         <f>RAWDATA!B6</f>
         <v>0</v>
@@ -2849,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="30" t="str">
-        <f>LOOKUP(E6,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E6,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G6" s="4"/>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <f>RAWDATA!B7</f>
         <v>0</v>
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="30" t="str">
-        <f>LOOKUP(E7,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E7,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G7" s="4"/>
@@ -2965,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="29">
         <f>RAWDATA!B8</f>
         <v>0</v>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="30" t="str">
-        <f>LOOKUP(E8,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E8,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G8" s="4"/>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="29">
         <f>RAWDATA!B9</f>
         <v>0</v>
@@ -3056,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="30" t="str">
-        <f>LOOKUP(E9,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E9,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G9" s="4"/>
@@ -3103,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="29">
         <f>RAWDATA!B10</f>
         <v>0</v>
@@ -3125,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="30" t="str">
-        <f>LOOKUP(E10,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E10,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G10" s="4"/>
@@ -3172,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="29">
         <f>RAWDATA!B11</f>
         <v>0</v>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="30" t="str">
-        <f>LOOKUP(E11,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E11,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G11" s="4"/>
@@ -3241,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <f>RAWDATA!B12</f>
         <v>0</v>
@@ -3263,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="30" t="str">
-        <f>LOOKUP(E12,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E12,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G12" s="4"/>
@@ -3310,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="29">
         <f>RAWDATA!B13</f>
         <v>0</v>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="30" t="str">
-        <f>LOOKUP(E13,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E13,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G13" s="4"/>
@@ -3379,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <f>RAWDATA!B14</f>
         <v>0</v>
@@ -3401,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="30" t="str">
-        <f>LOOKUP(E14,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E14,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G14" s="4"/>
@@ -3448,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="29">
         <f>RAWDATA!B15</f>
         <v>0</v>
@@ -3470,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="30" t="str">
-        <f>LOOKUP(E15,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E15,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G15" s="4"/>
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
         <f>RAWDATA!B16</f>
         <v>0</v>
@@ -3539,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="30" t="str">
-        <f>LOOKUP(E16,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E16,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G16" s="4"/>
@@ -3586,7 +3586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="29">
         <f>RAWDATA!B17</f>
         <v>0</v>
@@ -3608,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="30" t="str">
-        <f>LOOKUP(E17,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E17,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G17" s="4"/>
@@ -3655,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="29">
         <f>RAWDATA!B18</f>
         <v>0</v>
@@ -3677,7 +3677,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="30" t="str">
-        <f>LOOKUP(E18,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E18,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G18" s="4"/>
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="29">
         <f>RAWDATA!B19</f>
         <v>0</v>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="30" t="str">
-        <f>LOOKUP(E19,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E19,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G19" s="4"/>
@@ -3793,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="29">
         <f>RAWDATA!B20</f>
         <v>0</v>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="30" t="str">
-        <f>LOOKUP(E20,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E20,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G20" s="4"/>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <f>RAWDATA!B21</f>
         <v>0</v>
@@ -3884,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="30" t="str">
-        <f>LOOKUP(E21,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E21,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G21" s="4"/>
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <f>RAWDATA!B22</f>
         <v>0</v>
@@ -3953,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="30" t="str">
-        <f>LOOKUP(E22,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E22,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G22" s="4"/>
@@ -4000,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="29">
         <f>RAWDATA!B23</f>
         <v>0</v>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="30" t="str">
-        <f>LOOKUP(E23,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E23,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G23" s="4"/>
@@ -4069,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
         <f>RAWDATA!B24</f>
         <v>0</v>
@@ -4091,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="30" t="str">
-        <f>LOOKUP(E24,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E24,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G24" s="4"/>
@@ -4138,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
         <f>RAWDATA!B25</f>
         <v>0</v>
@@ -4160,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="30" t="str">
-        <f>LOOKUP(E25,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E25,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G25" s="4"/>
@@ -4190,7 +4190,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="11"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
         <f>RAWDATA!B26</f>
         <v>0</v>
@@ -4212,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="30" t="str">
-        <f>LOOKUP(E26,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E26,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G26" s="4"/>
@@ -4242,7 +4242,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="11"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="29">
         <f>RAWDATA!B27</f>
         <v>0</v>
@@ -4264,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="30" t="str">
-        <f>LOOKUP(E27,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E27,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G27" s="4"/>
@@ -4294,7 +4294,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="11"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <f>RAWDATA!B28</f>
         <v>0</v>
@@ -4316,7 +4316,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="30" t="str">
-        <f>LOOKUP(E28,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E28,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G28" s="4"/>
@@ -4346,7 +4346,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="11"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="29">
         <f>RAWDATA!B29</f>
         <v>0</v>
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="30" t="str">
-        <f>LOOKUP(E29,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E29,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G29" s="4"/>
@@ -4398,7 +4398,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="11"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <f>RAWDATA!B30</f>
         <v>0</v>
@@ -4420,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="30" t="str">
-        <f>LOOKUP(E30,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E30,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G30" s="4"/>
@@ -4450,7 +4450,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="11"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="29">
         <f>RAWDATA!B31</f>
         <v>0</v>
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="30" t="str">
-        <f>LOOKUP(E31,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E31,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G31" s="4"/>
@@ -4502,7 +4502,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="11"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <f>RAWDATA!B32</f>
         <v>0</v>
@@ -4524,7 +4524,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="30" t="str">
-        <f>LOOKUP(E32,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E32,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G32" s="4"/>
@@ -4554,7 +4554,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="11"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="29">
         <f>RAWDATA!B33</f>
         <v>0</v>
@@ -4576,7 +4576,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="30" t="str">
-        <f>LOOKUP(E33,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E33,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G33" s="4"/>
@@ -4606,7 +4606,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="11"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="29">
         <f>RAWDATA!B34</f>
         <v>0</v>
@@ -4628,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="30" t="str">
-        <f>LOOKUP(E34,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E34,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G34" s="4"/>
@@ -4658,7 +4658,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="11"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="29">
         <f>RAWDATA!B35</f>
         <v>0</v>
@@ -4680,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="30" t="str">
-        <f>LOOKUP(E35,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E35,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G35" s="4"/>
@@ -4727,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <f>RAWDATA!B36</f>
         <v>0</v>
@@ -4749,7 +4749,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="30" t="str">
-        <f>LOOKUP(E36,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E36,{0;1;49.1;55.1;61.1;67.1;72.1;78.1;84.1;89.1;94.1;97.1},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G36" s="4"/>
@@ -4796,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>10</v>
@@ -4816,7 +4816,7 @@
       <c r="M37" s="4"/>
       <c r="N37" s="22"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -4833,7 +4833,7 @@
       <c r="M38" s="4"/>
       <c r="N38" s="22"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
@@ -4854,7 +4854,7 @@
       <c r="M39" s="4"/>
       <c r="N39" s="22"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="22"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
@@ -4870,7 +4870,7 @@
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
@@ -4892,7 +4892,7 @@
       <c r="M41" s="31"/>
       <c r="N41" s="22"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
@@ -4912,7 +4912,7 @@
       <c r="M42" s="31"/>
       <c r="N42" s="22"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -4932,7 +4932,7 @@
       <c r="M43" s="31"/>
       <c r="N43" s="22"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -4952,7 +4952,7 @@
       <c r="M44" s="31"/>
       <c r="N44" s="22"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -4972,7 +4972,7 @@
       <c r="M45" s="31"/>
       <c r="N45" s="22"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>51</v>
       </c>
@@ -4992,7 +4992,7 @@
       <c r="M46" s="31"/>
       <c r="N46" s="22"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
@@ -5012,7 +5012,7 @@
       <c r="M47" s="31"/>
       <c r="N47" s="22"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>44</v>
       </c>
@@ -5032,55 +5032,55 @@
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
     </row>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="53"/>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="53"/>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="53"/>
     </row>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="53"/>
     </row>
-    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="53"/>
     </row>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="53"/>
     </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="53"/>
     </row>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="53"/>
     </row>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="53"/>
     </row>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="53"/>
     </row>
-    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="53"/>
     </row>
-    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="53"/>
     </row>
-    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="53"/>
     </row>
-    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="53"/>
     </row>
-    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="53"/>
     </row>
-    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="53"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
   <dataConsolidate/>
@@ -5088,7 +5088,7 @@
     <mergeCell ref="D41:G48"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Inkorrekte Semesterangabe" error="Bitte wählen Sie aus der Dropdown-Liste aus._x000a__x000a_Ihre Eingabe wird nicht automatisch korrigiert." promptTitle="Semester" prompt="Bitte geben Sie das entsprechende Semester an. Wählen Sie aus der Dropdown-Liste." sqref="B47" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Inkorrekte Semesterangabe" error="Bitte wählen Sie aus der Dropdown-Liste aus._x000a__x000a_Ihre Eingabe wird nicht automatisch korrigiert." promptTitle="Semester" prompt="Bitte geben Sie das entsprechende Semester an. Wählen Sie aus der Dropdown-Liste." sqref="B47"/>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.2598425196850394" bottom="1.0629921259842521" header="0.59055118110236227" footer="0.78740157480314965"/>
   <pageSetup paperSize="9" scale="82" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5101,7 +5101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5111,15 +5111,15 @@
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="7" customWidth="1"/>
-    <col min="3" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" hidden="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="7" customWidth="1"/>
+    <col min="3" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="str">
         <f>Notenliste!B44</f>
         <v>course.name</v>
@@ -5133,7 +5133,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1.3</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1.7</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>2.7</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>3.3</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3.7</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>4</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -5252,7 +5252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5262,22 +5262,22 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="14" width="8.6640625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" customWidth="1"/>
-    <col min="16" max="16" width="1.6640625" customWidth="1"/>
-    <col min="17" max="16384" width="11.44140625" hidden="1"/>
+    <col min="1" max="1" width="3.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" style="20" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="8.7109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="1.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="58" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="58" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>course.namecourse.alternative</v>
@@ -5297,7 +5297,7 @@
       <c r="N1" s="71"/>
       <c r="O1" s="71"/>
     </row>
-    <row r="2" spans="1:15" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
         <v>Dozent/in: course.teacher_name</v>
@@ -5320,7 +5320,7 @@
       <c r="N2" s="73"/>
       <c r="O2" s="73"/>
     </row>
-    <row r="3" spans="1:15" s="59" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="59" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>ATTENDANCE.TS_RECEIVED_STR</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>2</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>3</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>4</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>5</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>6</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>7</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>8</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>9</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>10</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>11</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>12</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>13</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>14</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>15</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>16</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>17</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>18</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>19</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>20</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>21</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>22</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>23</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>24</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>25</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>26</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>27</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>28</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>29</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>30</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>31</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>32</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>33</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>34</v>
       </c>
@@ -7441,7 +7441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>35</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="55"/>
       <c r="B39" s="56"/>
       <c r="C39" s="56"/>
@@ -7525,7 +7525,7 @@
       <c r="N39" s="55"/>
       <c r="O39" s="57"/>
     </row>
-    <row r="40" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="74" t="s">
         <v>42</v>
       </c>
@@ -7544,7 +7544,7 @@
       <c r="N40" s="74"/>
       <c r="O40" s="74"/>
     </row>
-    <row r="41" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="74"/>
       <c r="B41" s="74"/>
       <c r="C41" s="74"/>
@@ -7561,7 +7561,7 @@
       <c r="N41" s="74"/>
       <c r="O41" s="74"/>
     </row>
-    <row r="42" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="74"/>
       <c r="B42" s="74"/>
       <c r="C42" s="74"/>
@@ -7578,7 +7578,7 @@
       <c r="N42" s="74"/>
       <c r="O42" s="74"/>
     </row>
-    <row r="43" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="74"/>
       <c r="B43" s="74"/>
       <c r="C43" s="74"/>
@@ -7595,7 +7595,7 @@
       <c r="N43" s="74"/>
       <c r="O43" s="74"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="74"/>
       <c r="B44" s="74"/>
       <c r="C44" s="74"/>
@@ -7632,7 +7632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7642,24 +7642,24 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="0.88671875" style="20" customWidth="1"/>
-    <col min="7" max="20" width="7.6640625" style="20" customWidth="1"/>
-    <col min="21" max="21" width="0.88671875" style="20" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" style="51" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" style="52" customWidth="1"/>
-    <col min="24" max="24" width="10.6640625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="20" customWidth="1"/>
+    <col min="6" max="6" width="0.85546875" style="20" customWidth="1"/>
+    <col min="7" max="20" width="7.7109375" style="20" customWidth="1"/>
+    <col min="21" max="21" width="0.85546875" style="20" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="51" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" style="52" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="39" customWidth="1"/>
     <col min="25" max="31" width="0" hidden="1" customWidth="1"/>
-    <col min="32" max="16384" width="11.44140625" hidden="1"/>
+    <col min="32" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>course.namecourse.alternative</v>
@@ -7688,7 +7688,7 @@
       <c r="W1" s="77"/>
       <c r="X1" s="77"/>
     </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>40</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="W2" s="77"/>
       <c r="X2" s="77"/>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="78" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
         <v>Dozent/in: course.teacher_name</v>
@@ -7745,7 +7745,7 @@
       <c r="W3" s="79"/>
       <c r="X3" s="79"/>
     </row>
-    <row r="4" spans="1:24" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="80" t="s">
         <v>26</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="81"/>
       <c r="B5" s="81"/>
       <c r="C5" s="81"/>
@@ -7841,7 +7841,7 @@
       <c r="W5" s="76"/>
       <c r="X5" s="76"/>
     </row>
-    <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -7881,7 +7881,7 @@
       <c r="W6" s="50"/>
       <c r="X6" s="50"/>
     </row>
-    <row r="7" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>2</v>
       </c>
@@ -7921,7 +7921,7 @@
       <c r="W7" s="50"/>
       <c r="X7" s="50"/>
     </row>
-    <row r="8" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>3</v>
       </c>
@@ -7961,7 +7961,7 @@
       <c r="W8" s="50"/>
       <c r="X8" s="50"/>
     </row>
-    <row r="9" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>4</v>
       </c>
@@ -8001,7 +8001,7 @@
       <c r="W9" s="50"/>
       <c r="X9" s="50"/>
     </row>
-    <row r="10" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>5</v>
       </c>
@@ -8041,7 +8041,7 @@
       <c r="W10" s="50"/>
       <c r="X10" s="50"/>
     </row>
-    <row r="11" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>6</v>
       </c>
@@ -8081,7 +8081,7 @@
       <c r="W11" s="50"/>
       <c r="X11" s="50"/>
     </row>
-    <row r="12" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>7</v>
       </c>
@@ -8121,7 +8121,7 @@
       <c r="W12" s="50"/>
       <c r="X12" s="50"/>
     </row>
-    <row r="13" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>8</v>
       </c>
@@ -8161,7 +8161,7 @@
       <c r="W13" s="50"/>
       <c r="X13" s="50"/>
     </row>
-    <row r="14" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>9</v>
       </c>
@@ -8201,7 +8201,7 @@
       <c r="W14" s="50"/>
       <c r="X14" s="50"/>
     </row>
-    <row r="15" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>10</v>
       </c>
@@ -8241,7 +8241,7 @@
       <c r="W15" s="50"/>
       <c r="X15" s="50"/>
     </row>
-    <row r="16" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>11</v>
       </c>
@@ -8281,7 +8281,7 @@
       <c r="W16" s="50"/>
       <c r="X16" s="50"/>
     </row>
-    <row r="17" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>12</v>
       </c>
@@ -8321,7 +8321,7 @@
       <c r="W17" s="50"/>
       <c r="X17" s="50"/>
     </row>
-    <row r="18" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>13</v>
       </c>
@@ -8361,7 +8361,7 @@
       <c r="W18" s="50"/>
       <c r="X18" s="50"/>
     </row>
-    <row r="19" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>14</v>
       </c>
@@ -8401,7 +8401,7 @@
       <c r="W19" s="50"/>
       <c r="X19" s="50"/>
     </row>
-    <row r="20" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>15</v>
       </c>
@@ -8441,7 +8441,7 @@
       <c r="W20" s="50"/>
       <c r="X20" s="50"/>
     </row>
-    <row r="21" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>16</v>
       </c>
@@ -8481,7 +8481,7 @@
       <c r="W21" s="50"/>
       <c r="X21" s="50"/>
     </row>
-    <row r="22" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>17</v>
       </c>
@@ -8521,7 +8521,7 @@
       <c r="W22" s="50"/>
       <c r="X22" s="50"/>
     </row>
-    <row r="23" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>18</v>
       </c>
@@ -8561,7 +8561,7 @@
       <c r="W23" s="50"/>
       <c r="X23" s="50"/>
     </row>
-    <row r="24" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>19</v>
       </c>
@@ -8601,7 +8601,7 @@
       <c r="W24" s="50"/>
       <c r="X24" s="50"/>
     </row>
-    <row r="25" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>20</v>
       </c>
@@ -8641,7 +8641,7 @@
       <c r="W25" s="50"/>
       <c r="X25" s="50"/>
     </row>
-    <row r="26" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>21</v>
       </c>
@@ -8681,7 +8681,7 @@
       <c r="W26" s="50"/>
       <c r="X26" s="50"/>
     </row>
-    <row r="27" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>22</v>
       </c>
@@ -8721,7 +8721,7 @@
       <c r="W27" s="50"/>
       <c r="X27" s="50"/>
     </row>
-    <row r="28" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>23</v>
       </c>
@@ -8761,7 +8761,7 @@
       <c r="W28" s="50"/>
       <c r="X28" s="50"/>
     </row>
-    <row r="29" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>24</v>
       </c>
@@ -8801,7 +8801,7 @@
       <c r="W29" s="50"/>
       <c r="X29" s="50"/>
     </row>
-    <row r="30" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>25</v>
       </c>
@@ -8841,7 +8841,7 @@
       <c r="W30" s="50"/>
       <c r="X30" s="50"/>
     </row>
-    <row r="31" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>26</v>
       </c>
@@ -8881,7 +8881,7 @@
       <c r="W31" s="50"/>
       <c r="X31" s="50"/>
     </row>
-    <row r="32" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>27</v>
       </c>
@@ -8921,7 +8921,7 @@
       <c r="W32" s="50"/>
       <c r="X32" s="50"/>
     </row>
-    <row r="33" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>28</v>
       </c>
@@ -8961,7 +8961,7 @@
       <c r="W33" s="50"/>
       <c r="X33" s="50"/>
     </row>
-    <row r="34" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>29</v>
       </c>
@@ -9001,7 +9001,7 @@
       <c r="W34" s="50"/>
       <c r="X34" s="50"/>
     </row>
-    <row r="35" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>30</v>
       </c>
@@ -9041,7 +9041,7 @@
       <c r="W35" s="50"/>
       <c r="X35" s="50"/>
     </row>
-    <row r="36" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>31</v>
       </c>
@@ -9081,7 +9081,7 @@
       <c r="W36" s="50"/>
       <c r="X36" s="50"/>
     </row>
-    <row r="37" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>32</v>
       </c>
@@ -9121,7 +9121,7 @@
       <c r="W37" s="50"/>
       <c r="X37" s="50"/>
     </row>
-    <row r="38" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>33</v>
       </c>
@@ -9161,7 +9161,7 @@
       <c r="W38" s="50"/>
       <c r="X38" s="50"/>
     </row>
-    <row r="39" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>34</v>
       </c>
@@ -9201,7 +9201,7 @@
       <c r="W39" s="50"/>
       <c r="X39" s="50"/>
     </row>
-    <row r="40" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>35</v>
       </c>
@@ -9268,25 +9268,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="61" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="64" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" style="63" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="64" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="63" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>27</v>
       </c>
@@ -9312,7 +9312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="str">
         <f>IF(Notenliste!D2=0," ",Notenliste!D2)</f>
         <v>applicant.tag</v>
@@ -9334,7 +9334,7 @@
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="str">
         <f>IF(Notenliste!D3=0," ",Notenliste!D3)</f>
         <v xml:space="preserve"> </v>
@@ -9356,7 +9356,7 @@
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="str">
         <f>IF(Notenliste!D4=0," ",Notenliste!D4)</f>
         <v xml:space="preserve"> </v>
@@ -9378,7 +9378,7 @@
       <c r="G4" s="39"/>
       <c r="H4" s="39"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="str">
         <f>IF(Notenliste!D5=0," ",Notenliste!D5)</f>
         <v xml:space="preserve"> </v>
@@ -9400,7 +9400,7 @@
       <c r="G5" s="39"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="str">
         <f>IF(Notenliste!D6=0," ",Notenliste!D6)</f>
         <v xml:space="preserve"> </v>
@@ -9422,7 +9422,7 @@
       <c r="G6" s="39"/>
       <c r="H6" s="39"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="str">
         <f>IF(Notenliste!D7=0," ",Notenliste!D7)</f>
         <v xml:space="preserve"> </v>
@@ -9444,7 +9444,7 @@
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="str">
         <f>IF(Notenliste!D8=0," ",Notenliste!D8)</f>
         <v xml:space="preserve"> </v>
@@ -9466,7 +9466,7 @@
       <c r="G8" s="39"/>
       <c r="H8" s="39"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="str">
         <f>IF(Notenliste!D9=0," ",Notenliste!D9)</f>
         <v xml:space="preserve"> </v>
@@ -9488,7 +9488,7 @@
       <c r="G9" s="39"/>
       <c r="H9" s="39"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="str">
         <f>IF(Notenliste!D10=0," ",Notenliste!D10)</f>
         <v xml:space="preserve"> </v>
@@ -9510,7 +9510,7 @@
       <c r="G10" s="39"/>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="str">
         <f>IF(Notenliste!D11=0," ",Notenliste!D11)</f>
         <v xml:space="preserve"> </v>
@@ -9532,7 +9532,7 @@
       <c r="G11" s="39"/>
       <c r="H11" s="39"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="str">
         <f>IF(Notenliste!D12=0," ",Notenliste!D12)</f>
         <v xml:space="preserve"> </v>
@@ -9554,7 +9554,7 @@
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="str">
         <f>IF(Notenliste!D13=0," ",Notenliste!D13)</f>
         <v xml:space="preserve"> </v>
@@ -9576,7 +9576,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="str">
         <f>IF(Notenliste!D14=0," ",Notenliste!D14)</f>
         <v xml:space="preserve"> </v>
@@ -9598,7 +9598,7 @@
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="str">
         <f>IF(Notenliste!D15=0," ",Notenliste!D15)</f>
         <v xml:space="preserve"> </v>
@@ -9620,7 +9620,7 @@
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="str">
         <f>IF(Notenliste!D16=0," ",Notenliste!D16)</f>
         <v xml:space="preserve"> </v>
@@ -9642,7 +9642,7 @@
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="str">
         <f>IF(Notenliste!D17=0," ",Notenliste!D17)</f>
         <v xml:space="preserve"> </v>
@@ -9664,7 +9664,7 @@
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="str">
         <f>IF(Notenliste!D18=0," ",Notenliste!D18)</f>
         <v xml:space="preserve"> </v>
@@ -9686,7 +9686,7 @@
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="str">
         <f>IF(Notenliste!D19=0," ",Notenliste!D19)</f>
         <v xml:space="preserve"> </v>
@@ -9708,7 +9708,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="str">
         <f>IF(Notenliste!D20=0," ",Notenliste!D20)</f>
         <v xml:space="preserve"> </v>
@@ -9730,7 +9730,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="str">
         <f>IF(Notenliste!D21=0," ",Notenliste!D21)</f>
         <v xml:space="preserve"> </v>
@@ -9752,7 +9752,7 @@
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="str">
         <f>IF(Notenliste!D22=0," ",Notenliste!D22)</f>
         <v xml:space="preserve"> </v>
@@ -9774,7 +9774,7 @@
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="str">
         <f>IF(Notenliste!D23=0," ",Notenliste!D23)</f>
         <v xml:space="preserve"> </v>
@@ -9796,7 +9796,7 @@
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="str">
         <f>IF(Notenliste!D24=0," ",Notenliste!D24)</f>
         <v xml:space="preserve"> </v>
@@ -9818,7 +9818,7 @@
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="str">
         <f>IF(Notenliste!D25=0," ",Notenliste!D25)</f>
         <v xml:space="preserve"> </v>
@@ -9840,7 +9840,7 @@
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="str">
         <f>IF(Notenliste!D26=0," ",Notenliste!D26)</f>
         <v xml:space="preserve"> </v>
@@ -9862,7 +9862,7 @@
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="str">
         <f>IF(Notenliste!D27=0," ",Notenliste!D27)</f>
         <v xml:space="preserve"> </v>
@@ -9884,7 +9884,7 @@
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="str">
         <f>IF(Notenliste!D28=0," ",Notenliste!D28)</f>
         <v xml:space="preserve"> </v>
@@ -9906,7 +9906,7 @@
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="str">
         <f>IF(Notenliste!D29=0," ",Notenliste!D29)</f>
         <v xml:space="preserve"> </v>
@@ -9928,7 +9928,7 @@
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="str">
         <f>IF(Notenliste!D30=0," ",Notenliste!D30)</f>
         <v xml:space="preserve"> </v>
@@ -9950,7 +9950,7 @@
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="str">
         <f>IF(Notenliste!D31=0," ",Notenliste!D31)</f>
         <v xml:space="preserve"> </v>
@@ -9972,7 +9972,7 @@
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="str">
         <f>IF(Notenliste!D32=0," ",Notenliste!D32)</f>
         <v xml:space="preserve"> </v>
@@ -9994,7 +9994,7 @@
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="str">
         <f>IF(Notenliste!D33=0," ",Notenliste!D33)</f>
         <v xml:space="preserve"> </v>
@@ -10016,7 +10016,7 @@
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="str">
         <f>IF(Notenliste!D34=0," ",Notenliste!D34)</f>
         <v xml:space="preserve"> </v>
@@ -10038,7 +10038,7 @@
       <c r="G34" s="39"/>
       <c r="H34" s="39"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="str">
         <f>IF(Notenliste!D35=0," ",Notenliste!D35)</f>
         <v xml:space="preserve"> </v>
@@ -10060,7 +10060,7 @@
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="str">
         <f>IF(Notenliste!D36=0," ",Notenliste!D36)</f>
         <v xml:space="preserve"> </v>
@@ -10085,21 +10085,21 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>Anmeldestatus</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
       <formula1>Notenskala</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C37:C1048576" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C37:C1048576">
       <formula1>0</formula1>
       <formula2>120</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E37:E1048576" xr:uid="{00000000-0002-0000-0500-000003000000}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E37:E1048576">
       <formula1>41275</formula1>
       <formula2>73050</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A37:A1048576" xr:uid="{00000000-0002-0000-0500-000004000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A37:A1048576">
       <formula1>0</formula1>
       <formula2>99999999</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
minor excel template fixes
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\04_Hiwi\Datenbank\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F55AA-8EE0-426B-832A-006AB6693407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612F0BE7-A944-47C3-B92C-22AF17486DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,IF(Notenliste!I2&lt;&gt;0,Notenliste!I2,Notenliste!$B$33)," ")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Note" dataDxfId="5" totalsRowDxfId="4">
-      <calculatedColumnFormula>IF(OR(Notenliste!H2="x", Notenliste!H2="X"),"bestanden",IF(Notenliste!D2=0," ",IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2))))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Notenliste!D2=0," ",IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",IF(OR(Notenliste!H2="x", Notenliste!H2="X"),"bestanden",Notenliste!F2))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Datum" dataDxfId="3">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$48," ")</calculatedColumnFormula>
@@ -1956,7 +1956,7 @@
   <dimension ref="A1:WVY71"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5259,8 +5259,8 @@
   </sheetPr>
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView showZeros="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -5409,27 +5409,27 @@
         <v>0</v>
       </c>
       <c r="J4" s="17" t="str">
-        <f>IF(Notenliste!J2=0," ",UPPER(Notenliste!J2))</f>
+        <f>IF(AND(B4=0,E4=0)," ",IF(Notenliste!J2=0," ",UPPER(Notenliste!J2)))</f>
         <v>ATTENDANCE.TS_REQUESTED_STR</v>
       </c>
-      <c r="K4" s="17" t="str">
-        <f>Notenliste!I2</f>
-        <v>attendance.ects_points</v>
+      <c r="K4" s="17" t="e">
+        <f>IF(AND(B4=0,E4=0)," ",IF(Notenliste!F2="KP","",Notenliste!I2))</f>
+        <v>#N/A</v>
       </c>
       <c r="L4" s="17" t="e">
         <f>IF(OR(M4&lt;=4, M4="bestanden"),"X","")</f>
         <v>#N/A</v>
       </c>
       <c r="M4" s="17" t="e">
-        <f>IF(OR(Notenliste!H2="x", Notenliste!H2="X"), "bestanden",IF(Notenliste!F2="KP"," ",Notenliste!F2))</f>
+        <f>IF(AND(B4=0,E4=0),"",IF(Notenliste!F2="KP","",IF(OR(Notenliste!H2="x", Notenliste!H2="X"), "bestanden",Notenliste!F2)))</f>
         <v>#N/A</v>
       </c>
       <c r="N4" s="17" t="str">
-        <f>Notenliste!E2</f>
+        <f>IF(AND(B4=0,E4=0)," ",Notenliste!E2)</f>
         <v>attendance.sanitized_grade</v>
       </c>
       <c r="O4" s="19" t="str">
-        <f>IF(Notenliste!L2=0," ",UPPER(Notenliste!L2))</f>
+        <f>IF(AND(B4=0,E4=0)," ",IF(Notenliste!L2=0," ",UPPER(Notenliste!L2)))</f>
         <v>ATTENDANCE.TS_RECEIVED_STR</v>
       </c>
     </row>
@@ -5470,27 +5470,27 @@
         <v>0</v>
       </c>
       <c r="J5" s="17" t="str">
-        <f>IF(Notenliste!J3=0," ",UPPER(Notenliste!J3))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K5" s="17">
-        <f>Notenliste!I3</f>
-        <v>0</v>
+        <f>IF(AND(B5=0,E5=0)," ",IF(Notenliste!J3=0," ",UPPER(Notenliste!J3)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K5" s="17" t="str">
+        <f>IF(AND(B5=0,E5=0)," ",IF(Notenliste!F3="KP","",Notenliste!I3))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L5" s="17" t="str">
         <f t="shared" ref="L5:L38" si="0">IF(OR(M5&lt;=4, M5="bestanden"),"X","")</f>
         <v/>
       </c>
       <c r="M5" s="17" t="str">
-        <f>IF(OR(Notenliste!H3="x", Notenliste!H3="X"), "bestanden",IF(Notenliste!F3="KP"," ",Notenliste!F3))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N5" s="17">
-        <f>Notenliste!E3</f>
-        <v>0</v>
+        <f>IF(AND(B5=0,E5=0),"",IF(Notenliste!F3="KP","",IF(OR(Notenliste!H3="x", Notenliste!H3="X"), "bestanden",Notenliste!F3)))</f>
+        <v/>
+      </c>
+      <c r="N5" s="17" t="str">
+        <f>IF(AND(B5=0,E5=0)," ",Notenliste!E3)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O5" s="19" t="str">
-        <f>IF(Notenliste!L3=0," ",UPPER(Notenliste!L3))</f>
+        <f>IF(AND(B5=0,E5=0)," ",IF(Notenliste!L3=0," ",UPPER(Notenliste!L3)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5531,27 +5531,27 @@
         <v>0</v>
       </c>
       <c r="J6" s="17" t="str">
-        <f>IF(Notenliste!J4=0," ",UPPER(Notenliste!J4))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K6" s="17">
-        <f>Notenliste!I4</f>
-        <v>0</v>
+        <f>IF(AND(B6=0,E6=0)," ",IF(Notenliste!J4=0," ",UPPER(Notenliste!J4)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K6" s="17" t="str">
+        <f>IF(AND(B6=0,E6=0)," ",IF(Notenliste!F4="KP","",Notenliste!I4))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L6" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M6" s="17" t="str">
-        <f>IF(OR(Notenliste!H4="x", Notenliste!H4="X"), "bestanden",IF(Notenliste!F4="KP"," ",Notenliste!F4))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N6" s="17">
-        <f>Notenliste!E4</f>
-        <v>0</v>
+        <f>IF(AND(B6=0,E6=0),"",IF(Notenliste!F4="KP","",IF(OR(Notenliste!H4="x", Notenliste!H4="X"), "bestanden",Notenliste!F4)))</f>
+        <v/>
+      </c>
+      <c r="N6" s="17" t="str">
+        <f>IF(AND(B6=0,E6=0)," ",Notenliste!E4)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O6" s="19" t="str">
-        <f>IF(Notenliste!L4=0," ",UPPER(Notenliste!L4))</f>
+        <f>IF(AND(B6=0,E6=0)," ",IF(Notenliste!L4=0," ",UPPER(Notenliste!L4)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5592,27 +5592,27 @@
         <v>0</v>
       </c>
       <c r="J7" s="17" t="str">
-        <f>IF(Notenliste!J5=0," ",UPPER(Notenliste!J5))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K7" s="17">
-        <f>Notenliste!I5</f>
-        <v>0</v>
+        <f>IF(AND(B7=0,E7=0)," ",IF(Notenliste!J5=0," ",UPPER(Notenliste!J5)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K7" s="17" t="str">
+        <f>IF(AND(B7=0,E7=0)," ",IF(Notenliste!F5="KP","",Notenliste!I5))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L7" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M7" s="17" t="str">
-        <f>IF(OR(Notenliste!H5="x", Notenliste!H5="X"), "bestanden",IF(Notenliste!F5="KP"," ",Notenliste!F5))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N7" s="17">
-        <f>Notenliste!E5</f>
-        <v>0</v>
+        <f>IF(AND(B7=0,E7=0),"",IF(Notenliste!F5="KP","",IF(OR(Notenliste!H5="x", Notenliste!H5="X"), "bestanden",Notenliste!F5)))</f>
+        <v/>
+      </c>
+      <c r="N7" s="17" t="str">
+        <f>IF(AND(B7=0,E7=0)," ",Notenliste!E5)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O7" s="19" t="str">
-        <f>IF(Notenliste!L5=0," ",UPPER(Notenliste!L5))</f>
+        <f>IF(AND(B7=0,E7=0)," ",IF(Notenliste!L5=0," ",UPPER(Notenliste!L5)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5653,27 +5653,27 @@
         <v>0</v>
       </c>
       <c r="J8" s="17" t="str">
-        <f>IF(Notenliste!J6=0," ",UPPER(Notenliste!J6))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K8" s="17">
-        <f>Notenliste!I6</f>
-        <v>0</v>
+        <f>IF(AND(B8=0,E8=0)," ",IF(Notenliste!J6=0," ",UPPER(Notenliste!J6)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K8" s="17" t="str">
+        <f>IF(AND(B8=0,E8=0)," ",IF(Notenliste!F6="KP","",Notenliste!I6))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L8" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M8" s="17" t="str">
-        <f>IF(OR(Notenliste!H6="x", Notenliste!H6="X"), "bestanden",IF(Notenliste!F6="KP"," ",Notenliste!F6))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N8" s="17">
-        <f>Notenliste!E6</f>
-        <v>0</v>
+        <f>IF(AND(B8=0,E8=0),"",IF(Notenliste!F6="KP","",IF(OR(Notenliste!H6="x", Notenliste!H6="X"), "bestanden",Notenliste!F6)))</f>
+        <v/>
+      </c>
+      <c r="N8" s="17" t="str">
+        <f>IF(AND(B8=0,E8=0)," ",Notenliste!E6)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O8" s="19" t="str">
-        <f>IF(Notenliste!L6=0," ",UPPER(Notenliste!L6))</f>
+        <f>IF(AND(B8=0,E8=0)," ",IF(Notenliste!L6=0," ",UPPER(Notenliste!L6)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5714,27 +5714,27 @@
         <v>0</v>
       </c>
       <c r="J9" s="17" t="str">
-        <f>IF(Notenliste!J7=0," ",UPPER(Notenliste!J7))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K9" s="17">
-        <f>Notenliste!I7</f>
-        <v>0</v>
+        <f>IF(AND(B9=0,E9=0)," ",IF(Notenliste!J7=0," ",UPPER(Notenliste!J7)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K9" s="17" t="str">
+        <f>IF(AND(B9=0,E9=0)," ",IF(Notenliste!F7="KP","",Notenliste!I7))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L9" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M9" s="17" t="str">
-        <f>IF(OR(Notenliste!H7="x", Notenliste!H7="X"), "bestanden",IF(Notenliste!F7="KP"," ",Notenliste!F7))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N9" s="17">
-        <f>Notenliste!E7</f>
-        <v>0</v>
+        <f>IF(AND(B9=0,E9=0),"",IF(Notenliste!F7="KP","",IF(OR(Notenliste!H7="x", Notenliste!H7="X"), "bestanden",Notenliste!F7)))</f>
+        <v/>
+      </c>
+      <c r="N9" s="17" t="str">
+        <f>IF(AND(B9=0,E9=0)," ",Notenliste!E7)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O9" s="19" t="str">
-        <f>IF(Notenliste!L7=0," ",UPPER(Notenliste!L7))</f>
+        <f>IF(AND(B9=0,E9=0)," ",IF(Notenliste!L7=0," ",UPPER(Notenliste!L7)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5775,27 +5775,27 @@
         <v>0</v>
       </c>
       <c r="J10" s="17" t="str">
-        <f>IF(Notenliste!J8=0," ",UPPER(Notenliste!J8))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K10" s="17">
-        <f>Notenliste!I8</f>
-        <v>0</v>
+        <f>IF(AND(B10=0,E10=0)," ",IF(Notenliste!J8=0," ",UPPER(Notenliste!J8)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K10" s="17" t="str">
+        <f>IF(AND(B10=0,E10=0)," ",IF(Notenliste!F8="KP","",Notenliste!I8))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L10" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M10" s="17" t="str">
-        <f>IF(OR(Notenliste!H8="x", Notenliste!H8="X"), "bestanden",IF(Notenliste!F8="KP"," ",Notenliste!F8))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N10" s="17">
-        <f>Notenliste!E8</f>
-        <v>0</v>
+        <f>IF(AND(B10=0,E10=0),"",IF(Notenliste!F8="KP","",IF(OR(Notenliste!H8="x", Notenliste!H8="X"), "bestanden",Notenliste!F8)))</f>
+        <v/>
+      </c>
+      <c r="N10" s="17" t="str">
+        <f>IF(AND(B10=0,E10=0)," ",Notenliste!E8)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O10" s="19" t="str">
-        <f>IF(Notenliste!L8=0," ",UPPER(Notenliste!L8))</f>
+        <f>IF(AND(B10=0,E10=0)," ",IF(Notenliste!L8=0," ",UPPER(Notenliste!L8)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5836,27 +5836,27 @@
         <v>0</v>
       </c>
       <c r="J11" s="17" t="str">
-        <f>IF(Notenliste!J9=0," ",UPPER(Notenliste!J9))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K11" s="17">
-        <f>Notenliste!I9</f>
-        <v>0</v>
+        <f>IF(AND(B11=0,E11=0)," ",IF(Notenliste!J9=0," ",UPPER(Notenliste!J9)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K11" s="17" t="str">
+        <f>IF(AND(B11=0,E11=0)," ",IF(Notenliste!F9="KP","",Notenliste!I9))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L11" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M11" s="17" t="str">
-        <f>IF(OR(Notenliste!H9="x", Notenliste!H9="X"), "bestanden",IF(Notenliste!F9="KP"," ",Notenliste!F9))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N11" s="17">
-        <f>Notenliste!E9</f>
-        <v>0</v>
+        <f>IF(AND(B11=0,E11=0),"",IF(Notenliste!F9="KP","",IF(OR(Notenliste!H9="x", Notenliste!H9="X"), "bestanden",Notenliste!F9)))</f>
+        <v/>
+      </c>
+      <c r="N11" s="17" t="str">
+        <f>IF(AND(B11=0,E11=0)," ",Notenliste!E9)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O11" s="19" t="str">
-        <f>IF(Notenliste!L9=0," ",UPPER(Notenliste!L9))</f>
+        <f>IF(AND(B11=0,E11=0)," ",IF(Notenliste!L9=0," ",UPPER(Notenliste!L9)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5897,27 +5897,27 @@
         <v>0</v>
       </c>
       <c r="J12" s="17" t="str">
-        <f>IF(Notenliste!J10=0," ",UPPER(Notenliste!J10))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K12" s="17">
-        <f>Notenliste!I10</f>
-        <v>0</v>
+        <f>IF(AND(B12=0,E12=0)," ",IF(Notenliste!J10=0," ",UPPER(Notenliste!J10)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K12" s="17" t="str">
+        <f>IF(AND(B12=0,E12=0)," ",IF(Notenliste!F10="KP","",Notenliste!I10))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L12" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M12" s="17" t="str">
-        <f>IF(OR(Notenliste!H10="x", Notenliste!H10="X"), "bestanden",IF(Notenliste!F10="KP"," ",Notenliste!F10))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N12" s="17">
-        <f>Notenliste!E10</f>
-        <v>0</v>
+        <f>IF(AND(B12=0,E12=0),"",IF(Notenliste!F10="KP","",IF(OR(Notenliste!H10="x", Notenliste!H10="X"), "bestanden",Notenliste!F10)))</f>
+        <v/>
+      </c>
+      <c r="N12" s="17" t="str">
+        <f>IF(AND(B12=0,E12=0)," ",Notenliste!E10)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O12" s="19" t="str">
-        <f>IF(Notenliste!L10=0," ",UPPER(Notenliste!L10))</f>
+        <f>IF(AND(B12=0,E12=0)," ",IF(Notenliste!L10=0," ",UPPER(Notenliste!L10)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5958,27 +5958,27 @@
         <v>0</v>
       </c>
       <c r="J13" s="17" t="str">
-        <f>IF(Notenliste!J11=0," ",UPPER(Notenliste!J11))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K13" s="17">
-        <f>Notenliste!I11</f>
-        <v>0</v>
+        <f>IF(AND(B13=0,E13=0)," ",IF(Notenliste!J11=0," ",UPPER(Notenliste!J11)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K13" s="17" t="str">
+        <f>IF(AND(B13=0,E13=0)," ",IF(Notenliste!F11="KP","",Notenliste!I11))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L13" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M13" s="17" t="str">
-        <f>IF(OR(Notenliste!H11="x", Notenliste!H11="X"), "bestanden",IF(Notenliste!F11="KP"," ",Notenliste!F11))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N13" s="17">
-        <f>Notenliste!E11</f>
-        <v>0</v>
+        <f>IF(AND(B13=0,E13=0),"",IF(Notenliste!F11="KP","",IF(OR(Notenliste!H11="x", Notenliste!H11="X"), "bestanden",Notenliste!F11)))</f>
+        <v/>
+      </c>
+      <c r="N13" s="17" t="str">
+        <f>IF(AND(B13=0,E13=0)," ",Notenliste!E11)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O13" s="19" t="str">
-        <f>IF(Notenliste!L11=0," ",UPPER(Notenliste!L11))</f>
+        <f>IF(AND(B13=0,E13=0)," ",IF(Notenliste!L11=0," ",UPPER(Notenliste!L11)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6019,27 +6019,27 @@
         <v>0</v>
       </c>
       <c r="J14" s="17" t="str">
-        <f>IF(Notenliste!J12=0," ",UPPER(Notenliste!J12))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K14" s="17">
-        <f>Notenliste!I12</f>
-        <v>0</v>
+        <f>IF(AND(B14=0,E14=0)," ",IF(Notenliste!J12=0," ",UPPER(Notenliste!J12)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K14" s="17" t="str">
+        <f>IF(AND(B14=0,E14=0)," ",IF(Notenliste!F12="KP","",Notenliste!I12))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L14" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M14" s="17" t="str">
-        <f>IF(OR(Notenliste!H12="x", Notenliste!H12="X"), "bestanden",IF(Notenliste!F12="KP"," ",Notenliste!F12))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N14" s="17">
-        <f>Notenliste!E12</f>
-        <v>0</v>
+        <f>IF(AND(B14=0,E14=0),"",IF(Notenliste!F12="KP","",IF(OR(Notenliste!H12="x", Notenliste!H12="X"), "bestanden",Notenliste!F12)))</f>
+        <v/>
+      </c>
+      <c r="N14" s="17" t="str">
+        <f>IF(AND(B14=0,E14=0)," ",Notenliste!E12)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O14" s="19" t="str">
-        <f>IF(Notenliste!L12=0," ",UPPER(Notenliste!L12))</f>
+        <f>IF(AND(B14=0,E14=0)," ",IF(Notenliste!L12=0," ",UPPER(Notenliste!L12)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6080,27 +6080,27 @@
         <v>0</v>
       </c>
       <c r="J15" s="17" t="str">
-        <f>IF(Notenliste!J13=0," ",UPPER(Notenliste!J13))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K15" s="17">
-        <f>Notenliste!I13</f>
-        <v>0</v>
+        <f>IF(AND(B15=0,E15=0)," ",IF(Notenliste!J13=0," ",UPPER(Notenliste!J13)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K15" s="17" t="str">
+        <f>IF(AND(B15=0,E15=0)," ",IF(Notenliste!F13="KP","",Notenliste!I13))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L15" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M15" s="17" t="str">
-        <f>IF(OR(Notenliste!H13="x", Notenliste!H13="X"), "bestanden",IF(Notenliste!F13="KP"," ",Notenliste!F13))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N15" s="17">
-        <f>Notenliste!E13</f>
-        <v>0</v>
+        <f>IF(AND(B15=0,E15=0),"",IF(Notenliste!F13="KP","",IF(OR(Notenliste!H13="x", Notenliste!H13="X"), "bestanden",Notenliste!F13)))</f>
+        <v/>
+      </c>
+      <c r="N15" s="17" t="str">
+        <f>IF(AND(B15=0,E15=0)," ",Notenliste!E13)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O15" s="19" t="str">
-        <f>IF(Notenliste!L13=0," ",UPPER(Notenliste!L13))</f>
+        <f>IF(AND(B15=0,E15=0)," ",IF(Notenliste!L13=0," ",UPPER(Notenliste!L13)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6141,27 +6141,27 @@
         <v>0</v>
       </c>
       <c r="J16" s="17" t="str">
-        <f>IF(Notenliste!J14=0," ",UPPER(Notenliste!J14))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K16" s="17">
-        <f>Notenliste!I14</f>
-        <v>0</v>
+        <f>IF(AND(B16=0,E16=0)," ",IF(Notenliste!J14=0," ",UPPER(Notenliste!J14)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K16" s="17" t="str">
+        <f>IF(AND(B16=0,E16=0)," ",IF(Notenliste!F14="KP","",Notenliste!I14))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L16" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M16" s="17" t="str">
-        <f>IF(OR(Notenliste!H14="x", Notenliste!H14="X"), "bestanden",IF(Notenliste!F14="KP"," ",Notenliste!F14))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N16" s="17">
-        <f>Notenliste!E14</f>
-        <v>0</v>
+        <f>IF(AND(B16=0,E16=0),"",IF(Notenliste!F14="KP","",IF(OR(Notenliste!H14="x", Notenliste!H14="X"), "bestanden",Notenliste!F14)))</f>
+        <v/>
+      </c>
+      <c r="N16" s="17" t="str">
+        <f>IF(AND(B16=0,E16=0)," ",Notenliste!E14)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O16" s="19" t="str">
-        <f>IF(Notenliste!L14=0," ",UPPER(Notenliste!L14))</f>
+        <f>IF(AND(B16=0,E16=0)," ",IF(Notenliste!L14=0," ",UPPER(Notenliste!L14)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6202,27 +6202,27 @@
         <v>0</v>
       </c>
       <c r="J17" s="17" t="str">
-        <f>IF(Notenliste!J15=0," ",UPPER(Notenliste!J15))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K17" s="17">
-        <f>Notenliste!I15</f>
-        <v>0</v>
+        <f>IF(AND(B17=0,E17=0)," ",IF(Notenliste!J15=0," ",UPPER(Notenliste!J15)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K17" s="17" t="str">
+        <f>IF(AND(B17=0,E17=0)," ",IF(Notenliste!F15="KP","",Notenliste!I15))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L17" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M17" s="17" t="str">
-        <f>IF(OR(Notenliste!H15="x", Notenliste!H15="X"), "bestanden",IF(Notenliste!F15="KP"," ",Notenliste!F15))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N17" s="17">
-        <f>Notenliste!E15</f>
-        <v>0</v>
+        <f>IF(AND(B17=0,E17=0),"",IF(Notenliste!F15="KP","",IF(OR(Notenliste!H15="x", Notenliste!H15="X"), "bestanden",Notenliste!F15)))</f>
+        <v/>
+      </c>
+      <c r="N17" s="17" t="str">
+        <f>IF(AND(B17=0,E17=0)," ",Notenliste!E15)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O17" s="19" t="str">
-        <f>IF(Notenliste!L15=0," ",UPPER(Notenliste!L15))</f>
+        <f>IF(AND(B17=0,E17=0)," ",IF(Notenliste!L15=0," ",UPPER(Notenliste!L15)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6263,27 +6263,27 @@
         <v>0</v>
       </c>
       <c r="J18" s="17" t="str">
-        <f>IF(Notenliste!J16=0," ",UPPER(Notenliste!J16))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K18" s="17">
-        <f>Notenliste!I16</f>
-        <v>0</v>
+        <f>IF(AND(B18=0,E18=0)," ",IF(Notenliste!J16=0," ",UPPER(Notenliste!J16)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K18" s="17" t="str">
+        <f>IF(AND(B18=0,E18=0)," ",IF(Notenliste!F16="KP","",Notenliste!I16))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L18" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M18" s="17" t="str">
-        <f>IF(OR(Notenliste!H16="x", Notenliste!H16="X"), "bestanden",IF(Notenliste!F16="KP"," ",Notenliste!F16))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N18" s="17">
-        <f>Notenliste!E16</f>
-        <v>0</v>
+        <f>IF(AND(B18=0,E18=0),"",IF(Notenliste!F16="KP","",IF(OR(Notenliste!H16="x", Notenliste!H16="X"), "bestanden",Notenliste!F16)))</f>
+        <v/>
+      </c>
+      <c r="N18" s="17" t="str">
+        <f>IF(AND(B18=0,E18=0)," ",Notenliste!E16)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O18" s="19" t="str">
-        <f>IF(Notenliste!L16=0," ",UPPER(Notenliste!L16))</f>
+        <f>IF(AND(B18=0,E18=0)," ",IF(Notenliste!L16=0," ",UPPER(Notenliste!L16)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6324,27 +6324,27 @@
         <v>0</v>
       </c>
       <c r="J19" s="17" t="str">
-        <f>IF(Notenliste!J17=0," ",UPPER(Notenliste!J17))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K19" s="17">
-        <f>Notenliste!I17</f>
-        <v>0</v>
+        <f>IF(AND(B19=0,E19=0)," ",IF(Notenliste!J17=0," ",UPPER(Notenliste!J17)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K19" s="17" t="str">
+        <f>IF(AND(B19=0,E19=0)," ",IF(Notenliste!F17="KP","",Notenliste!I17))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L19" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M19" s="17" t="str">
-        <f>IF(OR(Notenliste!H17="x", Notenliste!H17="X"), "bestanden",IF(Notenliste!F17="KP"," ",Notenliste!F17))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N19" s="17">
-        <f>Notenliste!E17</f>
-        <v>0</v>
+        <f>IF(AND(B19=0,E19=0),"",IF(Notenliste!F17="KP","",IF(OR(Notenliste!H17="x", Notenliste!H17="X"), "bestanden",Notenliste!F17)))</f>
+        <v/>
+      </c>
+      <c r="N19" s="17" t="str">
+        <f>IF(AND(B19=0,E19=0)," ",Notenliste!E17)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O19" s="19" t="str">
-        <f>IF(Notenliste!L17=0," ",UPPER(Notenliste!L17))</f>
+        <f>IF(AND(B19=0,E19=0)," ",IF(Notenliste!L17=0," ",UPPER(Notenliste!L17)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6385,27 +6385,27 @@
         <v>0</v>
       </c>
       <c r="J20" s="17" t="str">
-        <f>IF(Notenliste!J18=0," ",UPPER(Notenliste!J18))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K20" s="17">
-        <f>Notenliste!I18</f>
-        <v>0</v>
+        <f>IF(AND(B20=0,E20=0)," ",IF(Notenliste!J18=0," ",UPPER(Notenliste!J18)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K20" s="17" t="str">
+        <f>IF(AND(B20=0,E20=0)," ",IF(Notenliste!F18="KP","",Notenliste!I18))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L20" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M20" s="17" t="str">
-        <f>IF(OR(Notenliste!H18="x", Notenliste!H18="X"), "bestanden",IF(Notenliste!F18="KP"," ",Notenliste!F18))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N20" s="17">
-        <f>Notenliste!E18</f>
-        <v>0</v>
+        <f>IF(AND(B20=0,E20=0),"",IF(Notenliste!F18="KP","",IF(OR(Notenliste!H18="x", Notenliste!H18="X"), "bestanden",Notenliste!F18)))</f>
+        <v/>
+      </c>
+      <c r="N20" s="17" t="str">
+        <f>IF(AND(B20=0,E20=0)," ",Notenliste!E18)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O20" s="19" t="str">
-        <f>IF(Notenliste!L18=0," ",UPPER(Notenliste!L18))</f>
+        <f>IF(AND(B20=0,E20=0)," ",IF(Notenliste!L18=0," ",UPPER(Notenliste!L18)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6446,27 +6446,27 @@
         <v>0</v>
       </c>
       <c r="J21" s="17" t="str">
-        <f>IF(Notenliste!J19=0," ",UPPER(Notenliste!J19))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K21" s="17">
-        <f>Notenliste!I19</f>
-        <v>0</v>
+        <f>IF(AND(B21=0,E21=0)," ",IF(Notenliste!J19=0," ",UPPER(Notenliste!J19)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K21" s="17" t="str">
+        <f>IF(AND(B21=0,E21=0)," ",IF(Notenliste!F19="KP","",Notenliste!I19))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L21" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M21" s="17" t="str">
-        <f>IF(OR(Notenliste!H19="x", Notenliste!H19="X"), "bestanden",IF(Notenliste!F19="KP"," ",Notenliste!F19))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N21" s="17">
-        <f>Notenliste!E19</f>
-        <v>0</v>
+        <f>IF(AND(B21=0,E21=0),"",IF(Notenliste!F19="KP","",IF(OR(Notenliste!H19="x", Notenliste!H19="X"), "bestanden",Notenliste!F19)))</f>
+        <v/>
+      </c>
+      <c r="N21" s="17" t="str">
+        <f>IF(AND(B21=0,E21=0)," ",Notenliste!E19)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O21" s="19" t="str">
-        <f>IF(Notenliste!L19=0," ",UPPER(Notenliste!L19))</f>
+        <f>IF(AND(B21=0,E21=0)," ",IF(Notenliste!L19=0," ",UPPER(Notenliste!L19)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6507,27 +6507,27 @@
         <v>0</v>
       </c>
       <c r="J22" s="17" t="str">
-        <f>IF(Notenliste!J20=0," ",UPPER(Notenliste!J20))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K22" s="17">
-        <f>Notenliste!I20</f>
-        <v>0</v>
+        <f>IF(AND(B22=0,E22=0)," ",IF(Notenliste!J20=0," ",UPPER(Notenliste!J20)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K22" s="17" t="str">
+        <f>IF(AND(B22=0,E22=0)," ",IF(Notenliste!F20="KP","",Notenliste!I20))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L22" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M22" s="17" t="str">
-        <f>IF(OR(Notenliste!H20="x", Notenliste!H20="X"), "bestanden",IF(Notenliste!F20="KP"," ",Notenliste!F20))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N22" s="17">
-        <f>Notenliste!E20</f>
-        <v>0</v>
+        <f>IF(AND(B22=0,E22=0),"",IF(Notenliste!F20="KP","",IF(OR(Notenliste!H20="x", Notenliste!H20="X"), "bestanden",Notenliste!F20)))</f>
+        <v/>
+      </c>
+      <c r="N22" s="17" t="str">
+        <f>IF(AND(B22=0,E22=0)," ",Notenliste!E20)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O22" s="19" t="str">
-        <f>IF(Notenliste!L20=0," ",UPPER(Notenliste!L20))</f>
+        <f>IF(AND(B22=0,E22=0)," ",IF(Notenliste!L20=0," ",UPPER(Notenliste!L20)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6568,27 +6568,27 @@
         <v>0</v>
       </c>
       <c r="J23" s="17" t="str">
-        <f>IF(Notenliste!J21=0," ",UPPER(Notenliste!J21))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K23" s="17">
-        <f>Notenliste!I21</f>
-        <v>0</v>
+        <f>IF(AND(B23=0,E23=0)," ",IF(Notenliste!J21=0," ",UPPER(Notenliste!J21)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K23" s="17" t="str">
+        <f>IF(AND(B23=0,E23=0)," ",IF(Notenliste!F21="KP","",Notenliste!I21))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L23" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M23" s="17" t="str">
-        <f>IF(OR(Notenliste!H21="x", Notenliste!H21="X"), "bestanden",IF(Notenliste!F21="KP"," ",Notenliste!F21))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N23" s="17">
-        <f>Notenliste!E21</f>
-        <v>0</v>
+        <f>IF(AND(B23=0,E23=0),"",IF(Notenliste!F21="KP","",IF(OR(Notenliste!H21="x", Notenliste!H21="X"), "bestanden",Notenliste!F21)))</f>
+        <v/>
+      </c>
+      <c r="N23" s="17" t="str">
+        <f>IF(AND(B23=0,E23=0)," ",Notenliste!E21)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O23" s="19" t="str">
-        <f>IF(Notenliste!L21=0," ",UPPER(Notenliste!L21))</f>
+        <f>IF(AND(B23=0,E23=0)," ",IF(Notenliste!L21=0," ",UPPER(Notenliste!L21)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6629,27 +6629,27 @@
         <v>0</v>
       </c>
       <c r="J24" s="17" t="str">
-        <f>IF(Notenliste!J22=0," ",UPPER(Notenliste!J22))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K24" s="17">
-        <f>Notenliste!I22</f>
-        <v>0</v>
+        <f>IF(AND(B24=0,E24=0)," ",IF(Notenliste!J22=0," ",UPPER(Notenliste!J22)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K24" s="17" t="str">
+        <f>IF(AND(B24=0,E24=0)," ",IF(Notenliste!F22="KP","",Notenliste!I22))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L24" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M24" s="17" t="str">
-        <f>IF(OR(Notenliste!H22="x", Notenliste!H22="X"), "bestanden",IF(Notenliste!F22="KP"," ",Notenliste!F22))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N24" s="17">
-        <f>Notenliste!E22</f>
-        <v>0</v>
+        <f>IF(AND(B24=0,E24=0),"",IF(Notenliste!F22="KP","",IF(OR(Notenliste!H22="x", Notenliste!H22="X"), "bestanden",Notenliste!F22)))</f>
+        <v/>
+      </c>
+      <c r="N24" s="17" t="str">
+        <f>IF(AND(B24=0,E24=0)," ",Notenliste!E22)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O24" s="19" t="str">
-        <f>IF(Notenliste!L22=0," ",UPPER(Notenliste!L22))</f>
+        <f>IF(AND(B24=0,E24=0)," ",IF(Notenliste!L22=0," ",UPPER(Notenliste!L22)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6690,27 +6690,27 @@
         <v>0</v>
       </c>
       <c r="J25" s="17" t="str">
-        <f>IF(Notenliste!J23=0," ",UPPER(Notenliste!J23))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K25" s="17">
-        <f>Notenliste!I23</f>
-        <v>0</v>
+        <f>IF(AND(B25=0,E25=0)," ",IF(Notenliste!J23=0," ",UPPER(Notenliste!J23)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K25" s="17" t="str">
+        <f>IF(AND(B25=0,E25=0)," ",IF(Notenliste!F23="KP","",Notenliste!I23))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L25" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M25" s="17" t="str">
-        <f>IF(OR(Notenliste!H23="x", Notenliste!H23="X"), "bestanden",IF(Notenliste!F23="KP"," ",Notenliste!F23))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N25" s="17">
-        <f>Notenliste!E23</f>
-        <v>0</v>
+        <f>IF(AND(B25=0,E25=0),"",IF(Notenliste!F23="KP","",IF(OR(Notenliste!H23="x", Notenliste!H23="X"), "bestanden",Notenliste!F23)))</f>
+        <v/>
+      </c>
+      <c r="N25" s="17" t="str">
+        <f>IF(AND(B25=0,E25=0)," ",Notenliste!E23)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O25" s="19" t="str">
-        <f>IF(Notenliste!L23=0," ",UPPER(Notenliste!L23))</f>
+        <f>IF(AND(B25=0,E25=0)," ",IF(Notenliste!L23=0," ",UPPER(Notenliste!L23)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6751,27 +6751,27 @@
         <v>0</v>
       </c>
       <c r="J26" s="17" t="str">
-        <f>IF(Notenliste!J24=0," ",UPPER(Notenliste!J24))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K26" s="17">
-        <f>Notenliste!I24</f>
-        <v>0</v>
+        <f>IF(AND(B26=0,E26=0)," ",IF(Notenliste!J24=0," ",UPPER(Notenliste!J24)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K26" s="17" t="str">
+        <f>IF(AND(B26=0,E26=0)," ",IF(Notenliste!F24="KP","",Notenliste!I24))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L26" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M26" s="17" t="str">
-        <f>IF(OR(Notenliste!H24="x", Notenliste!H24="X"), "bestanden",IF(Notenliste!F24="KP"," ",Notenliste!F24))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N26" s="17">
-        <f>Notenliste!E24</f>
-        <v>0</v>
+        <f>IF(AND(B26=0,E26=0),"",IF(Notenliste!F24="KP","",IF(OR(Notenliste!H24="x", Notenliste!H24="X"), "bestanden",Notenliste!F24)))</f>
+        <v/>
+      </c>
+      <c r="N26" s="17" t="str">
+        <f>IF(AND(B26=0,E26=0)," ",Notenliste!E24)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O26" s="19" t="str">
-        <f>IF(Notenliste!L24=0," ",UPPER(Notenliste!L24))</f>
+        <f>IF(AND(B26=0,E26=0)," ",IF(Notenliste!L24=0," ",UPPER(Notenliste!L24)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6812,27 +6812,27 @@
         <v>0</v>
       </c>
       <c r="J27" s="17" t="str">
-        <f>IF(Notenliste!J25=0," ",UPPER(Notenliste!J25))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K27" s="17">
-        <f>Notenliste!I25</f>
-        <v>0</v>
+        <f>IF(AND(B27=0,E27=0)," ",IF(Notenliste!J25=0," ",UPPER(Notenliste!J25)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K27" s="17" t="str">
+        <f>IF(AND(B27=0,E27=0)," ",IF(Notenliste!F25="KP","",Notenliste!I25))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L27" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M27" s="17" t="str">
-        <f>IF(OR(Notenliste!H25="x", Notenliste!H25="X"), "bestanden",IF(Notenliste!F25="KP"," ",Notenliste!F25))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N27" s="17">
-        <f>Notenliste!E25</f>
-        <v>0</v>
+        <f>IF(AND(B27=0,E27=0),"",IF(Notenliste!F25="KP","",IF(OR(Notenliste!H25="x", Notenliste!H25="X"), "bestanden",Notenliste!F25)))</f>
+        <v/>
+      </c>
+      <c r="N27" s="17" t="str">
+        <f>IF(AND(B27=0,E27=0)," ",Notenliste!E25)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O27" s="19" t="str">
-        <f>IF(Notenliste!L25=0," ",UPPER(Notenliste!L25))</f>
+        <f>IF(AND(B27=0,E27=0)," ",IF(Notenliste!L25=0," ",UPPER(Notenliste!L25)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6873,27 +6873,27 @@
         <v>0</v>
       </c>
       <c r="J28" s="17" t="str">
-        <f>IF(Notenliste!J26=0," ",UPPER(Notenliste!J26))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K28" s="17">
-        <f>Notenliste!I26</f>
-        <v>0</v>
+        <f>IF(AND(B28=0,E28=0)," ",IF(Notenliste!J26=0," ",UPPER(Notenliste!J26)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K28" s="17" t="str">
+        <f>IF(AND(B28=0,E28=0)," ",IF(Notenliste!F26="KP","",Notenliste!I26))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L28" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M28" s="17" t="str">
-        <f>IF(OR(Notenliste!H26="x", Notenliste!H26="X"), "bestanden",IF(Notenliste!F26="KP"," ",Notenliste!F26))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N28" s="17">
-        <f>Notenliste!E26</f>
-        <v>0</v>
+        <f>IF(AND(B28=0,E28=0),"",IF(Notenliste!F26="KP","",IF(OR(Notenliste!H26="x", Notenliste!H26="X"), "bestanden",Notenliste!F26)))</f>
+        <v/>
+      </c>
+      <c r="N28" s="17" t="str">
+        <f>IF(AND(B28=0,E28=0)," ",Notenliste!E26)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O28" s="19" t="str">
-        <f>IF(Notenliste!L26=0," ",UPPER(Notenliste!L26))</f>
+        <f>IF(AND(B28=0,E28=0)," ",IF(Notenliste!L26=0," ",UPPER(Notenliste!L26)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6934,27 +6934,27 @@
         <v>0</v>
       </c>
       <c r="J29" s="17" t="str">
-        <f>IF(Notenliste!J27=0," ",UPPER(Notenliste!J27))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K29" s="17">
-        <f>Notenliste!I27</f>
-        <v>0</v>
+        <f>IF(AND(B29=0,E29=0)," ",IF(Notenliste!J27=0," ",UPPER(Notenliste!J27)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K29" s="17" t="str">
+        <f>IF(AND(B29=0,E29=0)," ",IF(Notenliste!F27="KP","",Notenliste!I27))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L29" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M29" s="17" t="str">
-        <f>IF(OR(Notenliste!H27="x", Notenliste!H27="X"), "bestanden",IF(Notenliste!F27="KP"," ",Notenliste!F27))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N29" s="17">
-        <f>Notenliste!E27</f>
-        <v>0</v>
+        <f>IF(AND(B29=0,E29=0),"",IF(Notenliste!F27="KP","",IF(OR(Notenliste!H27="x", Notenliste!H27="X"), "bestanden",Notenliste!F27)))</f>
+        <v/>
+      </c>
+      <c r="N29" s="17" t="str">
+        <f>IF(AND(B29=0,E29=0)," ",Notenliste!E27)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O29" s="19" t="str">
-        <f>IF(Notenliste!L27=0," ",UPPER(Notenliste!L27))</f>
+        <f>IF(AND(B29=0,E29=0)," ",IF(Notenliste!L27=0," ",UPPER(Notenliste!L27)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6995,27 +6995,27 @@
         <v>0</v>
       </c>
       <c r="J30" s="17" t="str">
-        <f>IF(Notenliste!J28=0," ",UPPER(Notenliste!J28))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K30" s="17">
-        <f>Notenliste!I28</f>
-        <v>0</v>
+        <f>IF(AND(B30=0,E30=0)," ",IF(Notenliste!J28=0," ",UPPER(Notenliste!J28)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K30" s="17" t="str">
+        <f>IF(AND(B30=0,E30=0)," ",IF(Notenliste!F28="KP","",Notenliste!I28))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L30" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M30" s="17" t="str">
-        <f>IF(OR(Notenliste!H28="x", Notenliste!H28="X"), "bestanden",IF(Notenliste!F28="KP"," ",Notenliste!F28))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N30" s="17">
-        <f>Notenliste!E28</f>
-        <v>0</v>
+        <f>IF(AND(B30=0,E30=0),"",IF(Notenliste!F28="KP","",IF(OR(Notenliste!H28="x", Notenliste!H28="X"), "bestanden",Notenliste!F28)))</f>
+        <v/>
+      </c>
+      <c r="N30" s="17" t="str">
+        <f>IF(AND(B30=0,E30=0)," ",Notenliste!E28)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O30" s="19" t="str">
-        <f>IF(Notenliste!L28=0," ",UPPER(Notenliste!L28))</f>
+        <f>IF(AND(B30=0,E30=0)," ",IF(Notenliste!L28=0," ",UPPER(Notenliste!L28)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7056,27 +7056,27 @@
         <v>0</v>
       </c>
       <c r="J31" s="17" t="str">
-        <f>IF(Notenliste!J29=0," ",UPPER(Notenliste!J29))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K31" s="17">
-        <f>Notenliste!I29</f>
-        <v>0</v>
+        <f>IF(AND(B31=0,E31=0)," ",IF(Notenliste!J29=0," ",UPPER(Notenliste!J29)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K31" s="17" t="str">
+        <f>IF(AND(B31=0,E31=0)," ",IF(Notenliste!F29="KP","",Notenliste!I29))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L31" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M31" s="17" t="str">
-        <f>IF(OR(Notenliste!H29="x", Notenliste!H29="X"), "bestanden",IF(Notenliste!F29="KP"," ",Notenliste!F29))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N31" s="17">
-        <f>Notenliste!E29</f>
-        <v>0</v>
+        <f>IF(AND(B31=0,E31=0),"",IF(Notenliste!F29="KP","",IF(OR(Notenliste!H29="x", Notenliste!H29="X"), "bestanden",Notenliste!F29)))</f>
+        <v/>
+      </c>
+      <c r="N31" s="17" t="str">
+        <f>IF(AND(B31=0,E31=0)," ",Notenliste!E29)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O31" s="19" t="str">
-        <f>IF(Notenliste!L29=0," ",UPPER(Notenliste!L29))</f>
+        <f>IF(AND(B31=0,E31=0)," ",IF(Notenliste!L29=0," ",UPPER(Notenliste!L29)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7117,27 +7117,27 @@
         <v>0</v>
       </c>
       <c r="J32" s="17" t="str">
-        <f>IF(Notenliste!J30=0," ",UPPER(Notenliste!J30))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K32" s="17">
-        <f>Notenliste!I30</f>
-        <v>0</v>
+        <f>IF(AND(B32=0,E32=0)," ",IF(Notenliste!J30=0," ",UPPER(Notenliste!J30)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K32" s="17" t="str">
+        <f>IF(AND(B32=0,E32=0)," ",IF(Notenliste!F30="KP","",Notenliste!I30))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L32" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M32" s="17" t="str">
-        <f>IF(OR(Notenliste!H30="x", Notenliste!H30="X"), "bestanden",IF(Notenliste!F30="KP"," ",Notenliste!F30))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N32" s="17">
-        <f>Notenliste!E30</f>
-        <v>0</v>
+        <f>IF(AND(B32=0,E32=0),"",IF(Notenliste!F30="KP","",IF(OR(Notenliste!H30="x", Notenliste!H30="X"), "bestanden",Notenliste!F30)))</f>
+        <v/>
+      </c>
+      <c r="N32" s="17" t="str">
+        <f>IF(AND(B32=0,E32=0)," ",Notenliste!E30)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O32" s="19" t="str">
-        <f>IF(Notenliste!L30=0," ",UPPER(Notenliste!L30))</f>
+        <f>IF(AND(B32=0,E32=0)," ",IF(Notenliste!L30=0," ",UPPER(Notenliste!L30)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7178,27 +7178,27 @@
         <v>0</v>
       </c>
       <c r="J33" s="17" t="str">
-        <f>IF(Notenliste!J31=0," ",UPPER(Notenliste!J31))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K33" s="17">
-        <f>Notenliste!I31</f>
-        <v>0</v>
+        <f>IF(AND(B33=0,E33=0)," ",IF(Notenliste!J31=0," ",UPPER(Notenliste!J31)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K33" s="17" t="str">
+        <f>IF(AND(B33=0,E33=0)," ",IF(Notenliste!F31="KP","",Notenliste!I31))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L33" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M33" s="17" t="str">
-        <f>IF(OR(Notenliste!H31="x", Notenliste!H31="X"), "bestanden",IF(Notenliste!F31="KP"," ",Notenliste!F31))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N33" s="17">
-        <f>Notenliste!E31</f>
-        <v>0</v>
+        <f>IF(AND(B33=0,E33=0),"",IF(Notenliste!F31="KP","",IF(OR(Notenliste!H31="x", Notenliste!H31="X"), "bestanden",Notenliste!F31)))</f>
+        <v/>
+      </c>
+      <c r="N33" s="17" t="str">
+        <f>IF(AND(B33=0,E33=0)," ",Notenliste!E31)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O33" s="19" t="str">
-        <f>IF(Notenliste!L31=0," ",UPPER(Notenliste!L31))</f>
+        <f>IF(AND(B33=0,E33=0)," ",IF(Notenliste!L31=0," ",UPPER(Notenliste!L31)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7239,27 +7239,27 @@
         <v>0</v>
       </c>
       <c r="J34" s="17" t="str">
-        <f>IF(Notenliste!J32=0," ",UPPER(Notenliste!J32))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K34" s="17">
-        <f>Notenliste!I32</f>
-        <v>0</v>
+        <f>IF(AND(B34=0,E34=0)," ",IF(Notenliste!J32=0," ",UPPER(Notenliste!J32)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K34" s="17" t="str">
+        <f>IF(AND(B34=0,E34=0)," ",IF(Notenliste!F32="KP","",Notenliste!I32))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L34" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M34" s="17" t="str">
-        <f>IF(OR(Notenliste!H32="x", Notenliste!H32="X"), "bestanden",IF(Notenliste!F32="KP"," ",Notenliste!F32))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N34" s="17">
-        <f>Notenliste!E32</f>
-        <v>0</v>
+        <f>IF(AND(B34=0,E34=0),"",IF(Notenliste!F32="KP","",IF(OR(Notenliste!H32="x", Notenliste!H32="X"), "bestanden",Notenliste!F32)))</f>
+        <v/>
+      </c>
+      <c r="N34" s="17" t="str">
+        <f>IF(AND(B34=0,E34=0)," ",Notenliste!E32)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O34" s="19" t="str">
-        <f>IF(Notenliste!L32=0," ",UPPER(Notenliste!L32))</f>
+        <f>IF(AND(B34=0,E34=0)," ",IF(Notenliste!L32=0," ",UPPER(Notenliste!L32)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7300,27 +7300,27 @@
         <v>0</v>
       </c>
       <c r="J35" s="17" t="str">
-        <f>IF(Notenliste!J33=0," ",UPPER(Notenliste!J33))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K35" s="17">
-        <f>Notenliste!I33</f>
-        <v>0</v>
+        <f>IF(AND(B35=0,E35=0)," ",IF(Notenliste!J33=0," ",UPPER(Notenliste!J33)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K35" s="17" t="str">
+        <f>IF(AND(B35=0,E35=0)," ",IF(Notenliste!F33="KP","",Notenliste!I33))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L35" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M35" s="17" t="str">
-        <f>IF(OR(Notenliste!H33="x", Notenliste!H33="X"), "bestanden",IF(Notenliste!F33="KP"," ",Notenliste!F33))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N35" s="17">
-        <f>Notenliste!E33</f>
-        <v>0</v>
+        <f>IF(AND(B35=0,E35=0),"",IF(Notenliste!F33="KP","",IF(OR(Notenliste!H33="x", Notenliste!H33="X"), "bestanden",Notenliste!F33)))</f>
+        <v/>
+      </c>
+      <c r="N35" s="17" t="str">
+        <f>IF(AND(B35=0,E35=0)," ",Notenliste!E33)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O35" s="19" t="str">
-        <f>IF(Notenliste!L33=0," ",UPPER(Notenliste!L33))</f>
+        <f>IF(AND(B35=0,E35=0)," ",IF(Notenliste!L33=0," ",UPPER(Notenliste!L33)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7361,27 +7361,27 @@
         <v>0</v>
       </c>
       <c r="J36" s="17" t="str">
-        <f>IF(Notenliste!J34=0," ",UPPER(Notenliste!J34))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K36" s="17">
-        <f>Notenliste!I34</f>
-        <v>0</v>
+        <f>IF(AND(B36=0,E36=0)," ",IF(Notenliste!J34=0," ",UPPER(Notenliste!J34)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K36" s="17" t="str">
+        <f>IF(AND(B36=0,E36=0)," ",IF(Notenliste!F34="KP","",Notenliste!I34))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L36" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M36" s="17" t="str">
-        <f>IF(OR(Notenliste!H34="x", Notenliste!H34="X"), "bestanden",IF(Notenliste!F34="KP"," ",Notenliste!F34))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N36" s="17">
-        <f>Notenliste!E34</f>
-        <v>0</v>
+        <f>IF(AND(B36=0,E36=0),"",IF(Notenliste!F34="KP","",IF(OR(Notenliste!H34="x", Notenliste!H34="X"), "bestanden",Notenliste!F34)))</f>
+        <v/>
+      </c>
+      <c r="N36" s="17" t="str">
+        <f>IF(AND(B36=0,E36=0)," ",Notenliste!E34)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O36" s="19" t="str">
-        <f>IF(Notenliste!L34=0," ",UPPER(Notenliste!L34))</f>
+        <f>IF(AND(B36=0,E36=0)," ",IF(Notenliste!L34=0," ",UPPER(Notenliste!L34)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7422,27 +7422,27 @@
         <v>0</v>
       </c>
       <c r="J37" s="17" t="str">
-        <f>IF(Notenliste!J35=0," ",UPPER(Notenliste!J35))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K37" s="17">
-        <f>Notenliste!I35</f>
-        <v>0</v>
+        <f>IF(AND(B37=0,E37=0)," ",IF(Notenliste!J35=0," ",UPPER(Notenliste!J35)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K37" s="17" t="str">
+        <f>IF(AND(B37=0,E37=0)," ",IF(Notenliste!F35="KP","",Notenliste!I35))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L37" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M37" s="17" t="str">
-        <f>IF(OR(Notenliste!H35="x", Notenliste!H35="X"), "bestanden",IF(Notenliste!F35="KP"," ",Notenliste!F35))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N37" s="17">
-        <f>Notenliste!E35</f>
-        <v>0</v>
+        <f>IF(AND(B37=0,E37=0),"",IF(Notenliste!F35="KP","",IF(OR(Notenliste!H35="x", Notenliste!H35="X"), "bestanden",Notenliste!F35)))</f>
+        <v/>
+      </c>
+      <c r="N37" s="17" t="str">
+        <f>IF(AND(B37=0,E37=0)," ",Notenliste!E35)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O37" s="19" t="str">
-        <f>IF(Notenliste!L35=0," ",UPPER(Notenliste!L35))</f>
+        <f>IF(AND(B37=0,E37=0)," ",IF(Notenliste!L35=0," ",UPPER(Notenliste!L35)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -7483,27 +7483,27 @@
         <v>0</v>
       </c>
       <c r="J38" s="17" t="str">
-        <f>IF(Notenliste!J36=0," ",UPPER(Notenliste!J36))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K38" s="17">
-        <f>Notenliste!I36</f>
-        <v>0</v>
+        <f>IF(AND(B38=0,E38=0)," ",IF(Notenliste!J36=0," ",UPPER(Notenliste!J36)))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K38" s="17" t="str">
+        <f>IF(AND(B38=0,E38=0)," ",IF(Notenliste!F36="KP","",Notenliste!I36))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="L38" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M38" s="17" t="str">
-        <f>IF(OR(Notenliste!H36="x", Notenliste!H36="X"), "bestanden",IF(Notenliste!F36="KP"," ",Notenliste!F36))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N38" s="17">
-        <f>Notenliste!E36</f>
-        <v>0</v>
+        <f>IF(AND(B38=0,E38=0),"",IF(Notenliste!F36="KP","",IF(OR(Notenliste!H36="x", Notenliste!H36="X"), "bestanden",Notenliste!F36)))</f>
+        <v/>
+      </c>
+      <c r="N38" s="17" t="str">
+        <f>IF(AND(B38=0,E38=0)," ",Notenliste!E36)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="O38" s="19" t="str">
-        <f>IF(Notenliste!L36=0," ",UPPER(Notenliste!L36))</f>
+        <f>IF(AND(B38=0,E38=0)," ",IF(Notenliste!L36=0," ",UPPER(Notenliste!L36)))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -9277,8 +9277,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9329,7 +9329,7 @@
         <v>attendance.ects_points</v>
       </c>
       <c r="D2" s="65" t="e">
-        <f>IF(OR(Notenliste!H2="x", Notenliste!H2="X"),"bestanden",IF(Notenliste!D2=0," ",IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2))))</f>
+        <f>IF(Notenliste!D2=0," ",IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",IF(OR(Notenliste!H2="x", Notenliste!H2="X"),"bestanden",Notenliste!F2))))</f>
         <v>#N/A</v>
       </c>
       <c r="E2" s="66" t="str">
@@ -9351,7 +9351,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D3" s="65" t="str">
-        <f>IF(OR(Notenliste!H3="x", Notenliste!H3="X"),"bestanden",IF(Notenliste!D3=0," ",IF(Notenliste!F3="KP"," ",IF(Notenliste!F3="NB","nicht bestanden",Notenliste!F3))))</f>
+        <f>IF(Notenliste!D3=0," ",IF(Notenliste!F3="KP"," ",IF(Notenliste!F3="NB","nicht bestanden",IF(OR(Notenliste!H3="x", Notenliste!H3="X"),"bestanden",Notenliste!F3))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E3" s="66" t="str">
@@ -9373,7 +9373,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D4" s="65" t="str">
-        <f>IF(OR(Notenliste!H4="x", Notenliste!H4="X"),"bestanden",IF(Notenliste!D4=0," ",IF(Notenliste!F4="KP"," ",IF(Notenliste!F4="NB","nicht bestanden",Notenliste!F4))))</f>
+        <f>IF(Notenliste!D4=0," ",IF(Notenliste!F4="KP"," ",IF(Notenliste!F4="NB","nicht bestanden",IF(OR(Notenliste!H4="x", Notenliste!H4="X"),"bestanden",Notenliste!F4))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E4" s="66" t="str">
@@ -9395,7 +9395,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="65" t="str">
-        <f>IF(OR(Notenliste!H5="x", Notenliste!H5="X"),"bestanden",IF(Notenliste!D5=0," ",IF(Notenliste!F5="KP"," ",IF(Notenliste!F5="NB","nicht bestanden",Notenliste!F5))))</f>
+        <f>IF(Notenliste!D5=0," ",IF(Notenliste!F5="KP"," ",IF(Notenliste!F5="NB","nicht bestanden",IF(OR(Notenliste!H5="x", Notenliste!H5="X"),"bestanden",Notenliste!F5))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="66" t="str">
@@ -9417,7 +9417,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D6" s="65" t="str">
-        <f>IF(OR(Notenliste!H6="x", Notenliste!H6="X"),"bestanden",IF(Notenliste!D6=0," ",IF(Notenliste!F6="KP"," ",IF(Notenliste!F6="NB","nicht bestanden",Notenliste!F6))))</f>
+        <f>IF(Notenliste!D6=0," ",IF(Notenliste!F6="KP"," ",IF(Notenliste!F6="NB","nicht bestanden",IF(OR(Notenliste!H6="x", Notenliste!H6="X"),"bestanden",Notenliste!F6))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E6" s="66" t="str">
@@ -9439,7 +9439,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D7" s="65" t="str">
-        <f>IF(OR(Notenliste!H7="x", Notenliste!H7="X"),"bestanden",IF(Notenliste!D7=0," ",IF(Notenliste!F7="KP"," ",IF(Notenliste!F7="NB","nicht bestanden",Notenliste!F7))))</f>
+        <f>IF(Notenliste!D7=0," ",IF(Notenliste!F7="KP"," ",IF(Notenliste!F7="NB","nicht bestanden",IF(OR(Notenliste!H7="x", Notenliste!H7="X"),"bestanden",Notenliste!F7))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E7" s="66" t="str">
@@ -9461,7 +9461,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D8" s="65" t="str">
-        <f>IF(OR(Notenliste!H8="x", Notenliste!H8="X"),"bestanden",IF(Notenliste!D8=0," ",IF(Notenliste!F8="KP"," ",IF(Notenliste!F8="NB","nicht bestanden",Notenliste!F8))))</f>
+        <f>IF(Notenliste!D8=0," ",IF(Notenliste!F8="KP"," ",IF(Notenliste!F8="NB","nicht bestanden",IF(OR(Notenliste!H8="x", Notenliste!H8="X"),"bestanden",Notenliste!F8))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E8" s="66" t="str">
@@ -9483,7 +9483,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D9" s="65" t="str">
-        <f>IF(OR(Notenliste!H9="x", Notenliste!H9="X"),"bestanden",IF(Notenliste!D9=0," ",IF(Notenliste!F9="KP"," ",IF(Notenliste!F9="NB","nicht bestanden",Notenliste!F9))))</f>
+        <f>IF(Notenliste!D9=0," ",IF(Notenliste!F9="KP"," ",IF(Notenliste!F9="NB","nicht bestanden",IF(OR(Notenliste!H9="x", Notenliste!H9="X"),"bestanden",Notenliste!F9))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E9" s="66" t="str">
@@ -9505,7 +9505,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D10" s="65" t="str">
-        <f>IF(OR(Notenliste!H10="x", Notenliste!H10="X"),"bestanden",IF(Notenliste!D10=0," ",IF(Notenliste!F10="KP"," ",IF(Notenliste!F10="NB","nicht bestanden",Notenliste!F10))))</f>
+        <f>IF(Notenliste!D10=0," ",IF(Notenliste!F10="KP"," ",IF(Notenliste!F10="NB","nicht bestanden",IF(OR(Notenliste!H10="x", Notenliste!H10="X"),"bestanden",Notenliste!F10))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E10" s="66" t="str">
@@ -9527,7 +9527,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D11" s="65" t="str">
-        <f>IF(OR(Notenliste!H11="x", Notenliste!H11="X"),"bestanden",IF(Notenliste!D11=0," ",IF(Notenliste!F11="KP"," ",IF(Notenliste!F11="NB","nicht bestanden",Notenliste!F11))))</f>
+        <f>IF(Notenliste!D11=0," ",IF(Notenliste!F11="KP"," ",IF(Notenliste!F11="NB","nicht bestanden",IF(OR(Notenliste!H11="x", Notenliste!H11="X"),"bestanden",Notenliste!F11))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E11" s="66" t="str">
@@ -9549,7 +9549,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D12" s="65" t="str">
-        <f>IF(OR(Notenliste!H12="x", Notenliste!H12="X"),"bestanden",IF(Notenliste!D12=0," ",IF(Notenliste!F12="KP"," ",IF(Notenliste!F12="NB","nicht bestanden",Notenliste!F12))))</f>
+        <f>IF(Notenliste!D12=0," ",IF(Notenliste!F12="KP"," ",IF(Notenliste!F12="NB","nicht bestanden",IF(OR(Notenliste!H12="x", Notenliste!H12="X"),"bestanden",Notenliste!F12))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E12" s="66" t="str">
@@ -9571,7 +9571,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D13" s="65" t="str">
-        <f>IF(OR(Notenliste!H13="x", Notenliste!H13="X"),"bestanden",IF(Notenliste!D13=0," ",IF(Notenliste!F13="KP"," ",IF(Notenliste!F13="NB","nicht bestanden",Notenliste!F13))))</f>
+        <f>IF(Notenliste!D13=0," ",IF(Notenliste!F13="KP"," ",IF(Notenliste!F13="NB","nicht bestanden",IF(OR(Notenliste!H13="x", Notenliste!H13="X"),"bestanden",Notenliste!F13))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E13" s="66" t="str">
@@ -9593,7 +9593,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D14" s="65" t="str">
-        <f>IF(OR(Notenliste!H14="x", Notenliste!H14="X"),"bestanden",IF(Notenliste!D14=0," ",IF(Notenliste!F14="KP"," ",IF(Notenliste!F14="NB","nicht bestanden",Notenliste!F14))))</f>
+        <f>IF(Notenliste!D14=0," ",IF(Notenliste!F14="KP"," ",IF(Notenliste!F14="NB","nicht bestanden",IF(OR(Notenliste!H14="x", Notenliste!H14="X"),"bestanden",Notenliste!F14))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E14" s="66" t="str">
@@ -9615,7 +9615,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D15" s="65" t="str">
-        <f>IF(OR(Notenliste!H15="x", Notenliste!H15="X"),"bestanden",IF(Notenliste!D15=0," ",IF(Notenliste!F15="KP"," ",IF(Notenliste!F15="NB","nicht bestanden",Notenliste!F15))))</f>
+        <f>IF(Notenliste!D15=0," ",IF(Notenliste!F15="KP"," ",IF(Notenliste!F15="NB","nicht bestanden",IF(OR(Notenliste!H15="x", Notenliste!H15="X"),"bestanden",Notenliste!F15))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E15" s="66" t="str">
@@ -9637,7 +9637,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D16" s="65" t="str">
-        <f>IF(OR(Notenliste!H16="x", Notenliste!H16="X"),"bestanden",IF(Notenliste!D16=0," ",IF(Notenliste!F16="KP"," ",IF(Notenliste!F16="NB","nicht bestanden",Notenliste!F16))))</f>
+        <f>IF(Notenliste!D16=0," ",IF(Notenliste!F16="KP"," ",IF(Notenliste!F16="NB","nicht bestanden",IF(OR(Notenliste!H16="x", Notenliste!H16="X"),"bestanden",Notenliste!F16))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E16" s="66" t="str">
@@ -9659,7 +9659,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D17" s="65" t="str">
-        <f>IF(OR(Notenliste!H17="x", Notenliste!H17="X"),"bestanden",IF(Notenliste!D17=0," ",IF(Notenliste!F17="KP"," ",IF(Notenliste!F17="NB","nicht bestanden",Notenliste!F17))))</f>
+        <f>IF(Notenliste!D17=0," ",IF(Notenliste!F17="KP"," ",IF(Notenliste!F17="NB","nicht bestanden",IF(OR(Notenliste!H17="x", Notenliste!H17="X"),"bestanden",Notenliste!F17))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E17" s="66" t="str">
@@ -9681,7 +9681,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D18" s="65" t="str">
-        <f>IF(OR(Notenliste!H18="x", Notenliste!H18="X"),"bestanden",IF(Notenliste!D18=0," ",IF(Notenliste!F18="KP"," ",IF(Notenliste!F18="NB","nicht bestanden",Notenliste!F18))))</f>
+        <f>IF(Notenliste!D18=0," ",IF(Notenliste!F18="KP"," ",IF(Notenliste!F18="NB","nicht bestanden",IF(OR(Notenliste!H18="x", Notenliste!H18="X"),"bestanden",Notenliste!F18))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E18" s="66" t="str">
@@ -9703,7 +9703,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D19" s="65" t="str">
-        <f>IF(OR(Notenliste!H19="x", Notenliste!H19="X"),"bestanden",IF(Notenliste!D19=0," ",IF(Notenliste!F19="KP"," ",IF(Notenliste!F19="NB","nicht bestanden",Notenliste!F19))))</f>
+        <f>IF(Notenliste!D19=0," ",IF(Notenliste!F19="KP"," ",IF(Notenliste!F19="NB","nicht bestanden",IF(OR(Notenliste!H19="x", Notenliste!H19="X"),"bestanden",Notenliste!F19))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E19" s="66" t="str">
@@ -9725,7 +9725,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D20" s="65" t="str">
-        <f>IF(OR(Notenliste!H20="x", Notenliste!H20="X"),"bestanden",IF(Notenliste!D20=0," ",IF(Notenliste!F20="KP"," ",IF(Notenliste!F20="NB","nicht bestanden",Notenliste!F20))))</f>
+        <f>IF(Notenliste!D20=0," ",IF(Notenliste!F20="KP"," ",IF(Notenliste!F20="NB","nicht bestanden",IF(OR(Notenliste!H20="x", Notenliste!H20="X"),"bestanden",Notenliste!F20))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E20" s="66" t="str">
@@ -9747,7 +9747,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D21" s="65" t="str">
-        <f>IF(OR(Notenliste!H21="x", Notenliste!H21="X"),"bestanden",IF(Notenliste!D21=0," ",IF(Notenliste!F21="KP"," ",IF(Notenliste!F21="NB","nicht bestanden",Notenliste!F21))))</f>
+        <f>IF(Notenliste!D21=0," ",IF(Notenliste!F21="KP"," ",IF(Notenliste!F21="NB","nicht bestanden",IF(OR(Notenliste!H21="x", Notenliste!H21="X"),"bestanden",Notenliste!F21))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E21" s="66" t="str">
@@ -9769,7 +9769,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D22" s="65" t="str">
-        <f>IF(OR(Notenliste!H22="x", Notenliste!H22="X"),"bestanden",IF(Notenliste!D22=0," ",IF(Notenliste!F22="KP"," ",IF(Notenliste!F22="NB","nicht bestanden",Notenliste!F22))))</f>
+        <f>IF(Notenliste!D22=0," ",IF(Notenliste!F22="KP"," ",IF(Notenliste!F22="NB","nicht bestanden",IF(OR(Notenliste!H22="x", Notenliste!H22="X"),"bestanden",Notenliste!F22))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E22" s="66" t="str">
@@ -9791,7 +9791,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D23" s="65" t="str">
-        <f>IF(OR(Notenliste!H23="x", Notenliste!H23="X"),"bestanden",IF(Notenliste!D23=0," ",IF(Notenliste!F23="KP"," ",IF(Notenliste!F23="NB","nicht bestanden",Notenliste!F23))))</f>
+        <f>IF(Notenliste!D23=0," ",IF(Notenliste!F23="KP"," ",IF(Notenliste!F23="NB","nicht bestanden",IF(OR(Notenliste!H23="x", Notenliste!H23="X"),"bestanden",Notenliste!F23))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E23" s="66" t="str">
@@ -9813,7 +9813,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D24" s="65" t="str">
-        <f>IF(OR(Notenliste!H24="x", Notenliste!H24="X"),"bestanden",IF(Notenliste!D24=0," ",IF(Notenliste!F24="KP"," ",IF(Notenliste!F24="NB","nicht bestanden",Notenliste!F24))))</f>
+        <f>IF(Notenliste!D24=0," ",IF(Notenliste!F24="KP"," ",IF(Notenliste!F24="NB","nicht bestanden",IF(OR(Notenliste!H24="x", Notenliste!H24="X"),"bestanden",Notenliste!F24))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E24" s="66" t="str">
@@ -9835,7 +9835,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D25" s="65" t="str">
-        <f>IF(OR(Notenliste!H25="x", Notenliste!H25="X"),"bestanden",IF(Notenliste!D25=0," ",IF(Notenliste!F25="KP"," ",IF(Notenliste!F25="NB","nicht bestanden",Notenliste!F25))))</f>
+        <f>IF(Notenliste!D25=0," ",IF(Notenliste!F25="KP"," ",IF(Notenliste!F25="NB","nicht bestanden",IF(OR(Notenliste!H25="x", Notenliste!H25="X"),"bestanden",Notenliste!F25))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E25" s="66" t="str">
@@ -9857,7 +9857,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D26" s="65" t="str">
-        <f>IF(OR(Notenliste!H26="x", Notenliste!H26="X"),"bestanden",IF(Notenliste!D26=0," ",IF(Notenliste!F26="KP"," ",IF(Notenliste!F26="NB","nicht bestanden",Notenliste!F26))))</f>
+        <f>IF(Notenliste!D26=0," ",IF(Notenliste!F26="KP"," ",IF(Notenliste!F26="NB","nicht bestanden",IF(OR(Notenliste!H26="x", Notenliste!H26="X"),"bestanden",Notenliste!F26))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="66" t="str">
@@ -9879,7 +9879,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D27" s="65" t="str">
-        <f>IF(OR(Notenliste!H27="x", Notenliste!H27="X"),"bestanden",IF(Notenliste!D27=0," ",IF(Notenliste!F27="KP"," ",IF(Notenliste!F27="NB","nicht bestanden",Notenliste!F27))))</f>
+        <f>IF(Notenliste!D27=0," ",IF(Notenliste!F27="KP"," ",IF(Notenliste!F27="NB","nicht bestanden",IF(OR(Notenliste!H27="x", Notenliste!H27="X"),"bestanden",Notenliste!F27))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E27" s="66" t="str">
@@ -9901,7 +9901,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D28" s="65" t="str">
-        <f>IF(OR(Notenliste!H28="x", Notenliste!H28="X"),"bestanden",IF(Notenliste!D28=0," ",IF(Notenliste!F28="KP"," ",IF(Notenliste!F28="NB","nicht bestanden",Notenliste!F28))))</f>
+        <f>IF(Notenliste!D28=0," ",IF(Notenliste!F28="KP"," ",IF(Notenliste!F28="NB","nicht bestanden",IF(OR(Notenliste!H28="x", Notenliste!H28="X"),"bestanden",Notenliste!F28))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E28" s="66" t="str">
@@ -9923,7 +9923,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D29" s="65" t="str">
-        <f>IF(OR(Notenliste!H29="x", Notenliste!H29="X"),"bestanden",IF(Notenliste!D29=0," ",IF(Notenliste!F29="KP"," ",IF(Notenliste!F29="NB","nicht bestanden",Notenliste!F29))))</f>
+        <f>IF(Notenliste!D29=0," ",IF(Notenliste!F29="KP"," ",IF(Notenliste!F29="NB","nicht bestanden",IF(OR(Notenliste!H29="x", Notenliste!H29="X"),"bestanden",Notenliste!F29))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E29" s="66" t="str">
@@ -9945,7 +9945,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D30" s="65" t="str">
-        <f>IF(OR(Notenliste!H30="x", Notenliste!H30="X"),"bestanden",IF(Notenliste!D30=0," ",IF(Notenliste!F30="KP"," ",IF(Notenliste!F30="NB","nicht bestanden",Notenliste!F30))))</f>
+        <f>IF(Notenliste!D30=0," ",IF(Notenliste!F30="KP"," ",IF(Notenliste!F30="NB","nicht bestanden",IF(OR(Notenliste!H30="x", Notenliste!H30="X"),"bestanden",Notenliste!F30))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E30" s="66" t="str">
@@ -9967,7 +9967,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D31" s="65" t="str">
-        <f>IF(OR(Notenliste!H31="x", Notenliste!H31="X"),"bestanden",IF(Notenliste!D31=0," ",IF(Notenliste!F31="KP"," ",IF(Notenliste!F31="NB","nicht bestanden",Notenliste!F31))))</f>
+        <f>IF(Notenliste!D31=0," ",IF(Notenliste!F31="KP"," ",IF(Notenliste!F31="NB","nicht bestanden",IF(OR(Notenliste!H31="x", Notenliste!H31="X"),"bestanden",Notenliste!F31))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E31" s="66" t="str">
@@ -9989,7 +9989,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D32" s="65" t="str">
-        <f>IF(OR(Notenliste!H32="x", Notenliste!H32="X"),"bestanden",IF(Notenliste!D32=0," ",IF(Notenliste!F32="KP"," ",IF(Notenliste!F32="NB","nicht bestanden",Notenliste!F32))))</f>
+        <f>IF(Notenliste!D32=0," ",IF(Notenliste!F32="KP"," ",IF(Notenliste!F32="NB","nicht bestanden",IF(OR(Notenliste!H32="x", Notenliste!H32="X"),"bestanden",Notenliste!F32))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E32" s="66" t="str">
@@ -10011,7 +10011,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D33" s="65" t="str">
-        <f>IF(OR(Notenliste!H33="x", Notenliste!H33="X"),"bestanden",IF(Notenliste!D33=0," ",IF(Notenliste!F33="KP"," ",IF(Notenliste!F33="NB","nicht bestanden",Notenliste!F33))))</f>
+        <f>IF(Notenliste!D33=0," ",IF(Notenliste!F33="KP"," ",IF(Notenliste!F33="NB","nicht bestanden",IF(OR(Notenliste!H33="x", Notenliste!H33="X"),"bestanden",Notenliste!F33))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E33" s="66" t="str">
@@ -10033,7 +10033,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D34" s="65" t="str">
-        <f>IF(OR(Notenliste!H34="x", Notenliste!H34="X"),"bestanden",IF(Notenliste!D34=0," ",IF(Notenliste!F34="KP"," ",IF(Notenliste!F34="NB","nicht bestanden",Notenliste!F34))))</f>
+        <f>IF(Notenliste!D34=0," ",IF(Notenliste!F34="KP"," ",IF(Notenliste!F34="NB","nicht bestanden",IF(OR(Notenliste!H34="x", Notenliste!H34="X"),"bestanden",Notenliste!F34))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E34" s="66" t="str">
@@ -10055,7 +10055,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D35" s="65" t="str">
-        <f>IF(OR(Notenliste!H35="x", Notenliste!H35="X"),"bestanden",IF(Notenliste!D35=0," ",IF(Notenliste!F35="KP"," ",IF(Notenliste!F35="NB","nicht bestanden",Notenliste!F35))))</f>
+        <f>IF(Notenliste!D35=0," ",IF(Notenliste!F35="KP"," ",IF(Notenliste!F35="NB","nicht bestanden",IF(OR(Notenliste!H35="x", Notenliste!H35="X"),"bestanden",Notenliste!F35))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E35" s="66" t="str">
@@ -10077,7 +10077,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D36" s="65" t="str">
-        <f>IF(OR(Notenliste!H36="x", Notenliste!H36="X"),"bestanden",IF(Notenliste!D36=0," ",IF(Notenliste!F36="KP"," ",IF(Notenliste!F36="NB","nicht bestanden",Notenliste!F36))))</f>
+        <f>IF(Notenliste!D36=0," ",IF(Notenliste!F36="KP"," ",IF(Notenliste!F36="NB","nicht bestanden",IF(OR(Notenliste!H36="x", Notenliste!H36="X"),"bestanden",Notenliste!F36))))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E36" s="66" t="str">

</xml_diff>